<commit_message>
update the .dsm and the spreadsheet
</commit_message>
<xml_diff>
--- a/SPP/SPP.xlsx
+++ b/SPP/SPP.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1732" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1745" uniqueCount="230">
   <si>
     <t>Notes</t>
   </si>
@@ -714,6 +714,48 @@
   </si>
   <si>
     <t>adelikat &amp; Deign</t>
+  </si>
+  <si>
+    <t>Last frame of previous section</t>
+  </si>
+  <si>
+    <t>ous section</t>
+  </si>
+  <si>
+    <t>&lt;--- lol</t>
+  </si>
+  <si>
+    <t>Get to the first pipe</t>
+  </si>
+  <si>
+    <t>Get Toad 1, get to pipe</t>
+  </si>
+  <si>
+    <t>Get Toad 2, get to pipe</t>
+  </si>
+  <si>
+    <t>Get Toad 3, get 777 coins</t>
+  </si>
+  <si>
+    <t>Enter 1-2, to first black frame</t>
+  </si>
+  <si>
+    <t>Get Toad 1, and get to exit pipe</t>
+  </si>
+  <si>
+    <t>Get Toad 2, and get to pipe</t>
+  </si>
+  <si>
+    <t>Get Toad 3, and get to pipe</t>
+  </si>
+  <si>
+    <t>Get 777 coins</t>
+  </si>
+  <si>
+    <t>Get to wheel not 777 coins</t>
+  </si>
+  <si>
+    <t>Lost frames cause of 777 coins and toad speech is faster</t>
   </si>
 </sst>
 </file>
@@ -1470,6 +1512,17 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1480,17 +1533,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1554,28 +1596,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="10"/>
       </left>
       <right/>
@@ -1620,6 +1640,28 @@
       </left>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1928,15 +1970,14 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="41" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="43" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="31" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1945,34 +1986,35 @@
     <xf numFmtId="0" fontId="32" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1999,7 +2041,7 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="19" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2008,41 +2050,41 @@
     <xf numFmtId="0" fontId="40" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="43" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="41" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
   </cellXfs>
@@ -2348,8 +2390,8 @@
   <dimension ref="A1:K153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D160" sqref="D160"/>
+      <pane ySplit="6" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -2365,20 +2407,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="159" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="160" t="s">
+      <c r="B1" s="160"/>
+      <c r="C1" s="161" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="162"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="I1" s="139" t="s">
         <v>204</v>
@@ -2400,7 +2442,7 @@
       <c r="G2" s="138"/>
       <c r="H2" s="142">
         <f>IF(H1&lt;3600,H1/60,QUOTIENT(H1, 3600))</f>
-        <v>0</v>
+        <v>-1.6666666666666667</v>
       </c>
       <c r="I2" s="139" t="str">
         <f>IF(H1&lt;3600,"Seconds","Minutes")</f>
@@ -2452,14 +2494,18 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="163" t="s">
-        <v>186</v>
-      </c>
-      <c r="D5" s="163"/>
-      <c r="E5" s="145"/>
+      <c r="C5" s="157" t="s">
+        <v>216</v>
+      </c>
+      <c r="D5" s="157"/>
+      <c r="E5" s="145" t="s">
+        <v>217</v>
+      </c>
       <c r="F5" s="141"/>
       <c r="G5" s="138"/>
-      <c r="H5" s="138"/>
+      <c r="H5" s="138" t="s">
+        <v>218</v>
+      </c>
       <c r="I5" s="138"/>
       <c r="J5" s="138"/>
       <c r="K5" s="138"/>
@@ -2471,10 +2517,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="163" t="s">
+      <c r="C6" s="157" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="164"/>
+      <c r="D6" s="158"/>
       <c r="E6" s="145"/>
       <c r="F6" s="141"/>
       <c r="G6" s="138"/>
@@ -2492,7 +2538,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="162" t="s">
+      <c r="A8" s="163" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -2516,8 +2562,12 @@
       <c r="B9" s="97" t="s">
         <v>184</v>
       </c>
-      <c r="C9" s="98"/>
-      <c r="D9" s="98"/>
+      <c r="C9" s="98">
+        <v>0</v>
+      </c>
+      <c r="D9" s="98">
+        <v>0</v>
+      </c>
       <c r="E9" s="98"/>
       <c r="F9" s="103"/>
     </row>
@@ -2593,18 +2643,18 @@
         <v>187</v>
       </c>
       <c r="C16" s="98">
-        <v>0</v>
+        <v>511</v>
       </c>
       <c r="D16" s="98">
-        <v>0</v>
+        <v>505</v>
       </c>
       <c r="E16" s="100">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="F16" s="103"/>
     </row>
-    <row r="17" spans="1:7" ht="17.25" thickTop="1" thickBot="1">
+    <row r="17" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
       <c r="A17" s="115" t="s">
         <v>190</v>
       </c>
@@ -2613,25 +2663,25 @@
       </c>
       <c r="C17" s="102">
         <f>C16-C9</f>
-        <v>0</v>
+        <v>511</v>
       </c>
       <c r="D17" s="102">
         <f>D16-D9</f>
-        <v>0</v>
+        <v>505</v>
       </c>
       <c r="E17" s="120">
         <f>E16-E9</f>
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="F17" s="105"/>
       <c r="G17" s="111">
         <f>E17</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
-    <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="157" t="s">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="13.5" thickBot="1"/>
+    <row r="19" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A19" s="155" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -2650,64 +2700,95 @@
         <v>183</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="20" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="A20" s="156"/>
       <c r="B20" s="97" t="s">
         <v>184</v>
       </c>
-      <c r="C20" s="98"/>
-      <c r="D20" s="98"/>
+      <c r="C20" s="98">
+        <v>511</v>
+      </c>
+      <c r="D20" s="98">
+        <v>505</v>
+      </c>
       <c r="E20" s="121">
         <f t="shared" ref="E20:E33" si="1">IF(AND(C20&gt;0,D20&gt;0), D20-C20, 0)</f>
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="F20" s="103"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
+    <row r="21" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A21" s="156"/>
-      <c r="B21" s="99"/>
-      <c r="C21" s="100"/>
-      <c r="D21" s="100"/>
+      <c r="B21" s="99" t="s">
+        <v>219</v>
+      </c>
+      <c r="C21" s="100">
+        <v>1229</v>
+      </c>
+      <c r="D21" s="100">
+        <v>1218</v>
+      </c>
       <c r="E21" s="122">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-11</v>
       </c>
       <c r="F21" s="104"/>
     </row>
-    <row r="22" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="22" spans="1:9" ht="15" outlineLevel="1">
       <c r="A22" s="156"/>
-      <c r="B22" s="99"/>
-      <c r="C22" s="100"/>
-      <c r="D22" s="100"/>
+      <c r="B22" s="99" t="s">
+        <v>220</v>
+      </c>
+      <c r="C22" s="100">
+        <v>1970</v>
+      </c>
+      <c r="D22" s="100">
+        <v>1940</v>
+      </c>
       <c r="E22" s="121">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-30</v>
       </c>
       <c r="F22" s="104"/>
     </row>
-    <row r="23" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="23" spans="1:9" ht="15" outlineLevel="1">
       <c r="A23" s="156"/>
-      <c r="B23" s="99"/>
-      <c r="C23" s="100"/>
-      <c r="D23" s="100"/>
+      <c r="B23" s="99" t="s">
+        <v>221</v>
+      </c>
+      <c r="C23" s="100">
+        <v>3299</v>
+      </c>
+      <c r="D23" s="100">
+        <v>3261</v>
+      </c>
       <c r="E23" s="121">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-38</v>
       </c>
       <c r="F23" s="104"/>
     </row>
-    <row r="24" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="24" spans="1:9" ht="15" outlineLevel="1">
       <c r="A24" s="156"/>
-      <c r="B24" s="99"/>
-      <c r="C24" s="100"/>
-      <c r="D24" s="100"/>
+      <c r="B24" s="99" t="s">
+        <v>222</v>
+      </c>
+      <c r="C24" s="100">
+        <v>4384</v>
+      </c>
+      <c r="D24" s="100">
+        <v>4351</v>
+      </c>
       <c r="E24" s="121">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-33</v>
       </c>
       <c r="F24" s="104"/>
-    </row>
-    <row r="25" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+      <c r="I24" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15" outlineLevel="1">
       <c r="A25" s="156"/>
       <c r="B25" s="99"/>
       <c r="C25" s="100"/>
@@ -2718,7 +2799,7 @@
       </c>
       <c r="F25" s="104"/>
     </row>
-    <row r="26" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="26" spans="1:9" ht="15" outlineLevel="1">
       <c r="A26" s="156"/>
       <c r="B26" s="99"/>
       <c r="C26" s="100"/>
@@ -2729,7 +2810,7 @@
       </c>
       <c r="F26" s="104"/>
     </row>
-    <row r="27" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="27" spans="1:9" ht="15" outlineLevel="1">
       <c r="A27" s="156"/>
       <c r="B27" s="99"/>
       <c r="C27" s="100"/>
@@ -2740,7 +2821,7 @@
       </c>
       <c r="F27" s="104"/>
     </row>
-    <row r="28" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="28" spans="1:9" ht="15" outlineLevel="1">
       <c r="A28" s="156"/>
       <c r="B28" s="99"/>
       <c r="C28" s="100"/>
@@ -2751,7 +2832,7 @@
       </c>
       <c r="F28" s="104"/>
     </row>
-    <row r="29" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="29" spans="1:9" ht="15" outlineLevel="1">
       <c r="A29" s="156"/>
       <c r="B29" s="99"/>
       <c r="C29" s="100"/>
@@ -2762,7 +2843,7 @@
       </c>
       <c r="F29" s="104"/>
     </row>
-    <row r="30" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="30" spans="1:9" ht="15" outlineLevel="1">
       <c r="A30" s="156"/>
       <c r="B30" s="99"/>
       <c r="C30" s="100"/>
@@ -2773,7 +2854,7 @@
       </c>
       <c r="F30" s="104"/>
     </row>
-    <row r="31" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="31" spans="1:9" ht="15" outlineLevel="1">
       <c r="A31" s="156"/>
       <c r="B31" s="99"/>
       <c r="C31" s="100"/>
@@ -2784,7 +2865,7 @@
       </c>
       <c r="F31" s="104"/>
     </row>
-    <row r="32" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="32" spans="1:9" ht="15" outlineLevel="1">
       <c r="A32" s="156"/>
       <c r="B32" s="99"/>
       <c r="C32" s="100"/>
@@ -2795,20 +2876,24 @@
       </c>
       <c r="F32" s="104"/>
     </row>
-    <row r="33" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="33" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="A33" s="156"/>
       <c r="B33" s="97" t="s">
         <v>187</v>
       </c>
-      <c r="C33" s="98"/>
-      <c r="D33" s="98"/>
+      <c r="C33" s="98">
+        <v>4384</v>
+      </c>
+      <c r="D33" s="98">
+        <v>4351</v>
+      </c>
       <c r="E33" s="123">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-33</v>
       </c>
       <c r="F33" s="103"/>
     </row>
-    <row r="34" spans="1:7" ht="17.25" collapsed="1" thickTop="1" thickBot="1">
+    <row r="34" spans="1:7" ht="17.25" thickTop="1" thickBot="1">
       <c r="A34" s="116">
         <v>1</v>
       </c>
@@ -2817,25 +2902,25 @@
       </c>
       <c r="C34" s="102">
         <f>C33-C20</f>
-        <v>0</v>
+        <v>3873</v>
       </c>
       <c r="D34" s="102">
         <f>D33-D20</f>
-        <v>0</v>
+        <v>3846</v>
       </c>
       <c r="E34" s="124">
         <f>E33-E20</f>
-        <v>0</v>
+        <v>-27</v>
       </c>
       <c r="F34" s="107"/>
       <c r="G34" s="111">
         <f>E34</f>
-        <v>0</v>
+        <v>-27</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
-    <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="155" t="s">
+    <row r="36" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A36" s="164" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -2854,64 +2939,92 @@
         <v>183</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="37" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="A37" s="156"/>
       <c r="B37" s="97" t="s">
         <v>184</v>
       </c>
-      <c r="C37" s="98"/>
-      <c r="D37" s="98"/>
+      <c r="C37" s="98">
+        <v>4384</v>
+      </c>
+      <c r="D37" s="98">
+        <v>4351</v>
+      </c>
       <c r="E37" s="121">
         <f t="shared" ref="E37:E50" si="2">IF(AND(C37&gt;0,D37&gt;0), D37-C37, 0)</f>
-        <v>0</v>
+        <v>-33</v>
       </c>
       <c r="F37" s="103"/>
     </row>
-    <row r="38" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
+    <row r="38" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A38" s="156"/>
-      <c r="B38" s="99"/>
-      <c r="C38" s="100"/>
-      <c r="D38" s="100"/>
+      <c r="B38" s="99" t="s">
+        <v>223</v>
+      </c>
+      <c r="C38" s="100">
+        <v>4642</v>
+      </c>
+      <c r="D38" s="100">
+        <v>4606</v>
+      </c>
       <c r="E38" s="122">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-36</v>
       </c>
       <c r="F38" s="104"/>
     </row>
-    <row r="39" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="39" spans="1:7" ht="15" outlineLevel="1">
       <c r="A39" s="156"/>
-      <c r="B39" s="99"/>
-      <c r="C39" s="100"/>
-      <c r="D39" s="100"/>
+      <c r="B39" s="99" t="s">
+        <v>224</v>
+      </c>
+      <c r="C39" s="100">
+        <v>5951</v>
+      </c>
+      <c r="D39" s="100">
+        <v>5911</v>
+      </c>
       <c r="E39" s="121">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-40</v>
       </c>
       <c r="F39" s="104"/>
     </row>
-    <row r="40" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="40" spans="1:7" ht="15" outlineLevel="1">
       <c r="A40" s="156"/>
-      <c r="B40" s="99"/>
-      <c r="C40" s="100"/>
-      <c r="D40" s="100"/>
+      <c r="B40" s="99" t="s">
+        <v>225</v>
+      </c>
+      <c r="C40" s="100">
+        <v>6951</v>
+      </c>
+      <c r="D40" s="100">
+        <v>6867</v>
+      </c>
       <c r="E40" s="121">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-84</v>
       </c>
       <c r="F40" s="104"/>
     </row>
-    <row r="41" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="41" spans="1:7" ht="15" outlineLevel="1">
       <c r="A41" s="156"/>
-      <c r="B41" s="99"/>
-      <c r="C41" s="100"/>
-      <c r="D41" s="100"/>
+      <c r="B41" s="99" t="s">
+        <v>226</v>
+      </c>
+      <c r="C41" s="100">
+        <v>7848</v>
+      </c>
+      <c r="D41" s="100">
+        <v>7757</v>
+      </c>
       <c r="E41" s="121">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-91</v>
       </c>
       <c r="F41" s="104"/>
     </row>
-    <row r="42" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="42" spans="1:7" ht="15" outlineLevel="1">
       <c r="A42" s="156"/>
       <c r="B42" s="99"/>
       <c r="C42" s="100"/>
@@ -2922,7 +3035,7 @@
       </c>
       <c r="F42" s="104"/>
     </row>
-    <row r="43" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="43" spans="1:7" ht="15" outlineLevel="1">
       <c r="A43" s="156"/>
       <c r="B43" s="99"/>
       <c r="C43" s="100"/>
@@ -2933,7 +3046,7 @@
       </c>
       <c r="F43" s="104"/>
     </row>
-    <row r="44" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="44" spans="1:7" ht="15" outlineLevel="1">
       <c r="A44" s="156"/>
       <c r="B44" s="99"/>
       <c r="C44" s="100"/>
@@ -2944,7 +3057,7 @@
       </c>
       <c r="F44" s="104"/>
     </row>
-    <row r="45" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="45" spans="1:7" ht="15" outlineLevel="1">
       <c r="A45" s="156"/>
       <c r="B45" s="99"/>
       <c r="C45" s="100"/>
@@ -2955,7 +3068,7 @@
       </c>
       <c r="F45" s="104"/>
     </row>
-    <row r="46" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="46" spans="1:7" ht="15" outlineLevel="1">
       <c r="A46" s="156"/>
       <c r="B46" s="99"/>
       <c r="C46" s="100"/>
@@ -2966,7 +3079,7 @@
       </c>
       <c r="F46" s="104"/>
     </row>
-    <row r="47" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="47" spans="1:7" ht="15" outlineLevel="1">
       <c r="A47" s="156"/>
       <c r="B47" s="99"/>
       <c r="C47" s="100"/>
@@ -2977,42 +3090,56 @@
       </c>
       <c r="F47" s="104"/>
     </row>
-    <row r="48" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="48" spans="1:7" ht="15" outlineLevel="1">
       <c r="A48" s="156"/>
-      <c r="B48" s="99"/>
+      <c r="B48" s="99" t="s">
+        <v>228</v>
+      </c>
       <c r="C48" s="100"/>
-      <c r="D48" s="100"/>
+      <c r="D48" s="100">
+        <v>8815</v>
+      </c>
       <c r="E48" s="121">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F48" s="104"/>
     </row>
-    <row r="49" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="49" spans="1:7" ht="15" outlineLevel="1">
       <c r="A49" s="156"/>
-      <c r="B49" s="99"/>
-      <c r="C49" s="100"/>
-      <c r="D49" s="100"/>
+      <c r="B49" s="99" t="s">
+        <v>227</v>
+      </c>
+      <c r="C49" s="100">
+        <v>8924</v>
+      </c>
+      <c r="D49" s="100">
+        <v>8824</v>
+      </c>
       <c r="E49" s="121">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="F49" s="104"/>
     </row>
-    <row r="50" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="50" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="A50" s="156"/>
       <c r="B50" s="97" t="s">
         <v>187</v>
       </c>
-      <c r="C50" s="98"/>
-      <c r="D50" s="98"/>
+      <c r="C50" s="98">
+        <v>8924</v>
+      </c>
+      <c r="D50" s="98">
+        <v>8824</v>
+      </c>
       <c r="E50" s="123">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="F50" s="103"/>
     </row>
-    <row r="51" spans="1:7" ht="17.25" collapsed="1" thickTop="1" thickBot="1">
+    <row r="51" spans="1:7" ht="17.25" thickTop="1" thickBot="1">
       <c r="A51" s="115">
         <v>2</v>
       </c>
@@ -3021,25 +3148,25 @@
       </c>
       <c r="C51" s="102">
         <f>C50-C37</f>
-        <v>0</v>
+        <v>4540</v>
       </c>
       <c r="D51" s="102">
         <f>D50-D37</f>
-        <v>0</v>
+        <v>4473</v>
       </c>
       <c r="E51" s="124">
         <f>E50-E37</f>
-        <v>0</v>
+        <v>-67</v>
       </c>
       <c r="F51" s="106"/>
       <c r="G51" s="111">
         <f>E51</f>
-        <v>0</v>
+        <v>-67</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="157" t="s">
+      <c r="A53" s="155" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -3243,7 +3370,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="155" t="s">
+      <c r="A70" s="164" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -3447,7 +3574,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="157" t="s">
+      <c r="A87" s="155" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -3650,7 +3777,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="155" t="s">
+      <c r="A104" s="164" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -3853,7 +3980,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="157" t="s">
+      <c r="A121" s="155" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -4056,7 +4183,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="155" t="s">
+      <c r="A138" s="164" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -4260,19 +4387,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A8:A16"/>
-    <mergeCell ref="A19:A33"/>
-    <mergeCell ref="A36:A50"/>
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A138:A152"/>
     <mergeCell ref="A104:A118"/>
     <mergeCell ref="A70:A84"/>
     <mergeCell ref="A121:A135"/>
     <mergeCell ref="A87:A101"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A8:A16"/>
+    <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A36:A50"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5317,7 +5444,7 @@
       </c>
       <c r="C6" s="132">
         <f ca="1">'FrameCounts World 1'!H2</f>
-        <v>0</v>
+        <v>-1.6666666666666667</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -5329,7 +5456,7 @@
       </c>
       <c r="C7" s="133">
         <f>C6/60</f>
-        <v>0</v>
+        <v>-2.777777777777778E-2</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -5455,9 +5582,9 @@
       <c r="B20" s="126" t="s">
         <v>159</v>
       </c>
-      <c r="C20" s="130">
+      <c r="C20" s="130" t="str">
         <f ca="1">'FrameCounts World 1'!B21</f>
-        <v>0</v>
+        <v>Get to the first pipe</v>
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1">
@@ -5530,10 +5657,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="207" t="s">
+      <c r="A1" s="211" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="208"/>
+      <c r="B1" s="212"/>
       <c r="C1" s="117"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
@@ -5553,127 +5680,142 @@
       <c r="C3" s="118"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="211"/>
-      <c r="B4" s="212"/>
+      <c r="A4" s="215"/>
+      <c r="B4" s="216"/>
       <c r="C4" s="118"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="209" t="s">
+      <c r="A5" s="213" t="s">
         <v>202</v>
       </c>
-      <c r="B5" s="210"/>
+      <c r="B5" s="214"/>
       <c r="C5" s="118"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="215" t="s">
+      <c r="A7" s="205" t="s">
         <v>194</v>
       </c>
-      <c r="B7" s="216"/>
+      <c r="B7" s="206"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="118"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="213" t="s">
+      <c r="A9" s="207" t="s">
         <v>195</v>
       </c>
-      <c r="B9" s="214"/>
+      <c r="B9" s="208"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="203"/>
-      <c r="B10" s="204"/>
+      <c r="A10" s="209"/>
+      <c r="B10" s="210"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="205" t="s">
+      <c r="A11" s="201" t="s">
         <v>196</v>
       </c>
-      <c r="B11" s="206"/>
+      <c r="B11" s="202"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="205" t="s">
+      <c r="A12" s="201" t="s">
         <v>197</v>
       </c>
-      <c r="B12" s="206"/>
+      <c r="B12" s="202"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="205" t="s">
+      <c r="A13" s="201" t="s">
         <v>198</v>
       </c>
-      <c r="B13" s="206"/>
+      <c r="B13" s="202"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="205" t="s">
+      <c r="A14" s="201" t="s">
         <v>199</v>
       </c>
-      <c r="B14" s="206"/>
+      <c r="B14" s="202"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="205" t="s">
+      <c r="A15" s="201" t="s">
         <v>200</v>
       </c>
-      <c r="B15" s="206"/>
+      <c r="B15" s="202"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="205" t="s">
+      <c r="A16" s="201" t="s">
         <v>201</v>
       </c>
-      <c r="B16" s="206"/>
+      <c r="B16" s="202"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="201" t="s">
+      <c r="A17" s="203" t="s">
         <v>203</v>
       </c>
-      <c r="B17" s="202"/>
+      <c r="B17" s="204"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="215" t="s">
+      <c r="A19" s="205" t="s">
         <v>205</v>
       </c>
-      <c r="B19" s="216"/>
+      <c r="B19" s="206"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="118"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="213" t="s">
+      <c r="A21" s="207" t="s">
         <v>206</v>
       </c>
-      <c r="B21" s="214"/>
+      <c r="B21" s="208"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="203"/>
-      <c r="B22" s="204"/>
+      <c r="A22" s="209"/>
+      <c r="B22" s="210"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="205" t="s">
+      <c r="A23" s="201" t="s">
         <v>207</v>
       </c>
-      <c r="B23" s="206"/>
+      <c r="B23" s="202"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="205"/>
-      <c r="B24" s="206"/>
+      <c r="A24" s="201"/>
+      <c r="B24" s="202"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="205" t="s">
+      <c r="A25" s="201" t="s">
         <v>208</v>
       </c>
-      <c r="B25" s="206"/>
+      <c r="B25" s="202"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="205" t="s">
+      <c r="A26" s="201" t="s">
         <v>209</v>
       </c>
-      <c r="B26" s="206"/>
+      <c r="B26" s="202"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="201"/>
-      <c r="B27" s="202"/>
+      <c r="A27" s="203"/>
+      <c r="B27" s="204"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
@@ -5682,21 +5824,6 @@
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -5731,16 +5858,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="159" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="160" t="s">
+      <c r="B1" s="160"/>
+      <c r="C1" s="161" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="162"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -5818,10 +5945,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="163" t="s">
+      <c r="C5" s="157" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="163"/>
+      <c r="D5" s="157"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -5837,10 +5964,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="163" t="s">
+      <c r="C6" s="157" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="164"/>
+      <c r="D6" s="158"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -5858,7 +5985,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="162" t="s">
+      <c r="A8" s="163" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -5997,7 +6124,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="157" t="s">
+      <c r="A19" s="155" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -6201,7 +6328,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="155" t="s">
+      <c r="A36" s="164" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -6405,7 +6532,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="157" t="s">
+      <c r="A53" s="155" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -6609,7 +6736,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="155" t="s">
+      <c r="A70" s="164" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -6813,7 +6940,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="157" t="s">
+      <c r="A87" s="155" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -7016,7 +7143,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="155" t="s">
+      <c r="A104" s="164" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -7219,7 +7346,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="157" t="s">
+      <c r="A121" s="155" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -7422,7 +7549,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="155" t="s">
+      <c r="A138" s="164" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -7626,19 +7753,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A8:A16"/>
+    <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A36:A50"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A138:A152"/>
     <mergeCell ref="A104:A118"/>
     <mergeCell ref="A70:A84"/>
     <mergeCell ref="A121:A135"/>
     <mergeCell ref="A87:A101"/>
-    <mergeCell ref="A36:A50"/>
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A8:A16"/>
-    <mergeCell ref="A19:A33"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7672,16 +7799,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="159" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="160" t="s">
+      <c r="B1" s="160"/>
+      <c r="C1" s="161" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="162"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -7759,10 +7886,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="163" t="s">
+      <c r="C5" s="157" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="163"/>
+      <c r="D5" s="157"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -7778,10 +7905,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="163" t="s">
+      <c r="C6" s="157" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="164"/>
+      <c r="D6" s="158"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -7799,7 +7926,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="162" t="s">
+      <c r="A8" s="163" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -7938,7 +8065,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="157" t="s">
+      <c r="A19" s="155" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -8142,7 +8269,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="155" t="s">
+      <c r="A36" s="164" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -8346,7 +8473,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="157" t="s">
+      <c r="A53" s="155" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -8550,7 +8677,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="155" t="s">
+      <c r="A70" s="164" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -8754,7 +8881,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="157" t="s">
+      <c r="A87" s="155" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -8957,7 +9084,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="155" t="s">
+      <c r="A104" s="164" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -9160,7 +9287,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="157" t="s">
+      <c r="A121" s="155" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -9363,7 +9490,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="155" t="s">
+      <c r="A138" s="164" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -9567,19 +9694,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A8:A16"/>
-    <mergeCell ref="A19:A33"/>
-    <mergeCell ref="A36:A50"/>
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A138:A152"/>
     <mergeCell ref="A104:A118"/>
     <mergeCell ref="A70:A84"/>
     <mergeCell ref="A121:A135"/>
     <mergeCell ref="A87:A101"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A8:A16"/>
+    <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A36:A50"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9613,16 +9740,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="159" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="160" t="s">
+      <c r="B1" s="160"/>
+      <c r="C1" s="161" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="162"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -9700,10 +9827,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="163" t="s">
+      <c r="C5" s="157" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="163"/>
+      <c r="D5" s="157"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -9719,10 +9846,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="163" t="s">
+      <c r="C6" s="157" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="164"/>
+      <c r="D6" s="158"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -9740,7 +9867,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="162" t="s">
+      <c r="A8" s="163" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -9879,7 +10006,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="157" t="s">
+      <c r="A19" s="155" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -10083,7 +10210,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="155" t="s">
+      <c r="A36" s="164" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -10287,7 +10414,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="157" t="s">
+      <c r="A53" s="155" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -10491,7 +10618,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="155" t="s">
+      <c r="A70" s="164" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -10695,7 +10822,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="157" t="s">
+      <c r="A87" s="155" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -10898,7 +11025,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="155" t="s">
+      <c r="A104" s="164" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -11101,7 +11228,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="157" t="s">
+      <c r="A121" s="155" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -11304,7 +11431,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="155" t="s">
+      <c r="A138" s="164" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -11508,19 +11635,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A8:A16"/>
+    <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A36:A50"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A138:A152"/>
     <mergeCell ref="A104:A118"/>
     <mergeCell ref="A70:A84"/>
     <mergeCell ref="A121:A135"/>
     <mergeCell ref="A87:A101"/>
-    <mergeCell ref="A36:A50"/>
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A8:A16"/>
-    <mergeCell ref="A19:A33"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11554,16 +11681,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="159" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="160" t="s">
+      <c r="B1" s="160"/>
+      <c r="C1" s="161" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="162"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -11641,10 +11768,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="163" t="s">
+      <c r="C5" s="157" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="163"/>
+      <c r="D5" s="157"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -11660,10 +11787,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="163" t="s">
+      <c r="C6" s="157" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="164"/>
+      <c r="D6" s="158"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -11681,7 +11808,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="162" t="s">
+      <c r="A8" s="163" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -11820,7 +11947,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="157" t="s">
+      <c r="A19" s="155" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -12024,7 +12151,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="155" t="s">
+      <c r="A36" s="164" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -12228,7 +12355,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="157" t="s">
+      <c r="A53" s="155" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -12432,7 +12559,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="155" t="s">
+      <c r="A70" s="164" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -12636,7 +12763,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="157" t="s">
+      <c r="A87" s="155" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -12839,7 +12966,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="155" t="s">
+      <c r="A104" s="164" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -13042,7 +13169,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="157" t="s">
+      <c r="A121" s="155" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -13245,7 +13372,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="155" t="s">
+      <c r="A138" s="164" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -13449,19 +13576,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A8:A16"/>
-    <mergeCell ref="A19:A33"/>
-    <mergeCell ref="A36:A50"/>
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A138:A152"/>
     <mergeCell ref="A104:A118"/>
     <mergeCell ref="A70:A84"/>
     <mergeCell ref="A121:A135"/>
     <mergeCell ref="A87:A101"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A8:A16"/>
+    <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A36:A50"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13495,16 +13622,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="159" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="160" t="s">
+      <c r="B1" s="160"/>
+      <c r="C1" s="161" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="162"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -13582,10 +13709,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="163" t="s">
+      <c r="C5" s="157" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="163"/>
+      <c r="D5" s="157"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -13601,10 +13728,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="163" t="s">
+      <c r="C6" s="157" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="164"/>
+      <c r="D6" s="158"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -13622,7 +13749,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="162" t="s">
+      <c r="A8" s="163" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -13761,7 +13888,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="157" t="s">
+      <c r="A19" s="155" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -13965,7 +14092,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="155" t="s">
+      <c r="A36" s="164" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -14169,7 +14296,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="157" t="s">
+      <c r="A53" s="155" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -14373,7 +14500,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="155" t="s">
+      <c r="A70" s="164" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -14577,7 +14704,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="157" t="s">
+      <c r="A87" s="155" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -14780,7 +14907,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="155" t="s">
+      <c r="A104" s="164" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -14983,7 +15110,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="157" t="s">
+      <c r="A121" s="155" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -15186,7 +15313,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="155" t="s">
+      <c r="A138" s="164" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -15390,19 +15517,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A8:A16"/>
+    <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A36:A50"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A138:A152"/>
     <mergeCell ref="A104:A118"/>
     <mergeCell ref="A70:A84"/>
     <mergeCell ref="A121:A135"/>
     <mergeCell ref="A87:A101"/>
-    <mergeCell ref="A36:A50"/>
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A8:A16"/>
-    <mergeCell ref="A19:A33"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15436,16 +15563,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="159" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="160" t="s">
+      <c r="B1" s="160"/>
+      <c r="C1" s="161" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="162"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -15523,10 +15650,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="163" t="s">
+      <c r="C5" s="157" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="163"/>
+      <c r="D5" s="157"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -15542,10 +15669,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="163" t="s">
+      <c r="C6" s="157" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="164"/>
+      <c r="D6" s="158"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -15563,7 +15690,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="162" t="s">
+      <c r="A8" s="163" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -15702,7 +15829,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="157" t="s">
+      <c r="A19" s="155" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -15906,7 +16033,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="155" t="s">
+      <c r="A36" s="164" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -16110,7 +16237,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="157" t="s">
+      <c r="A53" s="155" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -16314,7 +16441,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="155" t="s">
+      <c r="A70" s="164" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -16518,7 +16645,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="157" t="s">
+      <c r="A87" s="155" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -16721,7 +16848,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="155" t="s">
+      <c r="A104" s="164" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -16924,7 +17051,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="157" t="s">
+      <c r="A121" s="155" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -17127,7 +17254,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="155" t="s">
+      <c r="A138" s="164" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -17331,19 +17458,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A8:A16"/>
-    <mergeCell ref="A19:A33"/>
-    <mergeCell ref="A36:A50"/>
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A138:A152"/>
     <mergeCell ref="A104:A118"/>
     <mergeCell ref="A70:A84"/>
     <mergeCell ref="A121:A135"/>
     <mergeCell ref="A87:A101"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A8:A16"/>
+    <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A36:A50"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17377,16 +17504,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="159" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="160" t="s">
+      <c r="B1" s="160"/>
+      <c r="C1" s="161" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="162"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -17464,10 +17591,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="163" t="s">
+      <c r="C5" s="157" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="163"/>
+      <c r="D5" s="157"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -17483,10 +17610,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="163" t="s">
+      <c r="C6" s="157" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="164"/>
+      <c r="D6" s="158"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -17504,7 +17631,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="162" t="s">
+      <c r="A8" s="163" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -17643,7 +17770,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="157" t="s">
+      <c r="A19" s="155" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -17847,7 +17974,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="155" t="s">
+      <c r="A36" s="164" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -18051,7 +18178,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="157" t="s">
+      <c r="A53" s="155" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -18255,7 +18382,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="155" t="s">
+      <c r="A70" s="164" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -18459,7 +18586,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="157" t="s">
+      <c r="A87" s="155" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -18662,7 +18789,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="155" t="s">
+      <c r="A104" s="164" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -18865,7 +18992,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="157" t="s">
+      <c r="A121" s="155" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -19068,7 +19195,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="155" t="s">
+      <c r="A138" s="164" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -19272,19 +19399,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A8:A16"/>
+    <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A36:A50"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A138:A152"/>
     <mergeCell ref="A104:A118"/>
     <mergeCell ref="A70:A84"/>
     <mergeCell ref="A121:A135"/>
     <mergeCell ref="A87:A101"/>
-    <mergeCell ref="A36:A50"/>
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A8:A16"/>
-    <mergeCell ref="A19:A33"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19318,13 +19445,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="183" t="s">
+      <c r="A1" s="167" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="183"/>
-      <c r="C1" s="183"/>
-      <c r="D1" s="183"/>
-      <c r="E1" s="183"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -19354,9 +19481,9 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="184"/>
-      <c r="D3" s="185"/>
-      <c r="E3" s="185"/>
+      <c r="C3" s="168"/>
+      <c r="D3" s="169"/>
+      <c r="E3" s="169"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
@@ -19517,9 +19644,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="169"/>
-      <c r="D21" s="170"/>
-      <c r="E21" s="170"/>
+      <c r="C21" s="170"/>
+      <c r="D21" s="171"/>
+      <c r="E21" s="171"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -21812,9 +21939,9 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="181"/>
-      <c r="D276" s="182"/>
-      <c r="E276" s="182"/>
+      <c r="C276" s="172"/>
+      <c r="D276" s="173"/>
+      <c r="E276" s="173"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
@@ -21974,9 +22101,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="169"/>
-      <c r="D294" s="170"/>
-      <c r="E294" s="170"/>
+      <c r="C294" s="170"/>
+      <c r="D294" s="171"/>
+      <c r="E294" s="171"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -24269,9 +24396,9 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="179"/>
-      <c r="D549" s="180"/>
-      <c r="E549" s="180"/>
+      <c r="C549" s="174"/>
+      <c r="D549" s="175"/>
+      <c r="E549" s="175"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
@@ -24431,9 +24558,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="169"/>
-      <c r="D567" s="170"/>
-      <c r="E567" s="170"/>
+      <c r="C567" s="170"/>
+      <c r="D567" s="171"/>
+      <c r="E567" s="171"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -26726,9 +26853,9 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="177"/>
-      <c r="D822" s="178"/>
-      <c r="E822" s="178"/>
+      <c r="C822" s="176"/>
+      <c r="D822" s="177"/>
+      <c r="E822" s="177"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
@@ -26888,9 +27015,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="169"/>
-      <c r="D840" s="170"/>
-      <c r="E840" s="170"/>
+      <c r="C840" s="170"/>
+      <c r="D840" s="171"/>
+      <c r="E840" s="171"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -29183,9 +29310,9 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="175"/>
-      <c r="D1095" s="176"/>
-      <c r="E1095" s="176"/>
+      <c r="C1095" s="178"/>
+      <c r="D1095" s="179"/>
+      <c r="E1095" s="179"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
@@ -29345,9 +29472,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="169"/>
-      <c r="D1113" s="170"/>
-      <c r="E1113" s="170"/>
+      <c r="C1113" s="170"/>
+      <c r="D1113" s="171"/>
+      <c r="E1113" s="171"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -31640,9 +31767,9 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="173"/>
-      <c r="D1368" s="174"/>
-      <c r="E1368" s="174"/>
+      <c r="C1368" s="180"/>
+      <c r="D1368" s="181"/>
+      <c r="E1368" s="181"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
@@ -31802,9 +31929,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="169"/>
-      <c r="D1386" s="170"/>
-      <c r="E1386" s="170"/>
+      <c r="C1386" s="170"/>
+      <c r="D1386" s="171"/>
+      <c r="E1386" s="171"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -34097,9 +34224,9 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="171"/>
-      <c r="D1641" s="172"/>
-      <c r="E1641" s="172"/>
+      <c r="C1641" s="182"/>
+      <c r="D1641" s="183"/>
+      <c r="E1641" s="183"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
@@ -34259,9 +34386,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="169"/>
-      <c r="D1659" s="170"/>
-      <c r="E1659" s="170"/>
+      <c r="C1659" s="170"/>
+      <c r="D1659" s="171"/>
+      <c r="E1659" s="171"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -36554,9 +36681,9 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="167"/>
-      <c r="D1914" s="168"/>
-      <c r="E1914" s="168"/>
+      <c r="C1914" s="184"/>
+      <c r="D1914" s="185"/>
+      <c r="E1914" s="185"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
@@ -36716,9 +36843,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="169"/>
-      <c r="D1932" s="170"/>
-      <c r="E1932" s="170"/>
+      <c r="C1932" s="170"/>
+      <c r="D1932" s="171"/>
+      <c r="E1932" s="171"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -39008,10 +39135,133 @@
     </row>
   </sheetData>
   <mergeCells count="137">
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C1932:E1932"/>
+    <mergeCell ref="C1949:E1949"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C2000:E2000"/>
+    <mergeCell ref="C2017:E2017"/>
+    <mergeCell ref="C1846:E1846"/>
+    <mergeCell ref="C1863:E1863"/>
+    <mergeCell ref="C1880:E1880"/>
+    <mergeCell ref="C1897:E1897"/>
+    <mergeCell ref="C1914:E1914"/>
+    <mergeCell ref="C1915:E1915"/>
+    <mergeCell ref="C1966:E1966"/>
+    <mergeCell ref="C1983:E1983"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
+    <mergeCell ref="C464:E464"/>
+    <mergeCell ref="C481:E481"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C396:E396"/>
+    <mergeCell ref="C413:E413"/>
+    <mergeCell ref="C430:E430"/>
+    <mergeCell ref="C447:E447"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C328:E328"/>
+    <mergeCell ref="C345:E345"/>
+    <mergeCell ref="C362:E362"/>
+    <mergeCell ref="C379:E379"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C294:E294"/>
+    <mergeCell ref="C311:E311"/>
     <mergeCell ref="C55:E55"/>
     <mergeCell ref="C72:E72"/>
     <mergeCell ref="C208:E208"/>
     <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
     <mergeCell ref="C242:E242"/>
     <mergeCell ref="C259:E259"/>
     <mergeCell ref="A1:E1"/>
@@ -39022,129 +39272,6 @@
     <mergeCell ref="C38:E38"/>
     <mergeCell ref="C106:E106"/>
     <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="C396:E396"/>
-    <mergeCell ref="C413:E413"/>
-    <mergeCell ref="C430:E430"/>
-    <mergeCell ref="C447:E447"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C294:E294"/>
-    <mergeCell ref="C311:E311"/>
-    <mergeCell ref="C328:E328"/>
-    <mergeCell ref="C345:E345"/>
-    <mergeCell ref="C362:E362"/>
-    <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C464:E464"/>
-    <mergeCell ref="C481:E481"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1966:E1966"/>
-    <mergeCell ref="C1983:E1983"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C2000:E2000"/>
-    <mergeCell ref="C2017:E2017"/>
-    <mergeCell ref="C1846:E1846"/>
-    <mergeCell ref="C1863:E1863"/>
-    <mergeCell ref="C1880:E1880"/>
-    <mergeCell ref="C1897:E1897"/>
-    <mergeCell ref="C1914:E1914"/>
-    <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C1932:E1932"/>
-    <mergeCell ref="C1949:E1949"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
End of 1-3, need to somehow save 2 or 3 frames on the last room to get the star, if not, then redo 1-3 buying before.
</commit_message>
<xml_diff>
--- a/SPP/SPP.xlsx
+++ b/SPP/SPP.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1745" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1759" uniqueCount="242">
   <si>
     <t>Notes</t>
   </si>
@@ -756,6 +756,42 @@
   </si>
   <si>
     <t>Lost frames cause of 777 coins and toad speech is faster</t>
+  </si>
+  <si>
+    <t>Enter 1-3 to first black frame</t>
+  </si>
+  <si>
+    <t>Get Toad 1, and get to pipe</t>
+  </si>
+  <si>
+    <t>Get Toad 2, and back out the pipe</t>
+  </si>
+  <si>
+    <t>Enter pipe to Toad 2</t>
+  </si>
+  <si>
+    <t>Get to pipe for Toad 3</t>
+  </si>
+  <si>
+    <t>Get Toad 3, and exit pipe</t>
+  </si>
+  <si>
+    <t>Get to last pipe</t>
+  </si>
+  <si>
+    <t>Exit Level 777 Coins</t>
+  </si>
+  <si>
+    <t>Waddle Bought</t>
+  </si>
+  <si>
+    <t>737</t>
+  </si>
+  <si>
+    <t>304</t>
+  </si>
+  <si>
+    <t>210</t>
   </si>
 </sst>
 </file>
@@ -1596,6 +1632,28 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="10"/>
       </left>
       <right/>
@@ -1640,28 +1698,6 @@
       </left>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1970,10 +2006,13 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1989,32 +2028,29 @@
     <xf numFmtId="0" fontId="28" fillId="20" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2050,41 +2086,41 @@
     <xf numFmtId="0" fontId="40" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="41" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="43" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
   </cellXfs>
@@ -2390,8 +2426,8 @@
   <dimension ref="A1:K153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
+      <pane ySplit="6" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -2407,20 +2443,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="160" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="161" t="s">
+      <c r="B1" s="161"/>
+      <c r="C1" s="162" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="163"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
-        <v>-100</v>
+        <v>-760</v>
       </c>
       <c r="I1" s="139" t="s">
         <v>204</v>
@@ -2442,7 +2478,7 @@
       <c r="G2" s="138"/>
       <c r="H2" s="142">
         <f>IF(H1&lt;3600,H1/60,QUOTIENT(H1, 3600))</f>
-        <v>-1.6666666666666667</v>
+        <v>-12.666666666666666</v>
       </c>
       <c r="I2" s="139" t="str">
         <f>IF(H1&lt;3600,"Seconds","Minutes")</f>
@@ -2494,10 +2530,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="157" t="s">
+      <c r="C5" s="158" t="s">
         <v>216</v>
       </c>
-      <c r="D5" s="157"/>
+      <c r="D5" s="158"/>
       <c r="E5" s="145" t="s">
         <v>217</v>
       </c>
@@ -2517,10 +2553,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="157" t="s">
+      <c r="C6" s="158" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="158"/>
+      <c r="D6" s="159"/>
       <c r="E6" s="145"/>
       <c r="F6" s="141"/>
       <c r="G6" s="138"/>
@@ -2537,8 +2573,8 @@
       <c r="E7" s="93"/>
       <c r="F7" s="93"/>
     </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="163" t="s">
+    <row r="8" spans="1:11" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="A8" s="164" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -2557,7 +2593,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="9" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A9" s="156"/>
       <c r="B9" s="97" t="s">
         <v>184</v>
@@ -2571,7 +2607,7 @@
       <c r="E9" s="98"/>
       <c r="F9" s="103"/>
     </row>
-    <row r="10" spans="1:11" ht="15.75" outlineLevel="1" thickTop="1">
+    <row r="10" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
       <c r="A10" s="156"/>
       <c r="B10" s="99"/>
       <c r="C10" s="100"/>
@@ -2582,7 +2618,7 @@
       </c>
       <c r="F10" s="104"/>
     </row>
-    <row r="11" spans="1:11" ht="15" outlineLevel="1">
+    <row r="11" spans="1:11" ht="15" hidden="1" outlineLevel="1">
       <c r="A11" s="156"/>
       <c r="B11" s="99"/>
       <c r="C11" s="100"/>
@@ -2593,7 +2629,7 @@
       </c>
       <c r="F11" s="104"/>
     </row>
-    <row r="12" spans="1:11" ht="15" outlineLevel="1">
+    <row r="12" spans="1:11" ht="15" hidden="1" outlineLevel="1">
       <c r="A12" s="156"/>
       <c r="B12" s="99"/>
       <c r="C12" s="100"/>
@@ -2604,7 +2640,7 @@
       </c>
       <c r="F12" s="104"/>
     </row>
-    <row r="13" spans="1:11" ht="15" outlineLevel="1">
+    <row r="13" spans="1:11" ht="15" hidden="1" outlineLevel="1">
       <c r="A13" s="156"/>
       <c r="B13" s="99"/>
       <c r="C13" s="100"/>
@@ -2615,7 +2651,7 @@
       </c>
       <c r="F13" s="104"/>
     </row>
-    <row r="14" spans="1:11" ht="15" outlineLevel="1">
+    <row r="14" spans="1:11" ht="15" hidden="1" outlineLevel="1">
       <c r="A14" s="156"/>
       <c r="B14" s="99"/>
       <c r="C14" s="100"/>
@@ -2626,7 +2662,7 @@
       </c>
       <c r="F14" s="104"/>
     </row>
-    <row r="15" spans="1:11" ht="15" outlineLevel="1">
+    <row r="15" spans="1:11" ht="15" hidden="1" outlineLevel="1">
       <c r="A15" s="156"/>
       <c r="B15" s="99"/>
       <c r="C15" s="100"/>
@@ -2637,7 +2673,7 @@
       </c>
       <c r="F15" s="104"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="16" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A16" s="156"/>
       <c r="B16" s="97" t="s">
         <v>187</v>
@@ -2654,7 +2690,7 @@
       </c>
       <c r="F16" s="103"/>
     </row>
-    <row r="17" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
+    <row r="17" spans="1:9" ht="17.25" collapsed="1" thickTop="1" thickBot="1">
       <c r="A17" s="115" t="s">
         <v>190</v>
       </c>
@@ -2680,8 +2716,8 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="13.5" thickBot="1"/>
-    <row r="19" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A19" s="155" t="s">
+    <row r="19" spans="1:9" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="A19" s="157" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -2700,7 +2736,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="20" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A20" s="156"/>
       <c r="B20" s="97" t="s">
         <v>184</v>
@@ -2717,7 +2753,7 @@
       </c>
       <c r="F20" s="103"/>
     </row>
-    <row r="21" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
+    <row r="21" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
       <c r="A21" s="156"/>
       <c r="B21" s="99" t="s">
         <v>219</v>
@@ -2734,7 +2770,7 @@
       </c>
       <c r="F21" s="104"/>
     </row>
-    <row r="22" spans="1:9" ht="15" outlineLevel="1">
+    <row r="22" spans="1:9" ht="15" hidden="1" outlineLevel="1">
       <c r="A22" s="156"/>
       <c r="B22" s="99" t="s">
         <v>220</v>
@@ -2751,7 +2787,7 @@
       </c>
       <c r="F22" s="104"/>
     </row>
-    <row r="23" spans="1:9" ht="15" outlineLevel="1">
+    <row r="23" spans="1:9" ht="15" hidden="1" outlineLevel="1">
       <c r="A23" s="156"/>
       <c r="B23" s="99" t="s">
         <v>221</v>
@@ -2768,7 +2804,7 @@
       </c>
       <c r="F23" s="104"/>
     </row>
-    <row r="24" spans="1:9" ht="15" outlineLevel="1">
+    <row r="24" spans="1:9" ht="15" hidden="1" outlineLevel="1">
       <c r="A24" s="156"/>
       <c r="B24" s="99" t="s">
         <v>222</v>
@@ -2788,7 +2824,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15" outlineLevel="1">
+    <row r="25" spans="1:9" ht="15" hidden="1" outlineLevel="1">
       <c r="A25" s="156"/>
       <c r="B25" s="99"/>
       <c r="C25" s="100"/>
@@ -2799,7 +2835,7 @@
       </c>
       <c r="F25" s="104"/>
     </row>
-    <row r="26" spans="1:9" ht="15" outlineLevel="1">
+    <row r="26" spans="1:9" ht="15" hidden="1" outlineLevel="1">
       <c r="A26" s="156"/>
       <c r="B26" s="99"/>
       <c r="C26" s="100"/>
@@ -2810,7 +2846,7 @@
       </c>
       <c r="F26" s="104"/>
     </row>
-    <row r="27" spans="1:9" ht="15" outlineLevel="1">
+    <row r="27" spans="1:9" ht="15" hidden="1" outlineLevel="1">
       <c r="A27" s="156"/>
       <c r="B27" s="99"/>
       <c r="C27" s="100"/>
@@ -2821,7 +2857,7 @@
       </c>
       <c r="F27" s="104"/>
     </row>
-    <row r="28" spans="1:9" ht="15" outlineLevel="1">
+    <row r="28" spans="1:9" ht="15" hidden="1" outlineLevel="1">
       <c r="A28" s="156"/>
       <c r="B28" s="99"/>
       <c r="C28" s="100"/>
@@ -2832,7 +2868,7 @@
       </c>
       <c r="F28" s="104"/>
     </row>
-    <row r="29" spans="1:9" ht="15" outlineLevel="1">
+    <row r="29" spans="1:9" ht="15" hidden="1" outlineLevel="1">
       <c r="A29" s="156"/>
       <c r="B29" s="99"/>
       <c r="C29" s="100"/>
@@ -2843,7 +2879,7 @@
       </c>
       <c r="F29" s="104"/>
     </row>
-    <row r="30" spans="1:9" ht="15" outlineLevel="1">
+    <row r="30" spans="1:9" ht="15" hidden="1" outlineLevel="1">
       <c r="A30" s="156"/>
       <c r="B30" s="99"/>
       <c r="C30" s="100"/>
@@ -2854,7 +2890,7 @@
       </c>
       <c r="F30" s="104"/>
     </row>
-    <row r="31" spans="1:9" ht="15" outlineLevel="1">
+    <row r="31" spans="1:9" ht="15" hidden="1" outlineLevel="1">
       <c r="A31" s="156"/>
       <c r="B31" s="99"/>
       <c r="C31" s="100"/>
@@ -2865,7 +2901,7 @@
       </c>
       <c r="F31" s="104"/>
     </row>
-    <row r="32" spans="1:9" ht="15" outlineLevel="1">
+    <row r="32" spans="1:9" ht="15" hidden="1" outlineLevel="1">
       <c r="A32" s="156"/>
       <c r="B32" s="99"/>
       <c r="C32" s="100"/>
@@ -2876,7 +2912,7 @@
       </c>
       <c r="F32" s="104"/>
     </row>
-    <row r="33" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="33" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A33" s="156"/>
       <c r="B33" s="97" t="s">
         <v>187</v>
@@ -2893,7 +2929,7 @@
       </c>
       <c r="F33" s="103"/>
     </row>
-    <row r="34" spans="1:7" ht="17.25" thickTop="1" thickBot="1">
+    <row r="34" spans="1:7" ht="17.25" collapsed="1" thickTop="1" thickBot="1">
       <c r="A34" s="116">
         <v>1</v>
       </c>
@@ -2920,7 +2956,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A36" s="164" t="s">
+      <c r="A36" s="155" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -3105,7 +3141,7 @@
       </c>
       <c r="F48" s="104"/>
     </row>
-    <row r="49" spans="1:7" ht="15" outlineLevel="1">
+    <row r="49" spans="1:9" ht="15" outlineLevel="1">
       <c r="A49" s="156"/>
       <c r="B49" s="99" t="s">
         <v>227</v>
@@ -3122,7 +3158,7 @@
       </c>
       <c r="F49" s="104"/>
     </row>
-    <row r="50" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="50" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="A50" s="156"/>
       <c r="B50" s="97" t="s">
         <v>187</v>
@@ -3139,7 +3175,7 @@
       </c>
       <c r="F50" s="103"/>
     </row>
-    <row r="51" spans="1:7" ht="17.25" thickTop="1" thickBot="1">
+    <row r="51" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
       <c r="A51" s="115">
         <v>2</v>
       </c>
@@ -3164,9 +3200,9 @@
         <v>-67</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
-    <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="155" t="s">
+    <row r="52" spans="1:9" ht="13.5" thickBot="1"/>
+    <row r="53" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A53" s="157" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -3185,97 +3221,154 @@
         <v>183</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="54" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="A54" s="156"/>
       <c r="B54" s="97" t="s">
         <v>184</v>
       </c>
-      <c r="C54" s="98"/>
-      <c r="D54" s="98"/>
+      <c r="C54" s="98">
+        <v>8924</v>
+      </c>
+      <c r="D54" s="98">
+        <v>8824</v>
+      </c>
       <c r="E54" s="121">
         <f t="shared" ref="E54:E67" si="3">IF(AND(C54&gt;0,D54&gt;0), D54-C54, 0)</f>
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="F54" s="103"/>
     </row>
-    <row r="55" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
+    <row r="55" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A55" s="156"/>
-      <c r="B55" s="99"/>
-      <c r="C55" s="100"/>
-      <c r="D55" s="100"/>
+      <c r="B55" s="99" t="s">
+        <v>230</v>
+      </c>
+      <c r="C55" s="100">
+        <v>9777</v>
+      </c>
+      <c r="D55" s="100">
+        <v>9079</v>
+      </c>
       <c r="E55" s="122">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-698</v>
       </c>
       <c r="F55" s="104"/>
-    </row>
-    <row r="56" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+      <c r="I55" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="15" outlineLevel="1">
       <c r="A56" s="156"/>
-      <c r="B56" s="99"/>
-      <c r="C56" s="100"/>
-      <c r="D56" s="100"/>
+      <c r="B56" s="99" t="s">
+        <v>231</v>
+      </c>
+      <c r="C56" s="100">
+        <v>10760</v>
+      </c>
+      <c r="D56" s="100">
+        <v>10032</v>
+      </c>
       <c r="E56" s="121">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F56" s="104"/>
-    </row>
-    <row r="57" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+        <v>-728</v>
+      </c>
+      <c r="F56" s="104" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="15" outlineLevel="1">
       <c r="A57" s="156"/>
-      <c r="B57" s="99"/>
-      <c r="C57" s="100"/>
-      <c r="D57" s="100"/>
+      <c r="B57" s="99" t="s">
+        <v>233</v>
+      </c>
+      <c r="C57" s="100">
+        <v>11291</v>
+      </c>
+      <c r="D57" s="100">
+        <v>10551</v>
+      </c>
       <c r="E57" s="121">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F57" s="104"/>
-    </row>
-    <row r="58" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+        <v>-740</v>
+      </c>
+      <c r="F57" s="104" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="15" outlineLevel="1">
       <c r="A58" s="156"/>
-      <c r="B58" s="99"/>
-      <c r="C58" s="100"/>
-      <c r="D58" s="100"/>
+      <c r="B58" s="99" t="s">
+        <v>232</v>
+      </c>
+      <c r="C58" s="100">
+        <v>11984</v>
+      </c>
+      <c r="D58" s="100">
+        <v>11243</v>
+      </c>
       <c r="E58" s="121">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F58" s="104"/>
-    </row>
-    <row r="59" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+        <v>-741</v>
+      </c>
+      <c r="F58" s="104" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="15" outlineLevel="1">
       <c r="A59" s="156"/>
-      <c r="B59" s="99"/>
-      <c r="C59" s="100"/>
-      <c r="D59" s="100"/>
+      <c r="B59" s="99" t="s">
+        <v>234</v>
+      </c>
+      <c r="C59" s="100">
+        <v>12595</v>
+      </c>
+      <c r="D59" s="100">
+        <v>11848</v>
+      </c>
       <c r="E59" s="121">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F59" s="104"/>
-    </row>
-    <row r="60" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+        <v>-747</v>
+      </c>
+      <c r="F59" s="104" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="15" outlineLevel="1">
       <c r="A60" s="156"/>
-      <c r="B60" s="99"/>
-      <c r="C60" s="100"/>
-      <c r="D60" s="100"/>
+      <c r="B60" s="99" t="s">
+        <v>235</v>
+      </c>
+      <c r="C60" s="100">
+        <v>13544</v>
+      </c>
+      <c r="D60" s="100">
+        <v>12784</v>
+      </c>
       <c r="E60" s="121">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-760</v>
       </c>
       <c r="F60" s="104"/>
     </row>
-    <row r="61" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="61" spans="1:9" ht="15" outlineLevel="1">
       <c r="A61" s="156"/>
-      <c r="B61" s="99"/>
-      <c r="C61" s="100"/>
-      <c r="D61" s="100"/>
+      <c r="B61" s="99" t="s">
+        <v>236</v>
+      </c>
+      <c r="C61" s="100">
+        <v>13808</v>
+      </c>
+      <c r="D61" s="100">
+        <v>13056</v>
+      </c>
       <c r="E61" s="121">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-752</v>
       </c>
       <c r="F61" s="104"/>
     </row>
-    <row r="62" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="62" spans="1:9" ht="15" outlineLevel="1">
       <c r="A62" s="156"/>
       <c r="B62" s="99"/>
       <c r="C62" s="100"/>
@@ -3286,7 +3379,7 @@
       </c>
       <c r="F62" s="104"/>
     </row>
-    <row r="63" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="63" spans="1:9" ht="15" outlineLevel="1">
       <c r="A63" s="156"/>
       <c r="B63" s="99"/>
       <c r="C63" s="100"/>
@@ -3297,7 +3390,7 @@
       </c>
       <c r="F63" s="104"/>
     </row>
-    <row r="64" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="64" spans="1:9" ht="15" outlineLevel="1">
       <c r="A64" s="156"/>
       <c r="B64" s="99"/>
       <c r="C64" s="100"/>
@@ -3308,20 +3401,28 @@
       </c>
       <c r="F64" s="104"/>
     </row>
-    <row r="65" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="65" spans="1:7" ht="15" outlineLevel="1">
       <c r="A65" s="156"/>
-      <c r="B65" s="99"/>
-      <c r="C65" s="100"/>
-      <c r="D65" s="100"/>
+      <c r="B65" s="99" t="s">
+        <v>228</v>
+      </c>
+      <c r="C65" s="100">
+        <v>14736</v>
+      </c>
+      <c r="D65" s="100">
+        <v>13976</v>
+      </c>
       <c r="E65" s="121">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-760</v>
       </c>
       <c r="F65" s="104"/>
     </row>
-    <row r="66" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="66" spans="1:7" ht="15" outlineLevel="1">
       <c r="A66" s="156"/>
-      <c r="B66" s="99"/>
+      <c r="B66" s="99" t="s">
+        <v>237</v>
+      </c>
       <c r="C66" s="100"/>
       <c r="D66" s="100"/>
       <c r="E66" s="121">
@@ -3330,20 +3431,24 @@
       </c>
       <c r="F66" s="104"/>
     </row>
-    <row r="67" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="67" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="A67" s="156"/>
       <c r="B67" s="97" t="s">
         <v>187</v>
       </c>
-      <c r="C67" s="98"/>
-      <c r="D67" s="98"/>
+      <c r="C67" s="98">
+        <v>14736</v>
+      </c>
+      <c r="D67" s="98">
+        <v>13976</v>
+      </c>
       <c r="E67" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-760</v>
       </c>
       <c r="F67" s="103"/>
     </row>
-    <row r="68" spans="1:7" ht="17.25" collapsed="1" thickTop="1" thickBot="1">
+    <row r="68" spans="1:7" ht="17.25" thickTop="1" thickBot="1">
       <c r="A68" s="116">
         <v>3</v>
       </c>
@@ -3352,25 +3457,25 @@
       </c>
       <c r="C68" s="102">
         <f>C67-C54</f>
-        <v>0</v>
+        <v>5812</v>
       </c>
       <c r="D68" s="102">
         <f>D67-D54</f>
-        <v>0</v>
+        <v>5152</v>
       </c>
       <c r="E68" s="124">
         <f>E67-E54</f>
-        <v>0</v>
+        <v>-660</v>
       </c>
       <c r="F68" s="107"/>
       <c r="G68" s="111">
         <f>E68</f>
-        <v>0</v>
+        <v>-660</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="164" t="s">
+      <c r="A70" s="155" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -3574,7 +3679,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="155" t="s">
+      <c r="A87" s="157" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -3777,7 +3882,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="164" t="s">
+      <c r="A104" s="155" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -3980,7 +4085,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="155" t="s">
+      <c r="A121" s="157" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -4183,7 +4288,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="164" t="s">
+      <c r="A138" s="155" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -4387,19 +4492,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A36:A50"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A8:A16"/>
+    <mergeCell ref="A19:A33"/>
     <mergeCell ref="A138:A152"/>
     <mergeCell ref="A104:A118"/>
     <mergeCell ref="A70:A84"/>
     <mergeCell ref="A121:A135"/>
     <mergeCell ref="A87:A101"/>
     <mergeCell ref="A53:A67"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A8:A16"/>
-    <mergeCell ref="A19:A33"/>
-    <mergeCell ref="A36:A50"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5444,7 +5549,7 @@
       </c>
       <c r="C6" s="132">
         <f ca="1">'FrameCounts World 1'!H2</f>
-        <v>-1.6666666666666667</v>
+        <v>-12.666666666666666</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -5456,7 +5561,7 @@
       </c>
       <c r="C7" s="133">
         <f>C6/60</f>
-        <v>-2.777777777777778E-2</v>
+        <v>-0.21111111111111111</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -5657,10 +5762,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="211" t="s">
+      <c r="A1" s="207" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="212"/>
+      <c r="B1" s="208"/>
       <c r="C1" s="117"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
@@ -5680,127 +5785,142 @@
       <c r="C3" s="118"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="215"/>
-      <c r="B4" s="216"/>
+      <c r="A4" s="211"/>
+      <c r="B4" s="212"/>
       <c r="C4" s="118"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="213" t="s">
+      <c r="A5" s="209" t="s">
         <v>202</v>
       </c>
-      <c r="B5" s="214"/>
+      <c r="B5" s="210"/>
       <c r="C5" s="118"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="205" t="s">
+      <c r="A7" s="215" t="s">
         <v>194</v>
       </c>
-      <c r="B7" s="206"/>
+      <c r="B7" s="216"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="118"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="207" t="s">
+      <c r="A9" s="213" t="s">
         <v>195</v>
       </c>
-      <c r="B9" s="208"/>
+      <c r="B9" s="214"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="209"/>
-      <c r="B10" s="210"/>
+      <c r="A10" s="203"/>
+      <c r="B10" s="204"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="201" t="s">
+      <c r="A11" s="205" t="s">
         <v>196</v>
       </c>
-      <c r="B11" s="202"/>
+      <c r="B11" s="206"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="201" t="s">
+      <c r="A12" s="205" t="s">
         <v>197</v>
       </c>
-      <c r="B12" s="202"/>
+      <c r="B12" s="206"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="201" t="s">
+      <c r="A13" s="205" t="s">
         <v>198</v>
       </c>
-      <c r="B13" s="202"/>
+      <c r="B13" s="206"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="201" t="s">
+      <c r="A14" s="205" t="s">
         <v>199</v>
       </c>
-      <c r="B14" s="202"/>
+      <c r="B14" s="206"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="201" t="s">
+      <c r="A15" s="205" t="s">
         <v>200</v>
       </c>
-      <c r="B15" s="202"/>
+      <c r="B15" s="206"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="201" t="s">
+      <c r="A16" s="205" t="s">
         <v>201</v>
       </c>
-      <c r="B16" s="202"/>
+      <c r="B16" s="206"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="203" t="s">
+      <c r="A17" s="201" t="s">
         <v>203</v>
       </c>
-      <c r="B17" s="204"/>
+      <c r="B17" s="202"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="205" t="s">
+      <c r="A19" s="215" t="s">
         <v>205</v>
       </c>
-      <c r="B19" s="206"/>
+      <c r="B19" s="216"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="118"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="207" t="s">
+      <c r="A21" s="213" t="s">
         <v>206</v>
       </c>
-      <c r="B21" s="208"/>
+      <c r="B21" s="214"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="209"/>
-      <c r="B22" s="210"/>
+      <c r="A22" s="203"/>
+      <c r="B22" s="204"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="201" t="s">
+      <c r="A23" s="205" t="s">
         <v>207</v>
       </c>
-      <c r="B23" s="202"/>
+      <c r="B23" s="206"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="201"/>
-      <c r="B24" s="202"/>
+      <c r="A24" s="205"/>
+      <c r="B24" s="206"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="201" t="s">
+      <c r="A25" s="205" t="s">
         <v>208</v>
       </c>
-      <c r="B25" s="202"/>
+      <c r="B25" s="206"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="201" t="s">
+      <c r="A26" s="205" t="s">
         <v>209</v>
       </c>
-      <c r="B26" s="202"/>
+      <c r="B26" s="206"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="203"/>
-      <c r="B27" s="204"/>
+      <c r="A27" s="201"/>
+      <c r="B27" s="202"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -5809,21 +5929,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -5858,16 +5963,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="160" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="161" t="s">
+      <c r="B1" s="161"/>
+      <c r="C1" s="162" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="163"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -5945,10 +6050,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="157" t="s">
+      <c r="C5" s="158" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="157"/>
+      <c r="D5" s="158"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -5964,10 +6069,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="157" t="s">
+      <c r="C6" s="158" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="158"/>
+      <c r="D6" s="159"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -5985,7 +6090,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="163" t="s">
+      <c r="A8" s="164" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -6124,7 +6229,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="155" t="s">
+      <c r="A19" s="157" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -6328,7 +6433,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="164" t="s">
+      <c r="A36" s="155" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -6532,7 +6637,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="155" t="s">
+      <c r="A53" s="157" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -6736,7 +6841,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="164" t="s">
+      <c r="A70" s="155" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -6940,7 +7045,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="155" t="s">
+      <c r="A87" s="157" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -7143,7 +7248,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="164" t="s">
+      <c r="A104" s="155" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -7346,7 +7451,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="155" t="s">
+      <c r="A121" s="157" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -7549,7 +7654,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="164" t="s">
+      <c r="A138" s="155" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -7753,19 +7858,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A8:A16"/>
-    <mergeCell ref="A19:A33"/>
-    <mergeCell ref="A36:A50"/>
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A138:A152"/>
     <mergeCell ref="A104:A118"/>
     <mergeCell ref="A70:A84"/>
     <mergeCell ref="A121:A135"/>
     <mergeCell ref="A87:A101"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A8:A16"/>
+    <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A36:A50"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7799,16 +7904,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="160" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="161" t="s">
+      <c r="B1" s="161"/>
+      <c r="C1" s="162" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="163"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -7886,10 +7991,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="157" t="s">
+      <c r="C5" s="158" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="157"/>
+      <c r="D5" s="158"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -7905,10 +8010,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="157" t="s">
+      <c r="C6" s="158" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="158"/>
+      <c r="D6" s="159"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -7926,7 +8031,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="163" t="s">
+      <c r="A8" s="164" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -8065,7 +8170,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="155" t="s">
+      <c r="A19" s="157" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -8269,7 +8374,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="164" t="s">
+      <c r="A36" s="155" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -8473,7 +8578,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="155" t="s">
+      <c r="A53" s="157" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -8677,7 +8782,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="164" t="s">
+      <c r="A70" s="155" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -8881,7 +8986,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="155" t="s">
+      <c r="A87" s="157" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -9084,7 +9189,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="164" t="s">
+      <c r="A104" s="155" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -9287,7 +9392,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="155" t="s">
+      <c r="A121" s="157" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -9490,7 +9595,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="164" t="s">
+      <c r="A138" s="155" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -9694,19 +9799,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A36:A50"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A8:A16"/>
+    <mergeCell ref="A19:A33"/>
     <mergeCell ref="A138:A152"/>
     <mergeCell ref="A104:A118"/>
     <mergeCell ref="A70:A84"/>
     <mergeCell ref="A121:A135"/>
     <mergeCell ref="A87:A101"/>
     <mergeCell ref="A53:A67"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A8:A16"/>
-    <mergeCell ref="A19:A33"/>
-    <mergeCell ref="A36:A50"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9740,16 +9845,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="160" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="161" t="s">
+      <c r="B1" s="161"/>
+      <c r="C1" s="162" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="163"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -9827,10 +9932,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="157" t="s">
+      <c r="C5" s="158" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="157"/>
+      <c r="D5" s="158"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -9846,10 +9951,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="157" t="s">
+      <c r="C6" s="158" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="158"/>
+      <c r="D6" s="159"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -9867,7 +9972,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="163" t="s">
+      <c r="A8" s="164" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -10006,7 +10111,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="155" t="s">
+      <c r="A19" s="157" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -10210,7 +10315,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="164" t="s">
+      <c r="A36" s="155" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -10414,7 +10519,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="155" t="s">
+      <c r="A53" s="157" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -10618,7 +10723,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="164" t="s">
+      <c r="A70" s="155" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -10822,7 +10927,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="155" t="s">
+      <c r="A87" s="157" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -11025,7 +11130,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="164" t="s">
+      <c r="A104" s="155" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -11228,7 +11333,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="155" t="s">
+      <c r="A121" s="157" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -11431,7 +11536,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="164" t="s">
+      <c r="A138" s="155" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -11635,19 +11740,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A8:A16"/>
-    <mergeCell ref="A19:A33"/>
-    <mergeCell ref="A36:A50"/>
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A138:A152"/>
     <mergeCell ref="A104:A118"/>
     <mergeCell ref="A70:A84"/>
     <mergeCell ref="A121:A135"/>
     <mergeCell ref="A87:A101"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A8:A16"/>
+    <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A36:A50"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11681,16 +11786,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="160" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="161" t="s">
+      <c r="B1" s="161"/>
+      <c r="C1" s="162" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="163"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -11768,10 +11873,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="157" t="s">
+      <c r="C5" s="158" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="157"/>
+      <c r="D5" s="158"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -11787,10 +11892,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="157" t="s">
+      <c r="C6" s="158" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="158"/>
+      <c r="D6" s="159"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -11808,7 +11913,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="163" t="s">
+      <c r="A8" s="164" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -11947,7 +12052,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="155" t="s">
+      <c r="A19" s="157" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -12151,7 +12256,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="164" t="s">
+      <c r="A36" s="155" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -12355,7 +12460,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="155" t="s">
+      <c r="A53" s="157" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -12559,7 +12664,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="164" t="s">
+      <c r="A70" s="155" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -12763,7 +12868,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="155" t="s">
+      <c r="A87" s="157" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -12966,7 +13071,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="164" t="s">
+      <c r="A104" s="155" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -13169,7 +13274,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="155" t="s">
+      <c r="A121" s="157" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -13372,7 +13477,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="164" t="s">
+      <c r="A138" s="155" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -13576,19 +13681,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A36:A50"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A8:A16"/>
+    <mergeCell ref="A19:A33"/>
     <mergeCell ref="A138:A152"/>
     <mergeCell ref="A104:A118"/>
     <mergeCell ref="A70:A84"/>
     <mergeCell ref="A121:A135"/>
     <mergeCell ref="A87:A101"/>
     <mergeCell ref="A53:A67"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A8:A16"/>
-    <mergeCell ref="A19:A33"/>
-    <mergeCell ref="A36:A50"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13622,16 +13727,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="160" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="161" t="s">
+      <c r="B1" s="161"/>
+      <c r="C1" s="162" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="163"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -13709,10 +13814,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="157" t="s">
+      <c r="C5" s="158" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="157"/>
+      <c r="D5" s="158"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -13728,10 +13833,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="157" t="s">
+      <c r="C6" s="158" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="158"/>
+      <c r="D6" s="159"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -13749,7 +13854,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="163" t="s">
+      <c r="A8" s="164" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -13888,7 +13993,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="155" t="s">
+      <c r="A19" s="157" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -14092,7 +14197,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="164" t="s">
+      <c r="A36" s="155" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -14296,7 +14401,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="155" t="s">
+      <c r="A53" s="157" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -14500,7 +14605,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="164" t="s">
+      <c r="A70" s="155" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -14704,7 +14809,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="155" t="s">
+      <c r="A87" s="157" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -14907,7 +15012,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="164" t="s">
+      <c r="A104" s="155" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -15110,7 +15215,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="155" t="s">
+      <c r="A121" s="157" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -15313,7 +15418,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="164" t="s">
+      <c r="A138" s="155" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -15517,19 +15622,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A8:A16"/>
-    <mergeCell ref="A19:A33"/>
-    <mergeCell ref="A36:A50"/>
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A138:A152"/>
     <mergeCell ref="A104:A118"/>
     <mergeCell ref="A70:A84"/>
     <mergeCell ref="A121:A135"/>
     <mergeCell ref="A87:A101"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A8:A16"/>
+    <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A36:A50"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15563,16 +15668,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="160" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="161" t="s">
+      <c r="B1" s="161"/>
+      <c r="C1" s="162" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="163"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -15650,10 +15755,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="157" t="s">
+      <c r="C5" s="158" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="157"/>
+      <c r="D5" s="158"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -15669,10 +15774,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="157" t="s">
+      <c r="C6" s="158" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="158"/>
+      <c r="D6" s="159"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -15690,7 +15795,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="163" t="s">
+      <c r="A8" s="164" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -15829,7 +15934,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="155" t="s">
+      <c r="A19" s="157" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -16033,7 +16138,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="164" t="s">
+      <c r="A36" s="155" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -16237,7 +16342,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="155" t="s">
+      <c r="A53" s="157" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -16441,7 +16546,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="164" t="s">
+      <c r="A70" s="155" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -16645,7 +16750,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="155" t="s">
+      <c r="A87" s="157" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -16848,7 +16953,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="164" t="s">
+      <c r="A104" s="155" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -17051,7 +17156,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="155" t="s">
+      <c r="A121" s="157" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -17254,7 +17359,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="164" t="s">
+      <c r="A138" s="155" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -17458,19 +17563,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A36:A50"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A8:A16"/>
+    <mergeCell ref="A19:A33"/>
     <mergeCell ref="A138:A152"/>
     <mergeCell ref="A104:A118"/>
     <mergeCell ref="A70:A84"/>
     <mergeCell ref="A121:A135"/>
     <mergeCell ref="A87:A101"/>
     <mergeCell ref="A53:A67"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A8:A16"/>
-    <mergeCell ref="A19:A33"/>
-    <mergeCell ref="A36:A50"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17504,16 +17609,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="160" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="161" t="s">
+      <c r="B1" s="161"/>
+      <c r="C1" s="162" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="163"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -17591,10 +17696,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="157" t="s">
+      <c r="C5" s="158" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="157"/>
+      <c r="D5" s="158"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -17610,10 +17715,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="157" t="s">
+      <c r="C6" s="158" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="158"/>
+      <c r="D6" s="159"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -17631,7 +17736,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="163" t="s">
+      <c r="A8" s="164" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -17770,7 +17875,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="155" t="s">
+      <c r="A19" s="157" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -17974,7 +18079,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="164" t="s">
+      <c r="A36" s="155" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -18178,7 +18283,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="155" t="s">
+      <c r="A53" s="157" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -18382,7 +18487,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="164" t="s">
+      <c r="A70" s="155" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -18586,7 +18691,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="155" t="s">
+      <c r="A87" s="157" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -18789,7 +18894,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="164" t="s">
+      <c r="A104" s="155" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -18992,7 +19097,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="155" t="s">
+      <c r="A121" s="157" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -19195,7 +19300,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="164" t="s">
+      <c r="A138" s="155" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -19399,19 +19504,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A8:A16"/>
-    <mergeCell ref="A19:A33"/>
-    <mergeCell ref="A36:A50"/>
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A138:A152"/>
     <mergeCell ref="A104:A118"/>
     <mergeCell ref="A70:A84"/>
     <mergeCell ref="A121:A135"/>
     <mergeCell ref="A87:A101"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A8:A16"/>
+    <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A36:A50"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19445,13 +19550,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="167" t="s">
+      <c r="A1" s="183" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="167"/>
-      <c r="C1" s="167"/>
-      <c r="D1" s="167"/>
-      <c r="E1" s="167"/>
+      <c r="B1" s="183"/>
+      <c r="C1" s="183"/>
+      <c r="D1" s="183"/>
+      <c r="E1" s="183"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -19481,9 +19586,9 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="168"/>
-      <c r="D3" s="169"/>
-      <c r="E3" s="169"/>
+      <c r="C3" s="184"/>
+      <c r="D3" s="185"/>
+      <c r="E3" s="185"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
@@ -19644,9 +19749,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="170"/>
-      <c r="D21" s="171"/>
-      <c r="E21" s="171"/>
+      <c r="C21" s="167"/>
+      <c r="D21" s="168"/>
+      <c r="E21" s="168"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -21939,9 +22044,9 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="172"/>
-      <c r="D276" s="173"/>
-      <c r="E276" s="173"/>
+      <c r="C276" s="181"/>
+      <c r="D276" s="182"/>
+      <c r="E276" s="182"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
@@ -22101,9 +22206,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="170"/>
-      <c r="D294" s="171"/>
-      <c r="E294" s="171"/>
+      <c r="C294" s="167"/>
+      <c r="D294" s="168"/>
+      <c r="E294" s="168"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -24396,9 +24501,9 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="174"/>
-      <c r="D549" s="175"/>
-      <c r="E549" s="175"/>
+      <c r="C549" s="179"/>
+      <c r="D549" s="180"/>
+      <c r="E549" s="180"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
@@ -24558,9 +24663,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="170"/>
-      <c r="D567" s="171"/>
-      <c r="E567" s="171"/>
+      <c r="C567" s="167"/>
+      <c r="D567" s="168"/>
+      <c r="E567" s="168"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -26853,9 +26958,9 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="176"/>
-      <c r="D822" s="177"/>
-      <c r="E822" s="177"/>
+      <c r="C822" s="177"/>
+      <c r="D822" s="178"/>
+      <c r="E822" s="178"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
@@ -27015,9 +27120,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="170"/>
-      <c r="D840" s="171"/>
-      <c r="E840" s="171"/>
+      <c r="C840" s="167"/>
+      <c r="D840" s="168"/>
+      <c r="E840" s="168"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -29310,9 +29415,9 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="178"/>
-      <c r="D1095" s="179"/>
-      <c r="E1095" s="179"/>
+      <c r="C1095" s="175"/>
+      <c r="D1095" s="176"/>
+      <c r="E1095" s="176"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
@@ -29472,9 +29577,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="170"/>
-      <c r="D1113" s="171"/>
-      <c r="E1113" s="171"/>
+      <c r="C1113" s="167"/>
+      <c r="D1113" s="168"/>
+      <c r="E1113" s="168"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -31767,9 +31872,9 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="180"/>
-      <c r="D1368" s="181"/>
-      <c r="E1368" s="181"/>
+      <c r="C1368" s="173"/>
+      <c r="D1368" s="174"/>
+      <c r="E1368" s="174"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
@@ -31929,9 +32034,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="170"/>
-      <c r="D1386" s="171"/>
-      <c r="E1386" s="171"/>
+      <c r="C1386" s="167"/>
+      <c r="D1386" s="168"/>
+      <c r="E1386" s="168"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -34224,9 +34329,9 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="182"/>
-      <c r="D1641" s="183"/>
-      <c r="E1641" s="183"/>
+      <c r="C1641" s="171"/>
+      <c r="D1641" s="172"/>
+      <c r="E1641" s="172"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
@@ -34386,9 +34491,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="170"/>
-      <c r="D1659" s="171"/>
-      <c r="E1659" s="171"/>
+      <c r="C1659" s="167"/>
+      <c r="D1659" s="168"/>
+      <c r="E1659" s="168"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -36681,9 +36786,9 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="184"/>
-      <c r="D1914" s="185"/>
-      <c r="E1914" s="185"/>
+      <c r="C1914" s="169"/>
+      <c r="D1914" s="170"/>
+      <c r="E1914" s="170"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
@@ -36843,9 +36948,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="170"/>
-      <c r="D1932" s="171"/>
-      <c r="E1932" s="171"/>
+      <c r="C1932" s="167"/>
+      <c r="D1932" s="168"/>
+      <c r="E1932" s="168"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -39135,105 +39240,32 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
-    <mergeCell ref="C1932:E1932"/>
-    <mergeCell ref="C1949:E1949"/>
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C2000:E2000"/>
-    <mergeCell ref="C2017:E2017"/>
-    <mergeCell ref="C1846:E1846"/>
-    <mergeCell ref="C1863:E1863"/>
-    <mergeCell ref="C1880:E1880"/>
-    <mergeCell ref="C1897:E1897"/>
-    <mergeCell ref="C1914:E1914"/>
-    <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C1966:E1966"/>
-    <mergeCell ref="C1983:E1983"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C328:E328"/>
+    <mergeCell ref="C345:E345"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C362:E362"/>
+    <mergeCell ref="C379:E379"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C294:E294"/>
+    <mergeCell ref="C311:E311"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
     <mergeCell ref="C550:E550"/>
     <mergeCell ref="C567:E567"/>
     <mergeCell ref="C464:E464"/>
@@ -39242,36 +39274,109 @@
     <mergeCell ref="C515:E515"/>
     <mergeCell ref="C396:E396"/>
     <mergeCell ref="C413:E413"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
     <mergeCell ref="C430:E430"/>
     <mergeCell ref="C447:E447"/>
     <mergeCell ref="C532:E532"/>
     <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C328:E328"/>
-    <mergeCell ref="C345:E345"/>
-    <mergeCell ref="C362:E362"/>
-    <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C294:E294"/>
-    <mergeCell ref="C311:E311"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1915:E1915"/>
+    <mergeCell ref="C1966:E1966"/>
+    <mergeCell ref="C1983:E1983"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1932:E1932"/>
+    <mergeCell ref="C1949:E1949"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2000:E2000"/>
+    <mergeCell ref="C2017:E2017"/>
+    <mergeCell ref="C1846:E1846"/>
+    <mergeCell ref="C1863:E1863"/>
+    <mergeCell ref="C1880:E1880"/>
+    <mergeCell ref="C1897:E1897"/>
+    <mergeCell ref="C1914:E1914"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
NOW 1-4 is completed with 241 frames faster than Waddle's WIP and extra entertainment goodness
</commit_message>
<xml_diff>
--- a/SPP/SPP.xlsx
+++ b/SPP/SPP.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1762" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="254">
   <si>
     <t>Notes</t>
   </si>
@@ -782,12 +782,6 @@
     <t>Exit Level 777 Coins</t>
   </si>
   <si>
-    <t>Bought in new version before 1-3</t>
-  </si>
-  <si>
-    <t>Bought in old version after 1-3</t>
-  </si>
-  <si>
     <t>716</t>
   </si>
   <si>
@@ -798,6 +792,42 @@
   </si>
   <si>
     <t>812</t>
+  </si>
+  <si>
+    <t>Enter Level</t>
+  </si>
+  <si>
+    <t>Get Toad 1, Get to Pipe</t>
+  </si>
+  <si>
+    <t>558</t>
+  </si>
+  <si>
+    <t>Get to next pipe</t>
+  </si>
+  <si>
+    <t>684</t>
+  </si>
+  <si>
+    <t>Get Toad 2, Get to Pipe</t>
+  </si>
+  <si>
+    <t>928</t>
+  </si>
+  <si>
+    <t>Get Toad 3, Get to Pipe</t>
+  </si>
+  <si>
+    <t>760</t>
+  </si>
+  <si>
+    <t>Get to Wheel</t>
+  </si>
+  <si>
+    <t>Enter 1-5</t>
+  </si>
+  <si>
+    <t>Bought extra vibe</t>
   </si>
 </sst>
 </file>
@@ -1644,6 +1674,28 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="10"/>
       </left>
       <right/>
@@ -1688,28 +1740,6 @@
       </left>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -2019,10 +2049,13 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="9" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -2038,32 +2071,29 @@
     <xf numFmtId="0" fontId="29" fillId="20" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="7" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2099,41 +2129,41 @@
     <xf numFmtId="0" fontId="41" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="41" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="43" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
   </cellXfs>
@@ -2436,11 +2466,11 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:K153"/>
+  <dimension ref="A1:L153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J65" sqref="J64:J65"/>
+      <pane ySplit="6" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -2456,20 +2486,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="161" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="162" t="s">
+      <c r="B1" s="162"/>
+      <c r="C1" s="163" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="164"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
-        <v>-51</v>
+        <v>-148</v>
       </c>
       <c r="I1" s="139" t="s">
         <v>204</v>
@@ -2491,7 +2521,7 @@
       <c r="G2" s="138"/>
       <c r="H2" s="142">
         <f>IF(H1&lt;3600,H1/60,QUOTIENT(H1, 3600))</f>
-        <v>-0.85</v>
+        <v>-2.4666666666666668</v>
       </c>
       <c r="I2" s="139" t="str">
         <f>IF(H1&lt;3600,"Seconds","Minutes")</f>
@@ -2543,10 +2573,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="158" t="s">
+      <c r="C5" s="159" t="s">
         <v>216</v>
       </c>
-      <c r="D5" s="158"/>
+      <c r="D5" s="159"/>
       <c r="E5" s="145" t="s">
         <v>217</v>
       </c>
@@ -2566,10 +2596,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="158" t="s">
+      <c r="C6" s="159" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="159"/>
+      <c r="D6" s="160"/>
       <c r="E6" s="145"/>
       <c r="F6" s="141"/>
       <c r="G6" s="138"/>
@@ -2587,7 +2617,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="164" t="s">
+      <c r="A8" s="165" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -2730,7 +2760,7 @@
     </row>
     <row r="18" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A19" s="165" t="s">
+      <c r="A19" s="156" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -2969,7 +2999,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A36" s="156" t="s">
+      <c r="A36" s="158" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -3154,7 +3184,7 @@
       </c>
       <c r="F48" s="104"/>
     </row>
-    <row r="49" spans="1:9" ht="15" outlineLevel="1">
+    <row r="49" spans="1:12" ht="15" outlineLevel="1">
       <c r="A49" s="157"/>
       <c r="B49" s="99" t="s">
         <v>227</v>
@@ -3171,7 +3201,7 @@
       </c>
       <c r="F49" s="104"/>
     </row>
-    <row r="50" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="50" spans="1:12" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="A50" s="157"/>
       <c r="B50" s="97" t="s">
         <v>187</v>
@@ -3188,7 +3218,7 @@
       </c>
       <c r="F50" s="103"/>
     </row>
-    <row r="51" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
+    <row r="51" spans="1:12" ht="17.25" thickTop="1" thickBot="1">
       <c r="A51" s="115">
         <v>2</v>
       </c>
@@ -3213,9 +3243,9 @@
         <v>-67</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="13.5" thickBot="1"/>
-    <row r="53" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A53" s="165" t="s">
+    <row r="52" spans="1:12" ht="13.5" thickBot="1"/>
+    <row r="53" spans="1:12" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A53" s="156" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -3234,7 +3264,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="54" spans="1:12" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="A54" s="157"/>
       <c r="B54" s="97" t="s">
         <v>184</v>
@@ -3251,7 +3281,7 @@
       </c>
       <c r="F54" s="103"/>
     </row>
-    <row r="55" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
+    <row r="55" spans="1:12" ht="16.5" outlineLevel="1" thickTop="1" thickBot="1">
       <c r="A55" s="157"/>
       <c r="B55" s="99" t="s">
         <v>230</v>
@@ -3259,19 +3289,20 @@
       <c r="C55" s="155">
         <v>9777</v>
       </c>
-      <c r="D55" s="100">
-        <v>9817</v>
+      <c r="D55" s="155">
+        <v>9964</v>
       </c>
       <c r="E55" s="122">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>187</v>
       </c>
       <c r="F55" s="104"/>
       <c r="I55" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="15" outlineLevel="1">
+        <v>253</v>
+      </c>
+      <c r="L55" s="98"/>
+    </row>
+    <row r="56" spans="1:12" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A56" s="157"/>
       <c r="B56" s="99" t="s">
         <v>231</v>
@@ -3279,18 +3310,19 @@
       <c r="C56" s="155">
         <v>10760</v>
       </c>
-      <c r="D56" s="100">
-        <v>10753</v>
+      <c r="D56" s="155">
+        <v>10900</v>
       </c>
       <c r="E56" s="121">
         <f t="shared" si="3"/>
-        <v>-7</v>
+        <v>140</v>
       </c>
       <c r="F56" s="104" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="15" outlineLevel="1">
+        <v>238</v>
+      </c>
+      <c r="L56" s="155"/>
+    </row>
+    <row r="57" spans="1:12" ht="15" outlineLevel="1">
       <c r="A57" s="157"/>
       <c r="B57" s="99" t="s">
         <v>233</v>
@@ -3298,18 +3330,19 @@
       <c r="C57" s="155">
         <v>11291</v>
       </c>
-      <c r="D57" s="100">
-        <v>11272</v>
+      <c r="D57" s="155">
+        <v>11419</v>
       </c>
       <c r="E57" s="121">
         <f t="shared" si="3"/>
-        <v>-19</v>
+        <v>128</v>
       </c>
       <c r="F57" s="104" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="15" outlineLevel="1">
+        <v>239</v>
+      </c>
+      <c r="L57" s="155"/>
+    </row>
+    <row r="58" spans="1:12" ht="15" outlineLevel="1">
       <c r="A58" s="157"/>
       <c r="B58" s="99" t="s">
         <v>232</v>
@@ -3317,18 +3350,19 @@
       <c r="C58" s="155">
         <v>11984</v>
       </c>
-      <c r="D58" s="100">
-        <v>11964</v>
+      <c r="D58" s="155">
+        <v>12111</v>
       </c>
       <c r="E58" s="121">
         <f t="shared" si="3"/>
-        <v>-20</v>
+        <v>127</v>
       </c>
       <c r="F58" s="104" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="15" outlineLevel="1">
+        <v>240</v>
+      </c>
+      <c r="L58" s="155"/>
+    </row>
+    <row r="59" spans="1:12" ht="15" outlineLevel="1">
       <c r="A59" s="157"/>
       <c r="B59" s="99" t="s">
         <v>234</v>
@@ -3336,18 +3370,19 @@
       <c r="C59" s="155">
         <v>12595</v>
       </c>
-      <c r="D59" s="100">
-        <v>12569</v>
+      <c r="D59" s="155">
+        <v>12716</v>
       </c>
       <c r="E59" s="121">
         <f t="shared" si="3"/>
-        <v>-26</v>
+        <v>121</v>
       </c>
       <c r="F59" s="104" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="15" outlineLevel="1">
+        <v>240</v>
+      </c>
+      <c r="L59" s="155"/>
+    </row>
+    <row r="60" spans="1:12" ht="15" outlineLevel="1">
       <c r="A60" s="157"/>
       <c r="B60" s="99" t="s">
         <v>235</v>
@@ -3355,18 +3390,19 @@
       <c r="C60" s="155">
         <v>13544</v>
       </c>
-      <c r="D60" s="100">
-        <v>13505</v>
+      <c r="D60" s="155">
+        <v>13652</v>
       </c>
       <c r="E60" s="121">
         <f t="shared" si="3"/>
-        <v>-39</v>
+        <v>108</v>
       </c>
       <c r="F60" s="104" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="15" outlineLevel="1">
+        <v>241</v>
+      </c>
+      <c r="L60" s="155"/>
+    </row>
+    <row r="61" spans="1:12" ht="15" outlineLevel="1">
       <c r="A61" s="157"/>
       <c r="B61" s="99" t="s">
         <v>236</v>
@@ -3374,51 +3410,55 @@
       <c r="C61" s="155">
         <v>13808</v>
       </c>
-      <c r="D61" s="100">
-        <v>13766</v>
+      <c r="D61" s="155">
+        <v>13913</v>
       </c>
       <c r="E61" s="121">
         <f t="shared" si="3"/>
-        <v>-42</v>
+        <v>105</v>
       </c>
       <c r="F61" s="104" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" ht="15" outlineLevel="1">
+        <v>241</v>
+      </c>
+      <c r="L61" s="155"/>
+    </row>
+    <row r="62" spans="1:12" ht="15" outlineLevel="1">
       <c r="A62" s="157"/>
       <c r="B62" s="99"/>
       <c r="C62" s="155"/>
-      <c r="D62" s="100"/>
+      <c r="D62" s="155"/>
       <c r="E62" s="121">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F62" s="104"/>
-    </row>
-    <row r="63" spans="1:9" ht="15" outlineLevel="1">
+      <c r="L62" s="155"/>
+    </row>
+    <row r="63" spans="1:12" ht="15" outlineLevel="1">
       <c r="A63" s="157"/>
       <c r="B63" s="99"/>
       <c r="C63" s="155"/>
-      <c r="D63" s="100"/>
+      <c r="D63" s="155"/>
       <c r="E63" s="121">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F63" s="104"/>
-    </row>
-    <row r="64" spans="1:9" ht="15" outlineLevel="1">
+      <c r="L63" s="155"/>
+    </row>
+    <row r="64" spans="1:12" ht="15" outlineLevel="1">
       <c r="A64" s="157"/>
       <c r="B64" s="99"/>
       <c r="C64" s="155"/>
-      <c r="D64" s="100"/>
+      <c r="D64" s="155"/>
       <c r="E64" s="121">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F64" s="104"/>
-    </row>
-    <row r="65" spans="1:9" ht="15" outlineLevel="1">
+      <c r="L64" s="155"/>
+    </row>
+    <row r="65" spans="1:12" ht="15" outlineLevel="1">
       <c r="A65" s="157"/>
       <c r="B65" s="99" t="s">
         <v>228</v>
@@ -3426,29 +3466,31 @@
       <c r="C65" s="155">
         <v>14736</v>
       </c>
-      <c r="D65" s="100">
-        <v>14685</v>
+      <c r="D65" s="155">
+        <v>14832</v>
       </c>
       <c r="E65" s="121">
         <f t="shared" si="3"/>
-        <v>-51</v>
+        <v>96</v>
       </c>
       <c r="F65" s="104"/>
-    </row>
-    <row r="66" spans="1:9" ht="15" outlineLevel="1">
+      <c r="L65" s="155"/>
+    </row>
+    <row r="66" spans="1:12" ht="15" outlineLevel="1">
       <c r="A66" s="157"/>
       <c r="B66" s="99" t="s">
         <v>237</v>
       </c>
       <c r="C66" s="155"/>
-      <c r="D66" s="100"/>
+      <c r="D66" s="155"/>
       <c r="E66" s="121">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F66" s="104"/>
-    </row>
-    <row r="67" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="L66" s="155"/>
+    </row>
+    <row r="67" spans="1:12" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="A67" s="157"/>
       <c r="B67" s="97" t="s">
         <v>187</v>
@@ -3457,15 +3499,16 @@
         <v>14736</v>
       </c>
       <c r="D67" s="98">
-        <v>14685</v>
+        <v>14832</v>
       </c>
       <c r="E67" s="123">
         <f t="shared" si="3"/>
-        <v>-51</v>
+        <v>96</v>
       </c>
       <c r="F67" s="103"/>
-    </row>
-    <row r="68" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
+      <c r="L67" s="155"/>
+    </row>
+    <row r="68" spans="1:12" ht="17.25" thickTop="1" thickBot="1">
       <c r="A68" s="116">
         <v>3</v>
       </c>
@@ -3478,21 +3521,22 @@
       </c>
       <c r="D68" s="102">
         <f>D67-D54</f>
-        <v>5861</v>
+        <v>6008</v>
       </c>
       <c r="E68" s="124">
         <f>E67-E54</f>
-        <v>49</v>
+        <v>196</v>
       </c>
       <c r="F68" s="107"/>
       <c r="G68" s="111">
         <f>E68</f>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" ht="13.5" thickBot="1"/>
-    <row r="70" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A70" s="156" t="s">
+        <v>196</v>
+      </c>
+      <c r="L68" s="98"/>
+    </row>
+    <row r="69" spans="1:12" ht="13.5" thickBot="1"/>
+    <row r="70" spans="1:12" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A70" s="158" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -3511,101 +3555,138 @@
         <v>183</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="71" spans="1:12" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="A71" s="157"/>
       <c r="B71" s="97" t="s">
         <v>184</v>
       </c>
       <c r="C71" s="98">
-        <v>14685</v>
+        <v>14736</v>
       </c>
       <c r="D71" s="98">
-        <v>14685</v>
+        <v>14832</v>
       </c>
       <c r="E71" s="121">
         <f t="shared" ref="E71:E84" si="4">IF(AND(C71&gt;0,D71&gt;0), D71-C71, 0)</f>
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="F71" s="103"/>
-    </row>
-    <row r="72" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
+      <c r="L71" s="98"/>
+    </row>
+    <row r="72" spans="1:12" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A72" s="157"/>
-      <c r="B72" s="99"/>
+      <c r="B72" s="99" t="s">
+        <v>242</v>
+      </c>
       <c r="C72" s="100">
-        <v>14940</v>
+        <v>14994</v>
       </c>
       <c r="D72" s="100">
-        <v>14940</v>
+        <v>15087</v>
       </c>
       <c r="E72" s="122">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="F72" s="104"/>
-      <c r="I72" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="15" outlineLevel="1">
+      <c r="L72" s="100"/>
+    </row>
+    <row r="73" spans="1:12" ht="15" outlineLevel="1">
       <c r="A73" s="157"/>
-      <c r="B73" s="99"/>
+      <c r="B73" s="99" t="s">
+        <v>243</v>
+      </c>
       <c r="C73" s="100">
-        <v>15010</v>
+        <v>16123</v>
       </c>
       <c r="D73" s="100">
-        <v>15010</v>
+        <v>16130</v>
       </c>
       <c r="E73" s="121">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F73" s="104"/>
-    </row>
-    <row r="74" spans="1:9" ht="15" outlineLevel="1">
+        <v>7</v>
+      </c>
+      <c r="F73" s="104" t="s">
+        <v>244</v>
+      </c>
+      <c r="L73" s="100"/>
+    </row>
+    <row r="74" spans="1:12" ht="15" outlineLevel="1">
       <c r="A74" s="157"/>
-      <c r="B74" s="99"/>
-      <c r="C74" s="100"/>
-      <c r="D74" s="100"/>
+      <c r="B74" s="99" t="s">
+        <v>245</v>
+      </c>
+      <c r="C74" s="100">
+        <v>16883</v>
+      </c>
+      <c r="D74" s="100">
+        <v>16881</v>
+      </c>
       <c r="E74" s="121">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F74" s="104"/>
-    </row>
-    <row r="75" spans="1:9" ht="15" outlineLevel="1">
+        <v>-2</v>
+      </c>
+      <c r="F74" s="104" t="s">
+        <v>246</v>
+      </c>
+      <c r="L74" s="100"/>
+    </row>
+    <row r="75" spans="1:12" ht="15" outlineLevel="1">
       <c r="A75" s="157"/>
-      <c r="B75" s="99"/>
-      <c r="C75" s="100"/>
-      <c r="D75" s="100"/>
+      <c r="B75" s="99" t="s">
+        <v>247</v>
+      </c>
+      <c r="C75" s="100">
+        <v>17971</v>
+      </c>
+      <c r="D75" s="100">
+        <v>17904</v>
+      </c>
       <c r="E75" s="121">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F75" s="104"/>
-    </row>
-    <row r="76" spans="1:9" ht="15" outlineLevel="1">
+        <v>-67</v>
+      </c>
+      <c r="F75" s="104" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" ht="15" outlineLevel="1">
       <c r="A76" s="157"/>
-      <c r="B76" s="99"/>
-      <c r="C76" s="100"/>
-      <c r="D76" s="100"/>
+      <c r="B76" s="99" t="s">
+        <v>249</v>
+      </c>
+      <c r="C76" s="100">
+        <v>19416</v>
+      </c>
+      <c r="D76" s="100">
+        <v>19305</v>
+      </c>
       <c r="E76" s="121">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F76" s="104"/>
-    </row>
-    <row r="77" spans="1:9" ht="15" outlineLevel="1">
+        <v>-111</v>
+      </c>
+      <c r="F76" s="104" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="15" outlineLevel="1">
       <c r="A77" s="157"/>
-      <c r="B77" s="99"/>
-      <c r="C77" s="100"/>
-      <c r="D77" s="100"/>
+      <c r="B77" s="99" t="s">
+        <v>251</v>
+      </c>
+      <c r="C77" s="100">
+        <v>20430</v>
+      </c>
+      <c r="D77" s="100">
+        <v>20310</v>
+      </c>
       <c r="E77" s="121">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F77" s="104"/>
     </row>
-    <row r="78" spans="1:9" ht="15" outlineLevel="1">
+    <row r="78" spans="1:12" ht="15" outlineLevel="1">
       <c r="A78" s="157"/>
       <c r="B78" s="99"/>
       <c r="C78" s="100"/>
@@ -3616,7 +3697,7 @@
       </c>
       <c r="F78" s="104"/>
     </row>
-    <row r="79" spans="1:9" ht="15" outlineLevel="1">
+    <row r="79" spans="1:12" ht="15" outlineLevel="1">
       <c r="A79" s="157"/>
       <c r="B79" s="99"/>
       <c r="C79" s="100"/>
@@ -3627,7 +3708,7 @@
       </c>
       <c r="F79" s="104"/>
     </row>
-    <row r="80" spans="1:9" ht="15" outlineLevel="1">
+    <row r="80" spans="1:12" ht="15" outlineLevel="1">
       <c r="A80" s="157"/>
       <c r="B80" s="99"/>
       <c r="C80" s="100"/>
@@ -3676,11 +3757,15 @@
       <c r="B84" s="97" t="s">
         <v>187</v>
       </c>
-      <c r="C84" s="98"/>
-      <c r="D84" s="98"/>
+      <c r="C84" s="98">
+        <v>20850</v>
+      </c>
+      <c r="D84" s="98">
+        <v>20705</v>
+      </c>
       <c r="E84" s="123">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-145</v>
       </c>
       <c r="F84" s="103"/>
     </row>
@@ -3693,25 +3778,25 @@
       </c>
       <c r="C85" s="102">
         <f>C84-C71</f>
-        <v>-14685</v>
+        <v>6114</v>
       </c>
       <c r="D85" s="102">
         <f>D84-D71</f>
-        <v>-14685</v>
+        <v>5873</v>
       </c>
       <c r="E85" s="124">
         <f>E84-E71</f>
-        <v>0</v>
+        <v>-241</v>
       </c>
       <c r="F85" s="106"/>
       <c r="G85" s="111">
         <f>E85</f>
-        <v>0</v>
+        <v>-241</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
-    <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="165" t="s">
+    <row r="87" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A87" s="156" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -3730,31 +3815,41 @@
         <v>183</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="88" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="A88" s="157"/>
       <c r="B88" s="97" t="s">
         <v>184</v>
       </c>
-      <c r="C88" s="98"/>
-      <c r="D88" s="98"/>
+      <c r="C88" s="98">
+        <v>20850</v>
+      </c>
+      <c r="D88" s="98">
+        <v>20725</v>
+      </c>
       <c r="E88" s="121">
         <f t="shared" ref="E88:E101" si="5">IF(AND(C88&gt;0,D88&gt;0), D88-C88, 0)</f>
-        <v>0</v>
+        <v>-125</v>
       </c>
       <c r="F88" s="103"/>
     </row>
-    <row r="89" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
+    <row r="89" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A89" s="157"/>
-      <c r="B89" s="99"/>
-      <c r="C89" s="100"/>
-      <c r="D89" s="100"/>
+      <c r="B89" s="99" t="s">
+        <v>252</v>
+      </c>
+      <c r="C89" s="100">
+        <v>21141</v>
+      </c>
+      <c r="D89" s="100">
+        <v>21013</v>
+      </c>
       <c r="E89" s="122">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-128</v>
       </c>
       <c r="F89" s="104"/>
     </row>
-    <row r="90" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="90" spans="1:7" ht="15" outlineLevel="1">
       <c r="A90" s="157"/>
       <c r="B90" s="99"/>
       <c r="C90" s="100"/>
@@ -3765,7 +3860,7 @@
       </c>
       <c r="F90" s="104"/>
     </row>
-    <row r="91" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="91" spans="1:7" ht="15" outlineLevel="1">
       <c r="A91" s="157"/>
       <c r="B91" s="99"/>
       <c r="C91" s="100"/>
@@ -3776,7 +3871,7 @@
       </c>
       <c r="F91" s="104"/>
     </row>
-    <row r="92" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="92" spans="1:7" ht="15" outlineLevel="1">
       <c r="A92" s="157"/>
       <c r="B92" s="99"/>
       <c r="C92" s="100"/>
@@ -3787,7 +3882,7 @@
       </c>
       <c r="F92" s="104"/>
     </row>
-    <row r="93" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="93" spans="1:7" ht="15" outlineLevel="1">
       <c r="A93" s="157"/>
       <c r="B93" s="99"/>
       <c r="C93" s="100"/>
@@ -3798,7 +3893,7 @@
       </c>
       <c r="F93" s="104"/>
     </row>
-    <row r="94" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="94" spans="1:7" ht="15" outlineLevel="1">
       <c r="A94" s="157"/>
       <c r="B94" s="99"/>
       <c r="C94" s="100"/>
@@ -3809,7 +3904,7 @@
       </c>
       <c r="F94" s="104"/>
     </row>
-    <row r="95" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="95" spans="1:7" ht="15" outlineLevel="1">
       <c r="A95" s="157"/>
       <c r="B95" s="99"/>
       <c r="C95" s="100"/>
@@ -3820,7 +3915,7 @@
       </c>
       <c r="F95" s="104"/>
     </row>
-    <row r="96" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="96" spans="1:7" ht="15" outlineLevel="1">
       <c r="A96" s="157"/>
       <c r="B96" s="99"/>
       <c r="C96" s="100"/>
@@ -3831,7 +3926,7 @@
       </c>
       <c r="F96" s="104"/>
     </row>
-    <row r="97" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="97" spans="1:7" ht="15" outlineLevel="1">
       <c r="A97" s="157"/>
       <c r="B97" s="99"/>
       <c r="C97" s="100"/>
@@ -3842,7 +3937,7 @@
       </c>
       <c r="F97" s="104"/>
     </row>
-    <row r="98" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="98" spans="1:7" ht="15" outlineLevel="1">
       <c r="A98" s="157"/>
       <c r="B98" s="99"/>
       <c r="C98" s="100"/>
@@ -3853,7 +3948,7 @@
       </c>
       <c r="F98" s="104"/>
     </row>
-    <row r="99" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="99" spans="1:7" ht="15" outlineLevel="1">
       <c r="A99" s="157"/>
       <c r="B99" s="99"/>
       <c r="C99" s="100"/>
@@ -3864,7 +3959,7 @@
       </c>
       <c r="F99" s="104"/>
     </row>
-    <row r="100" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="100" spans="1:7" ht="15" outlineLevel="1">
       <c r="A100" s="157"/>
       <c r="B100" s="99"/>
       <c r="C100" s="100"/>
@@ -3875,20 +3970,24 @@
       </c>
       <c r="F100" s="104"/>
     </row>
-    <row r="101" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="101" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="A101" s="157"/>
       <c r="B101" s="97" t="s">
         <v>187</v>
       </c>
-      <c r="C101" s="98"/>
-      <c r="D101" s="98"/>
+      <c r="C101" s="98">
+        <v>21141</v>
+      </c>
+      <c r="D101" s="98">
+        <v>21013</v>
+      </c>
       <c r="E101" s="123">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-128</v>
       </c>
       <c r="F101" s="103"/>
     </row>
-    <row r="102" spans="1:7" ht="17.25" collapsed="1" thickTop="1" thickBot="1">
+    <row r="102" spans="1:7" ht="17.25" thickTop="1" thickBot="1">
       <c r="A102" s="116">
         <v>5</v>
       </c>
@@ -3897,24 +3996,24 @@
       </c>
       <c r="C102" s="102">
         <f>C101-C88</f>
-        <v>0</v>
+        <v>291</v>
       </c>
       <c r="D102" s="102">
         <f>D101-D88</f>
-        <v>0</v>
+        <v>288</v>
       </c>
       <c r="E102" s="124">
         <f>E101-E88</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="F102" s="107"/>
       <c r="G102" s="111">
         <f>E102</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="156" t="s">
+      <c r="A104" s="158" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -4117,7 +4216,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="165" t="s">
+      <c r="A121" s="156" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -4320,7 +4419,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="156" t="s">
+      <c r="A138" s="158" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -4524,12 +4623,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="A138:A152"/>
-    <mergeCell ref="A104:A118"/>
-    <mergeCell ref="A70:A84"/>
-    <mergeCell ref="A121:A135"/>
-    <mergeCell ref="A87:A101"/>
     <mergeCell ref="A36:A50"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
@@ -4537,6 +4630,12 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="A138:A152"/>
+    <mergeCell ref="A104:A118"/>
+    <mergeCell ref="A70:A84"/>
+    <mergeCell ref="A121:A135"/>
+    <mergeCell ref="A87:A101"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5581,7 +5680,7 @@
       </c>
       <c r="C6" s="132">
         <f ca="1">'FrameCounts World 1'!H2</f>
-        <v>-0.85</v>
+        <v>-2.4666666666666668</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -5593,7 +5692,7 @@
       </c>
       <c r="C7" s="133">
         <f>C6/60</f>
-        <v>-1.4166666666666666E-2</v>
+        <v>-4.1111111111111112E-2</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -5794,10 +5893,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="212" t="s">
+      <c r="A1" s="208" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="213"/>
+      <c r="B1" s="209"/>
       <c r="C1" s="117"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
@@ -5817,127 +5916,142 @@
       <c r="C3" s="118"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="216"/>
-      <c r="B4" s="217"/>
+      <c r="A4" s="212"/>
+      <c r="B4" s="213"/>
       <c r="C4" s="118"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="214" t="s">
+      <c r="A5" s="210" t="s">
         <v>202</v>
       </c>
-      <c r="B5" s="215"/>
+      <c r="B5" s="211"/>
       <c r="C5" s="118"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="206" t="s">
+      <c r="A7" s="216" t="s">
         <v>194</v>
       </c>
-      <c r="B7" s="207"/>
+      <c r="B7" s="217"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="118"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="208" t="s">
+      <c r="A9" s="214" t="s">
         <v>195</v>
       </c>
-      <c r="B9" s="209"/>
+      <c r="B9" s="215"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="210"/>
-      <c r="B10" s="211"/>
+      <c r="A10" s="204"/>
+      <c r="B10" s="205"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="202" t="s">
+      <c r="A11" s="206" t="s">
         <v>196</v>
       </c>
-      <c r="B11" s="203"/>
+      <c r="B11" s="207"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="202" t="s">
+      <c r="A12" s="206" t="s">
         <v>197</v>
       </c>
-      <c r="B12" s="203"/>
+      <c r="B12" s="207"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="202" t="s">
+      <c r="A13" s="206" t="s">
         <v>198</v>
       </c>
-      <c r="B13" s="203"/>
+      <c r="B13" s="207"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="202" t="s">
+      <c r="A14" s="206" t="s">
         <v>199</v>
       </c>
-      <c r="B14" s="203"/>
+      <c r="B14" s="207"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="202" t="s">
+      <c r="A15" s="206" t="s">
         <v>200</v>
       </c>
-      <c r="B15" s="203"/>
+      <c r="B15" s="207"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="202" t="s">
+      <c r="A16" s="206" t="s">
         <v>201</v>
       </c>
-      <c r="B16" s="203"/>
+      <c r="B16" s="207"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="204" t="s">
+      <c r="A17" s="202" t="s">
         <v>203</v>
       </c>
-      <c r="B17" s="205"/>
+      <c r="B17" s="203"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="206" t="s">
+      <c r="A19" s="216" t="s">
         <v>205</v>
       </c>
-      <c r="B19" s="207"/>
+      <c r="B19" s="217"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="118"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="208" t="s">
+      <c r="A21" s="214" t="s">
         <v>206</v>
       </c>
-      <c r="B21" s="209"/>
+      <c r="B21" s="215"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="210"/>
-      <c r="B22" s="211"/>
+      <c r="A22" s="204"/>
+      <c r="B22" s="205"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="202" t="s">
+      <c r="A23" s="206" t="s">
         <v>207</v>
       </c>
-      <c r="B23" s="203"/>
+      <c r="B23" s="207"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="202"/>
-      <c r="B24" s="203"/>
+      <c r="A24" s="206"/>
+      <c r="B24" s="207"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="202" t="s">
+      <c r="A25" s="206" t="s">
         <v>208</v>
       </c>
-      <c r="B25" s="203"/>
+      <c r="B25" s="207"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="202" t="s">
+      <c r="A26" s="206" t="s">
         <v>209</v>
       </c>
-      <c r="B26" s="203"/>
+      <c r="B26" s="207"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="204"/>
-      <c r="B27" s="205"/>
+      <c r="A27" s="202"/>
+      <c r="B27" s="203"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -5946,21 +6060,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -5995,16 +6094,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="161" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="162" t="s">
+      <c r="B1" s="162"/>
+      <c r="C1" s="163" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="164"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -6082,10 +6181,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="158" t="s">
+      <c r="C5" s="159" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="158"/>
+      <c r="D5" s="159"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -6101,10 +6200,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="158" t="s">
+      <c r="C6" s="159" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="159"/>
+      <c r="D6" s="160"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -6122,7 +6221,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="164" t="s">
+      <c r="A8" s="165" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -6261,7 +6360,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="165" t="s">
+      <c r="A19" s="156" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -6465,7 +6564,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="156" t="s">
+      <c r="A36" s="158" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -6669,7 +6768,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="165" t="s">
+      <c r="A53" s="156" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -6873,7 +6972,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="156" t="s">
+      <c r="A70" s="158" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -7077,7 +7176,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="165" t="s">
+      <c r="A87" s="156" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -7280,7 +7379,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="156" t="s">
+      <c r="A104" s="158" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -7483,7 +7582,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="165" t="s">
+      <c r="A121" s="156" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -7686,7 +7785,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="156" t="s">
+      <c r="A138" s="158" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -7890,6 +7989,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="A138:A152"/>
+    <mergeCell ref="A104:A118"/>
+    <mergeCell ref="A70:A84"/>
+    <mergeCell ref="A121:A135"/>
+    <mergeCell ref="A87:A101"/>
     <mergeCell ref="A36:A50"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
@@ -7897,12 +8002,6 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
-    <mergeCell ref="A138:A152"/>
-    <mergeCell ref="A104:A118"/>
-    <mergeCell ref="A70:A84"/>
-    <mergeCell ref="A121:A135"/>
-    <mergeCell ref="A87:A101"/>
-    <mergeCell ref="A53:A67"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7936,16 +8035,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="161" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="162" t="s">
+      <c r="B1" s="162"/>
+      <c r="C1" s="163" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="164"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -8023,10 +8122,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="158" t="s">
+      <c r="C5" s="159" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="158"/>
+      <c r="D5" s="159"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -8042,10 +8141,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="158" t="s">
+      <c r="C6" s="159" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="159"/>
+      <c r="D6" s="160"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -8063,7 +8162,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="164" t="s">
+      <c r="A8" s="165" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -8202,7 +8301,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="165" t="s">
+      <c r="A19" s="156" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -8406,7 +8505,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="156" t="s">
+      <c r="A36" s="158" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -8610,7 +8709,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="165" t="s">
+      <c r="A53" s="156" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -8814,7 +8913,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="156" t="s">
+      <c r="A70" s="158" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -9018,7 +9117,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="165" t="s">
+      <c r="A87" s="156" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -9221,7 +9320,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="156" t="s">
+      <c r="A104" s="158" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -9424,7 +9523,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="165" t="s">
+      <c r="A121" s="156" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -9627,7 +9726,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="156" t="s">
+      <c r="A138" s="158" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -9831,12 +9930,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="A138:A152"/>
-    <mergeCell ref="A104:A118"/>
-    <mergeCell ref="A70:A84"/>
-    <mergeCell ref="A121:A135"/>
-    <mergeCell ref="A87:A101"/>
     <mergeCell ref="A36:A50"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
@@ -9844,6 +9937,12 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="A138:A152"/>
+    <mergeCell ref="A104:A118"/>
+    <mergeCell ref="A70:A84"/>
+    <mergeCell ref="A121:A135"/>
+    <mergeCell ref="A87:A101"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9877,16 +9976,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="161" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="162" t="s">
+      <c r="B1" s="162"/>
+      <c r="C1" s="163" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="164"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -9964,10 +10063,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="158" t="s">
+      <c r="C5" s="159" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="158"/>
+      <c r="D5" s="159"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -9983,10 +10082,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="158" t="s">
+      <c r="C6" s="159" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="159"/>
+      <c r="D6" s="160"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -10004,7 +10103,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="164" t="s">
+      <c r="A8" s="165" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -10143,7 +10242,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="165" t="s">
+      <c r="A19" s="156" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -10347,7 +10446,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="156" t="s">
+      <c r="A36" s="158" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -10551,7 +10650,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="165" t="s">
+      <c r="A53" s="156" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -10755,7 +10854,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="156" t="s">
+      <c r="A70" s="158" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -10959,7 +11058,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="165" t="s">
+      <c r="A87" s="156" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -11162,7 +11261,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="156" t="s">
+      <c r="A104" s="158" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -11365,7 +11464,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="165" t="s">
+      <c r="A121" s="156" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -11568,7 +11667,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="156" t="s">
+      <c r="A138" s="158" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -11772,6 +11871,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="A138:A152"/>
+    <mergeCell ref="A104:A118"/>
+    <mergeCell ref="A70:A84"/>
+    <mergeCell ref="A121:A135"/>
+    <mergeCell ref="A87:A101"/>
     <mergeCell ref="A36:A50"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
@@ -11779,12 +11884,6 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
-    <mergeCell ref="A138:A152"/>
-    <mergeCell ref="A104:A118"/>
-    <mergeCell ref="A70:A84"/>
-    <mergeCell ref="A121:A135"/>
-    <mergeCell ref="A87:A101"/>
-    <mergeCell ref="A53:A67"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11818,16 +11917,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="161" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="162" t="s">
+      <c r="B1" s="162"/>
+      <c r="C1" s="163" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="164"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -11905,10 +12004,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="158" t="s">
+      <c r="C5" s="159" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="158"/>
+      <c r="D5" s="159"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -11924,10 +12023,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="158" t="s">
+      <c r="C6" s="159" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="159"/>
+      <c r="D6" s="160"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -11945,7 +12044,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="164" t="s">
+      <c r="A8" s="165" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -12084,7 +12183,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="165" t="s">
+      <c r="A19" s="156" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -12288,7 +12387,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="156" t="s">
+      <c r="A36" s="158" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -12492,7 +12591,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="165" t="s">
+      <c r="A53" s="156" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -12696,7 +12795,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="156" t="s">
+      <c r="A70" s="158" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -12900,7 +12999,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="165" t="s">
+      <c r="A87" s="156" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -13103,7 +13202,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="156" t="s">
+      <c r="A104" s="158" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -13306,7 +13405,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="165" t="s">
+      <c r="A121" s="156" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -13509,7 +13608,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="156" t="s">
+      <c r="A138" s="158" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -13713,12 +13812,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="A138:A152"/>
-    <mergeCell ref="A104:A118"/>
-    <mergeCell ref="A70:A84"/>
-    <mergeCell ref="A121:A135"/>
-    <mergeCell ref="A87:A101"/>
     <mergeCell ref="A36:A50"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
@@ -13726,6 +13819,12 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="A138:A152"/>
+    <mergeCell ref="A104:A118"/>
+    <mergeCell ref="A70:A84"/>
+    <mergeCell ref="A121:A135"/>
+    <mergeCell ref="A87:A101"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13759,16 +13858,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="161" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="162" t="s">
+      <c r="B1" s="162"/>
+      <c r="C1" s="163" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="164"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -13846,10 +13945,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="158" t="s">
+      <c r="C5" s="159" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="158"/>
+      <c r="D5" s="159"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -13865,10 +13964,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="158" t="s">
+      <c r="C6" s="159" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="159"/>
+      <c r="D6" s="160"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -13886,7 +13985,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="164" t="s">
+      <c r="A8" s="165" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -14025,7 +14124,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="165" t="s">
+      <c r="A19" s="156" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -14229,7 +14328,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="156" t="s">
+      <c r="A36" s="158" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -14433,7 +14532,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="165" t="s">
+      <c r="A53" s="156" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -14637,7 +14736,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="156" t="s">
+      <c r="A70" s="158" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -14841,7 +14940,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="165" t="s">
+      <c r="A87" s="156" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -15044,7 +15143,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="156" t="s">
+      <c r="A104" s="158" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -15247,7 +15346,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="165" t="s">
+      <c r="A121" s="156" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -15450,7 +15549,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="156" t="s">
+      <c r="A138" s="158" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -15654,6 +15753,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="A138:A152"/>
+    <mergeCell ref="A104:A118"/>
+    <mergeCell ref="A70:A84"/>
+    <mergeCell ref="A121:A135"/>
+    <mergeCell ref="A87:A101"/>
     <mergeCell ref="A36:A50"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
@@ -15661,12 +15766,6 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
-    <mergeCell ref="A138:A152"/>
-    <mergeCell ref="A104:A118"/>
-    <mergeCell ref="A70:A84"/>
-    <mergeCell ref="A121:A135"/>
-    <mergeCell ref="A87:A101"/>
-    <mergeCell ref="A53:A67"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15700,16 +15799,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="161" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="162" t="s">
+      <c r="B1" s="162"/>
+      <c r="C1" s="163" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="164"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -15787,10 +15886,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="158" t="s">
+      <c r="C5" s="159" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="158"/>
+      <c r="D5" s="159"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -15806,10 +15905,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="158" t="s">
+      <c r="C6" s="159" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="159"/>
+      <c r="D6" s="160"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -15827,7 +15926,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="164" t="s">
+      <c r="A8" s="165" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -15966,7 +16065,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="165" t="s">
+      <c r="A19" s="156" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -16170,7 +16269,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="156" t="s">
+      <c r="A36" s="158" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -16374,7 +16473,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="165" t="s">
+      <c r="A53" s="156" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -16578,7 +16677,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="156" t="s">
+      <c r="A70" s="158" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -16782,7 +16881,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="165" t="s">
+      <c r="A87" s="156" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -16985,7 +17084,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="156" t="s">
+      <c r="A104" s="158" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -17188,7 +17287,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="165" t="s">
+      <c r="A121" s="156" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -17391,7 +17490,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="156" t="s">
+      <c r="A138" s="158" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -17595,12 +17694,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="A138:A152"/>
-    <mergeCell ref="A104:A118"/>
-    <mergeCell ref="A70:A84"/>
-    <mergeCell ref="A121:A135"/>
-    <mergeCell ref="A87:A101"/>
     <mergeCell ref="A36:A50"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
@@ -17608,6 +17701,12 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="A138:A152"/>
+    <mergeCell ref="A104:A118"/>
+    <mergeCell ref="A70:A84"/>
+    <mergeCell ref="A121:A135"/>
+    <mergeCell ref="A87:A101"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17641,16 +17740,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="161" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="162" t="s">
+      <c r="B1" s="162"/>
+      <c r="C1" s="163" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="164"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -17728,10 +17827,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="158" t="s">
+      <c r="C5" s="159" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="158"/>
+      <c r="D5" s="159"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -17747,10 +17846,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="158" t="s">
+      <c r="C6" s="159" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="159"/>
+      <c r="D6" s="160"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -17768,7 +17867,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="164" t="s">
+      <c r="A8" s="165" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -17907,7 +18006,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="165" t="s">
+      <c r="A19" s="156" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -18111,7 +18210,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="156" t="s">
+      <c r="A36" s="158" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -18315,7 +18414,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="165" t="s">
+      <c r="A53" s="156" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -18519,7 +18618,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="156" t="s">
+      <c r="A70" s="158" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -18723,7 +18822,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="165" t="s">
+      <c r="A87" s="156" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -18926,7 +19025,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="156" t="s">
+      <c r="A104" s="158" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -19129,7 +19228,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="165" t="s">
+      <c r="A121" s="156" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -19332,7 +19431,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="156" t="s">
+      <c r="A138" s="158" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -19536,6 +19635,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="A138:A152"/>
+    <mergeCell ref="A104:A118"/>
+    <mergeCell ref="A70:A84"/>
+    <mergeCell ref="A121:A135"/>
+    <mergeCell ref="A87:A101"/>
     <mergeCell ref="A36:A50"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
@@ -19543,12 +19648,6 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
-    <mergeCell ref="A138:A152"/>
-    <mergeCell ref="A104:A118"/>
-    <mergeCell ref="A70:A84"/>
-    <mergeCell ref="A121:A135"/>
-    <mergeCell ref="A87:A101"/>
-    <mergeCell ref="A53:A67"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19582,13 +19681,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="168" t="s">
+      <c r="A1" s="184" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="168"/>
-      <c r="C1" s="168"/>
-      <c r="D1" s="168"/>
-      <c r="E1" s="168"/>
+      <c r="B1" s="184"/>
+      <c r="C1" s="184"/>
+      <c r="D1" s="184"/>
+      <c r="E1" s="184"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -19618,18 +19717,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="169"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="170"/>
+      <c r="C3" s="185"/>
+      <c r="D3" s="186"/>
+      <c r="E3" s="186"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="166"/>
-      <c r="D4" s="167"/>
-      <c r="E4" s="167"/>
+      <c r="C4" s="168"/>
+      <c r="D4" s="169"/>
+      <c r="E4" s="169"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -19781,9 +19880,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="171"/>
-      <c r="D21" s="172"/>
-      <c r="E21" s="172"/>
+      <c r="C21" s="166"/>
+      <c r="D21" s="167"/>
+      <c r="E21" s="167"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -19934,9 +20033,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="166"/>
-      <c r="D38" s="167"/>
-      <c r="E38" s="167"/>
+      <c r="C38" s="168"/>
+      <c r="D38" s="169"/>
+      <c r="E38" s="169"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -20087,9 +20186,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="166"/>
-      <c r="D55" s="167"/>
-      <c r="E55" s="167"/>
+      <c r="C55" s="168"/>
+      <c r="D55" s="169"/>
+      <c r="E55" s="169"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -20240,9 +20339,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="166"/>
-      <c r="D72" s="167"/>
-      <c r="E72" s="167"/>
+      <c r="C72" s="168"/>
+      <c r="D72" s="169"/>
+      <c r="E72" s="169"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -20393,9 +20492,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="166"/>
-      <c r="D89" s="167"/>
-      <c r="E89" s="167"/>
+      <c r="C89" s="168"/>
+      <c r="D89" s="169"/>
+      <c r="E89" s="169"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -20546,9 +20645,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="166"/>
-      <c r="D106" s="167"/>
-      <c r="E106" s="167"/>
+      <c r="C106" s="168"/>
+      <c r="D106" s="169"/>
+      <c r="E106" s="169"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -20699,9 +20798,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="166"/>
-      <c r="D123" s="167"/>
-      <c r="E123" s="167"/>
+      <c r="C123" s="168"/>
+      <c r="D123" s="169"/>
+      <c r="E123" s="169"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -20852,9 +20951,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="166"/>
-      <c r="D140" s="167"/>
-      <c r="E140" s="167"/>
+      <c r="C140" s="168"/>
+      <c r="D140" s="169"/>
+      <c r="E140" s="169"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -21005,9 +21104,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="166"/>
-      <c r="D157" s="167"/>
-      <c r="E157" s="167"/>
+      <c r="C157" s="168"/>
+      <c r="D157" s="169"/>
+      <c r="E157" s="169"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -21158,9 +21257,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="166"/>
-      <c r="D174" s="167"/>
-      <c r="E174" s="167"/>
+      <c r="C174" s="168"/>
+      <c r="D174" s="169"/>
+      <c r="E174" s="169"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -21311,9 +21410,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="166"/>
-      <c r="D191" s="167"/>
-      <c r="E191" s="167"/>
+      <c r="C191" s="168"/>
+      <c r="D191" s="169"/>
+      <c r="E191" s="169"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -21464,9 +21563,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="166"/>
-      <c r="D208" s="167"/>
-      <c r="E208" s="167"/>
+      <c r="C208" s="168"/>
+      <c r="D208" s="169"/>
+      <c r="E208" s="169"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -21617,9 +21716,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="166"/>
-      <c r="D225" s="167"/>
-      <c r="E225" s="167"/>
+      <c r="C225" s="168"/>
+      <c r="D225" s="169"/>
+      <c r="E225" s="169"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -21770,9 +21869,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="166"/>
-      <c r="D242" s="167"/>
-      <c r="E242" s="167"/>
+      <c r="C242" s="168"/>
+      <c r="D242" s="169"/>
+      <c r="E242" s="169"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -21923,9 +22022,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="166"/>
-      <c r="D259" s="167"/>
-      <c r="E259" s="167"/>
+      <c r="C259" s="168"/>
+      <c r="D259" s="169"/>
+      <c r="E259" s="169"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -22076,18 +22175,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="173"/>
-      <c r="D276" s="174"/>
-      <c r="E276" s="174"/>
+      <c r="C276" s="182"/>
+      <c r="D276" s="183"/>
+      <c r="E276" s="183"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="166"/>
-      <c r="D277" s="167"/>
-      <c r="E277" s="167"/>
+      <c r="C277" s="168"/>
+      <c r="D277" s="169"/>
+      <c r="E277" s="169"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -22238,9 +22337,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="171"/>
-      <c r="D294" s="172"/>
-      <c r="E294" s="172"/>
+      <c r="C294" s="166"/>
+      <c r="D294" s="167"/>
+      <c r="E294" s="167"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -22391,9 +22490,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="166"/>
-      <c r="D311" s="167"/>
-      <c r="E311" s="167"/>
+      <c r="C311" s="168"/>
+      <c r="D311" s="169"/>
+      <c r="E311" s="169"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -22544,9 +22643,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="166"/>
-      <c r="D328" s="167"/>
-      <c r="E328" s="167"/>
+      <c r="C328" s="168"/>
+      <c r="D328" s="169"/>
+      <c r="E328" s="169"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -22697,9 +22796,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="166"/>
-      <c r="D345" s="167"/>
-      <c r="E345" s="167"/>
+      <c r="C345" s="168"/>
+      <c r="D345" s="169"/>
+      <c r="E345" s="169"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -22850,9 +22949,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="166"/>
-      <c r="D362" s="167"/>
-      <c r="E362" s="167"/>
+      <c r="C362" s="168"/>
+      <c r="D362" s="169"/>
+      <c r="E362" s="169"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -23003,9 +23102,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="166"/>
-      <c r="D379" s="167"/>
-      <c r="E379" s="167"/>
+      <c r="C379" s="168"/>
+      <c r="D379" s="169"/>
+      <c r="E379" s="169"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -23156,9 +23255,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="166"/>
-      <c r="D396" s="167"/>
-      <c r="E396" s="167"/>
+      <c r="C396" s="168"/>
+      <c r="D396" s="169"/>
+      <c r="E396" s="169"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -23309,9 +23408,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="166"/>
-      <c r="D413" s="167"/>
-      <c r="E413" s="167"/>
+      <c r="C413" s="168"/>
+      <c r="D413" s="169"/>
+      <c r="E413" s="169"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -23462,9 +23561,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="166"/>
-      <c r="D430" s="167"/>
-      <c r="E430" s="167"/>
+      <c r="C430" s="168"/>
+      <c r="D430" s="169"/>
+      <c r="E430" s="169"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -23615,9 +23714,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="166"/>
-      <c r="D447" s="167"/>
-      <c r="E447" s="167"/>
+      <c r="C447" s="168"/>
+      <c r="D447" s="169"/>
+      <c r="E447" s="169"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -23768,9 +23867,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="166"/>
-      <c r="D464" s="167"/>
-      <c r="E464" s="167"/>
+      <c r="C464" s="168"/>
+      <c r="D464" s="169"/>
+      <c r="E464" s="169"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -23921,9 +24020,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="166"/>
-      <c r="D481" s="167"/>
-      <c r="E481" s="167"/>
+      <c r="C481" s="168"/>
+      <c r="D481" s="169"/>
+      <c r="E481" s="169"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -24074,9 +24173,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="166"/>
-      <c r="D498" s="167"/>
-      <c r="E498" s="167"/>
+      <c r="C498" s="168"/>
+      <c r="D498" s="169"/>
+      <c r="E498" s="169"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -24227,9 +24326,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="166"/>
-      <c r="D515" s="167"/>
-      <c r="E515" s="167"/>
+      <c r="C515" s="168"/>
+      <c r="D515" s="169"/>
+      <c r="E515" s="169"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -24380,9 +24479,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="166"/>
-      <c r="D532" s="167"/>
-      <c r="E532" s="167"/>
+      <c r="C532" s="168"/>
+      <c r="D532" s="169"/>
+      <c r="E532" s="169"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -24533,18 +24632,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="175"/>
-      <c r="D549" s="176"/>
-      <c r="E549" s="176"/>
+      <c r="C549" s="180"/>
+      <c r="D549" s="181"/>
+      <c r="E549" s="181"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="166"/>
-      <c r="D550" s="167"/>
-      <c r="E550" s="167"/>
+      <c r="C550" s="168"/>
+      <c r="D550" s="169"/>
+      <c r="E550" s="169"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -24695,9 +24794,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="171"/>
-      <c r="D567" s="172"/>
-      <c r="E567" s="172"/>
+      <c r="C567" s="166"/>
+      <c r="D567" s="167"/>
+      <c r="E567" s="167"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -24848,9 +24947,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="166"/>
-      <c r="D584" s="167"/>
-      <c r="E584" s="167"/>
+      <c r="C584" s="168"/>
+      <c r="D584" s="169"/>
+      <c r="E584" s="169"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -25001,9 +25100,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="166"/>
-      <c r="D601" s="167"/>
-      <c r="E601" s="167"/>
+      <c r="C601" s="168"/>
+      <c r="D601" s="169"/>
+      <c r="E601" s="169"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -25154,9 +25253,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="166"/>
-      <c r="D618" s="167"/>
-      <c r="E618" s="167"/>
+      <c r="C618" s="168"/>
+      <c r="D618" s="169"/>
+      <c r="E618" s="169"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -25307,9 +25406,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="166"/>
-      <c r="D635" s="167"/>
-      <c r="E635" s="167"/>
+      <c r="C635" s="168"/>
+      <c r="D635" s="169"/>
+      <c r="E635" s="169"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -25460,9 +25559,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="166"/>
-      <c r="D652" s="167"/>
-      <c r="E652" s="167"/>
+      <c r="C652" s="168"/>
+      <c r="D652" s="169"/>
+      <c r="E652" s="169"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -25613,9 +25712,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="166"/>
-      <c r="D669" s="167"/>
-      <c r="E669" s="167"/>
+      <c r="C669" s="168"/>
+      <c r="D669" s="169"/>
+      <c r="E669" s="169"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -25766,9 +25865,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="166"/>
-      <c r="D686" s="167"/>
-      <c r="E686" s="167"/>
+      <c r="C686" s="168"/>
+      <c r="D686" s="169"/>
+      <c r="E686" s="169"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -25919,9 +26018,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="166"/>
-      <c r="D703" s="167"/>
-      <c r="E703" s="167"/>
+      <c r="C703" s="168"/>
+      <c r="D703" s="169"/>
+      <c r="E703" s="169"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -26072,9 +26171,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="166"/>
-      <c r="D720" s="167"/>
-      <c r="E720" s="167"/>
+      <c r="C720" s="168"/>
+      <c r="D720" s="169"/>
+      <c r="E720" s="169"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -26225,9 +26324,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="166"/>
-      <c r="D737" s="167"/>
-      <c r="E737" s="167"/>
+      <c r="C737" s="168"/>
+      <c r="D737" s="169"/>
+      <c r="E737" s="169"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -26378,9 +26477,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="166"/>
-      <c r="D754" s="167"/>
-      <c r="E754" s="167"/>
+      <c r="C754" s="168"/>
+      <c r="D754" s="169"/>
+      <c r="E754" s="169"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -26531,9 +26630,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="166"/>
-      <c r="D771" s="167"/>
-      <c r="E771" s="167"/>
+      <c r="C771" s="168"/>
+      <c r="D771" s="169"/>
+      <c r="E771" s="169"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -26684,9 +26783,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="166"/>
-      <c r="D788" s="167"/>
-      <c r="E788" s="167"/>
+      <c r="C788" s="168"/>
+      <c r="D788" s="169"/>
+      <c r="E788" s="169"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -26837,9 +26936,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="166"/>
-      <c r="D805" s="167"/>
-      <c r="E805" s="167"/>
+      <c r="C805" s="168"/>
+      <c r="D805" s="169"/>
+      <c r="E805" s="169"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -26990,18 +27089,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="177"/>
-      <c r="D822" s="178"/>
-      <c r="E822" s="178"/>
+      <c r="C822" s="178"/>
+      <c r="D822" s="179"/>
+      <c r="E822" s="179"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="166"/>
-      <c r="D823" s="167"/>
-      <c r="E823" s="167"/>
+      <c r="C823" s="168"/>
+      <c r="D823" s="169"/>
+      <c r="E823" s="169"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -27152,9 +27251,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="171"/>
-      <c r="D840" s="172"/>
-      <c r="E840" s="172"/>
+      <c r="C840" s="166"/>
+      <c r="D840" s="167"/>
+      <c r="E840" s="167"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -27305,9 +27404,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="166"/>
-      <c r="D857" s="167"/>
-      <c r="E857" s="167"/>
+      <c r="C857" s="168"/>
+      <c r="D857" s="169"/>
+      <c r="E857" s="169"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -27458,9 +27557,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="166"/>
-      <c r="D874" s="167"/>
-      <c r="E874" s="167"/>
+      <c r="C874" s="168"/>
+      <c r="D874" s="169"/>
+      <c r="E874" s="169"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -27611,9 +27710,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="166"/>
-      <c r="D891" s="167"/>
-      <c r="E891" s="167"/>
+      <c r="C891" s="168"/>
+      <c r="D891" s="169"/>
+      <c r="E891" s="169"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -27764,9 +27863,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="166"/>
-      <c r="D908" s="167"/>
-      <c r="E908" s="167"/>
+      <c r="C908" s="168"/>
+      <c r="D908" s="169"/>
+      <c r="E908" s="169"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -27917,9 +28016,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="166"/>
-      <c r="D925" s="167"/>
-      <c r="E925" s="167"/>
+      <c r="C925" s="168"/>
+      <c r="D925" s="169"/>
+      <c r="E925" s="169"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -28070,9 +28169,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="166"/>
-      <c r="D942" s="167"/>
-      <c r="E942" s="167"/>
+      <c r="C942" s="168"/>
+      <c r="D942" s="169"/>
+      <c r="E942" s="169"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -28223,9 +28322,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="166"/>
-      <c r="D959" s="167"/>
-      <c r="E959" s="167"/>
+      <c r="C959" s="168"/>
+      <c r="D959" s="169"/>
+      <c r="E959" s="169"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -28376,9 +28475,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="166"/>
-      <c r="D976" s="167"/>
-      <c r="E976" s="167"/>
+      <c r="C976" s="168"/>
+      <c r="D976" s="169"/>
+      <c r="E976" s="169"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -28529,9 +28628,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="166"/>
-      <c r="D993" s="167"/>
-      <c r="E993" s="167"/>
+      <c r="C993" s="168"/>
+      <c r="D993" s="169"/>
+      <c r="E993" s="169"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -28682,9 +28781,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="166"/>
-      <c r="D1010" s="167"/>
-      <c r="E1010" s="167"/>
+      <c r="C1010" s="168"/>
+      <c r="D1010" s="169"/>
+      <c r="E1010" s="169"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -28835,9 +28934,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="166"/>
-      <c r="D1027" s="167"/>
-      <c r="E1027" s="167"/>
+      <c r="C1027" s="168"/>
+      <c r="D1027" s="169"/>
+      <c r="E1027" s="169"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -28988,9 +29087,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="166"/>
-      <c r="D1044" s="167"/>
-      <c r="E1044" s="167"/>
+      <c r="C1044" s="168"/>
+      <c r="D1044" s="169"/>
+      <c r="E1044" s="169"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -29141,9 +29240,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="166"/>
-      <c r="D1061" s="167"/>
-      <c r="E1061" s="167"/>
+      <c r="C1061" s="168"/>
+      <c r="D1061" s="169"/>
+      <c r="E1061" s="169"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -29294,9 +29393,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="166"/>
-      <c r="D1078" s="167"/>
-      <c r="E1078" s="167"/>
+      <c r="C1078" s="168"/>
+      <c r="D1078" s="169"/>
+      <c r="E1078" s="169"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -29447,18 +29546,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="179"/>
-      <c r="D1095" s="180"/>
-      <c r="E1095" s="180"/>
+      <c r="C1095" s="176"/>
+      <c r="D1095" s="177"/>
+      <c r="E1095" s="177"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="166"/>
-      <c r="D1096" s="167"/>
-      <c r="E1096" s="167"/>
+      <c r="C1096" s="168"/>
+      <c r="D1096" s="169"/>
+      <c r="E1096" s="169"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -29609,9 +29708,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="171"/>
-      <c r="D1113" s="172"/>
-      <c r="E1113" s="172"/>
+      <c r="C1113" s="166"/>
+      <c r="D1113" s="167"/>
+      <c r="E1113" s="167"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -29762,9 +29861,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="166"/>
-      <c r="D1130" s="167"/>
-      <c r="E1130" s="167"/>
+      <c r="C1130" s="168"/>
+      <c r="D1130" s="169"/>
+      <c r="E1130" s="169"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -29915,9 +30014,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="166"/>
-      <c r="D1147" s="167"/>
-      <c r="E1147" s="167"/>
+      <c r="C1147" s="168"/>
+      <c r="D1147" s="169"/>
+      <c r="E1147" s="169"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -30068,9 +30167,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="166"/>
-      <c r="D1164" s="167"/>
-      <c r="E1164" s="167"/>
+      <c r="C1164" s="168"/>
+      <c r="D1164" s="169"/>
+      <c r="E1164" s="169"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -30221,9 +30320,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="166"/>
-      <c r="D1181" s="167"/>
-      <c r="E1181" s="167"/>
+      <c r="C1181" s="168"/>
+      <c r="D1181" s="169"/>
+      <c r="E1181" s="169"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -30374,9 +30473,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="166"/>
-      <c r="D1198" s="167"/>
-      <c r="E1198" s="167"/>
+      <c r="C1198" s="168"/>
+      <c r="D1198" s="169"/>
+      <c r="E1198" s="169"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -30527,9 +30626,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="166"/>
-      <c r="D1215" s="167"/>
-      <c r="E1215" s="167"/>
+      <c r="C1215" s="168"/>
+      <c r="D1215" s="169"/>
+      <c r="E1215" s="169"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -30680,9 +30779,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="166"/>
-      <c r="D1232" s="167"/>
-      <c r="E1232" s="167"/>
+      <c r="C1232" s="168"/>
+      <c r="D1232" s="169"/>
+      <c r="E1232" s="169"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -30833,9 +30932,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="166"/>
-      <c r="D1249" s="167"/>
-      <c r="E1249" s="167"/>
+      <c r="C1249" s="168"/>
+      <c r="D1249" s="169"/>
+      <c r="E1249" s="169"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -30986,9 +31085,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="166"/>
-      <c r="D1266" s="167"/>
-      <c r="E1266" s="167"/>
+      <c r="C1266" s="168"/>
+      <c r="D1266" s="169"/>
+      <c r="E1266" s="169"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -31139,9 +31238,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="166"/>
-      <c r="D1283" s="167"/>
-      <c r="E1283" s="167"/>
+      <c r="C1283" s="168"/>
+      <c r="D1283" s="169"/>
+      <c r="E1283" s="169"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -31292,9 +31391,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="166"/>
-      <c r="D1300" s="167"/>
-      <c r="E1300" s="167"/>
+      <c r="C1300" s="168"/>
+      <c r="D1300" s="169"/>
+      <c r="E1300" s="169"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -31445,9 +31544,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="166"/>
-      <c r="D1317" s="167"/>
-      <c r="E1317" s="167"/>
+      <c r="C1317" s="168"/>
+      <c r="D1317" s="169"/>
+      <c r="E1317" s="169"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -31598,9 +31697,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="166"/>
-      <c r="D1334" s="167"/>
-      <c r="E1334" s="167"/>
+      <c r="C1334" s="168"/>
+      <c r="D1334" s="169"/>
+      <c r="E1334" s="169"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -31751,9 +31850,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="166"/>
-      <c r="D1351" s="167"/>
-      <c r="E1351" s="167"/>
+      <c r="C1351" s="168"/>
+      <c r="D1351" s="169"/>
+      <c r="E1351" s="169"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -31904,18 +32003,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="181"/>
-      <c r="D1368" s="182"/>
-      <c r="E1368" s="182"/>
+      <c r="C1368" s="174"/>
+      <c r="D1368" s="175"/>
+      <c r="E1368" s="175"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="166"/>
-      <c r="D1369" s="167"/>
-      <c r="E1369" s="167"/>
+      <c r="C1369" s="168"/>
+      <c r="D1369" s="169"/>
+      <c r="E1369" s="169"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -32066,9 +32165,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="171"/>
-      <c r="D1386" s="172"/>
-      <c r="E1386" s="172"/>
+      <c r="C1386" s="166"/>
+      <c r="D1386" s="167"/>
+      <c r="E1386" s="167"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -32219,9 +32318,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="166"/>
-      <c r="D1403" s="167"/>
-      <c r="E1403" s="167"/>
+      <c r="C1403" s="168"/>
+      <c r="D1403" s="169"/>
+      <c r="E1403" s="169"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -32372,9 +32471,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="166"/>
-      <c r="D1420" s="167"/>
-      <c r="E1420" s="167"/>
+      <c r="C1420" s="168"/>
+      <c r="D1420" s="169"/>
+      <c r="E1420" s="169"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -32525,9 +32624,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="166"/>
-      <c r="D1437" s="167"/>
-      <c r="E1437" s="167"/>
+      <c r="C1437" s="168"/>
+      <c r="D1437" s="169"/>
+      <c r="E1437" s="169"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -32678,9 +32777,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="166"/>
-      <c r="D1454" s="167"/>
-      <c r="E1454" s="167"/>
+      <c r="C1454" s="168"/>
+      <c r="D1454" s="169"/>
+      <c r="E1454" s="169"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -32831,9 +32930,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="166"/>
-      <c r="D1471" s="167"/>
-      <c r="E1471" s="167"/>
+      <c r="C1471" s="168"/>
+      <c r="D1471" s="169"/>
+      <c r="E1471" s="169"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -32984,9 +33083,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="166"/>
-      <c r="D1488" s="167"/>
-      <c r="E1488" s="167"/>
+      <c r="C1488" s="168"/>
+      <c r="D1488" s="169"/>
+      <c r="E1488" s="169"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -33137,9 +33236,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="166"/>
-      <c r="D1505" s="167"/>
-      <c r="E1505" s="167"/>
+      <c r="C1505" s="168"/>
+      <c r="D1505" s="169"/>
+      <c r="E1505" s="169"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -33290,9 +33389,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="166"/>
-      <c r="D1522" s="167"/>
-      <c r="E1522" s="167"/>
+      <c r="C1522" s="168"/>
+      <c r="D1522" s="169"/>
+      <c r="E1522" s="169"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -33443,9 +33542,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="166"/>
-      <c r="D1539" s="167"/>
-      <c r="E1539" s="167"/>
+      <c r="C1539" s="168"/>
+      <c r="D1539" s="169"/>
+      <c r="E1539" s="169"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -33596,9 +33695,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="166"/>
-      <c r="D1556" s="167"/>
-      <c r="E1556" s="167"/>
+      <c r="C1556" s="168"/>
+      <c r="D1556" s="169"/>
+      <c r="E1556" s="169"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -33749,9 +33848,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="166"/>
-      <c r="D1573" s="167"/>
-      <c r="E1573" s="167"/>
+      <c r="C1573" s="168"/>
+      <c r="D1573" s="169"/>
+      <c r="E1573" s="169"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -33902,9 +34001,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="166"/>
-      <c r="D1590" s="167"/>
-      <c r="E1590" s="167"/>
+      <c r="C1590" s="168"/>
+      <c r="D1590" s="169"/>
+      <c r="E1590" s="169"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -34055,9 +34154,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="166"/>
-      <c r="D1607" s="167"/>
-      <c r="E1607" s="167"/>
+      <c r="C1607" s="168"/>
+      <c r="D1607" s="169"/>
+      <c r="E1607" s="169"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -34208,9 +34307,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="166"/>
-      <c r="D1624" s="167"/>
-      <c r="E1624" s="167"/>
+      <c r="C1624" s="168"/>
+      <c r="D1624" s="169"/>
+      <c r="E1624" s="169"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -34361,18 +34460,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="183"/>
-      <c r="D1641" s="184"/>
-      <c r="E1641" s="184"/>
+      <c r="C1641" s="172"/>
+      <c r="D1641" s="173"/>
+      <c r="E1641" s="173"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="166"/>
-      <c r="D1642" s="167"/>
-      <c r="E1642" s="167"/>
+      <c r="C1642" s="168"/>
+      <c r="D1642" s="169"/>
+      <c r="E1642" s="169"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -34523,9 +34622,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="171"/>
-      <c r="D1659" s="172"/>
-      <c r="E1659" s="172"/>
+      <c r="C1659" s="166"/>
+      <c r="D1659" s="167"/>
+      <c r="E1659" s="167"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -34676,9 +34775,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="166"/>
-      <c r="D1676" s="167"/>
-      <c r="E1676" s="167"/>
+      <c r="C1676" s="168"/>
+      <c r="D1676" s="169"/>
+      <c r="E1676" s="169"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -34829,9 +34928,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="166"/>
-      <c r="D1693" s="167"/>
-      <c r="E1693" s="167"/>
+      <c r="C1693" s="168"/>
+      <c r="D1693" s="169"/>
+      <c r="E1693" s="169"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -34982,9 +35081,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="166"/>
-      <c r="D1710" s="167"/>
-      <c r="E1710" s="167"/>
+      <c r="C1710" s="168"/>
+      <c r="D1710" s="169"/>
+      <c r="E1710" s="169"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -35135,9 +35234,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="166"/>
-      <c r="D1727" s="167"/>
-      <c r="E1727" s="167"/>
+      <c r="C1727" s="168"/>
+      <c r="D1727" s="169"/>
+      <c r="E1727" s="169"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -35288,9 +35387,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="166"/>
-      <c r="D1744" s="167"/>
-      <c r="E1744" s="167"/>
+      <c r="C1744" s="168"/>
+      <c r="D1744" s="169"/>
+      <c r="E1744" s="169"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -35441,9 +35540,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="166"/>
-      <c r="D1761" s="167"/>
-      <c r="E1761" s="167"/>
+      <c r="C1761" s="168"/>
+      <c r="D1761" s="169"/>
+      <c r="E1761" s="169"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -35594,9 +35693,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="166"/>
-      <c r="D1778" s="167"/>
-      <c r="E1778" s="167"/>
+      <c r="C1778" s="168"/>
+      <c r="D1778" s="169"/>
+      <c r="E1778" s="169"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -35747,9 +35846,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="166"/>
-      <c r="D1795" s="167"/>
-      <c r="E1795" s="167"/>
+      <c r="C1795" s="168"/>
+      <c r="D1795" s="169"/>
+      <c r="E1795" s="169"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -35900,9 +35999,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="166"/>
-      <c r="D1812" s="167"/>
-      <c r="E1812" s="167"/>
+      <c r="C1812" s="168"/>
+      <c r="D1812" s="169"/>
+      <c r="E1812" s="169"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -36053,9 +36152,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="166"/>
-      <c r="D1829" s="167"/>
-      <c r="E1829" s="167"/>
+      <c r="C1829" s="168"/>
+      <c r="D1829" s="169"/>
+      <c r="E1829" s="169"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -36206,9 +36305,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="166"/>
-      <c r="D1846" s="167"/>
-      <c r="E1846" s="167"/>
+      <c r="C1846" s="168"/>
+      <c r="D1846" s="169"/>
+      <c r="E1846" s="169"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -36359,9 +36458,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="166"/>
-      <c r="D1863" s="167"/>
-      <c r="E1863" s="167"/>
+      <c r="C1863" s="168"/>
+      <c r="D1863" s="169"/>
+      <c r="E1863" s="169"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -36512,9 +36611,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="166"/>
-      <c r="D1880" s="167"/>
-      <c r="E1880" s="167"/>
+      <c r="C1880" s="168"/>
+      <c r="D1880" s="169"/>
+      <c r="E1880" s="169"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -36665,9 +36764,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="166"/>
-      <c r="D1897" s="167"/>
-      <c r="E1897" s="167"/>
+      <c r="C1897" s="168"/>
+      <c r="D1897" s="169"/>
+      <c r="E1897" s="169"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -36818,18 +36917,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="185"/>
-      <c r="D1914" s="186"/>
-      <c r="E1914" s="186"/>
+      <c r="C1914" s="170"/>
+      <c r="D1914" s="171"/>
+      <c r="E1914" s="171"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="166"/>
-      <c r="D1915" s="167"/>
-      <c r="E1915" s="167"/>
+      <c r="C1915" s="168"/>
+      <c r="D1915" s="169"/>
+      <c r="E1915" s="169"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -36980,9 +37079,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="171"/>
-      <c r="D1932" s="172"/>
-      <c r="E1932" s="172"/>
+      <c r="C1932" s="166"/>
+      <c r="D1932" s="167"/>
+      <c r="E1932" s="167"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -37133,9 +37232,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="166"/>
-      <c r="D1949" s="167"/>
-      <c r="E1949" s="167"/>
+      <c r="C1949" s="168"/>
+      <c r="D1949" s="169"/>
+      <c r="E1949" s="169"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -37286,9 +37385,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="166"/>
-      <c r="D1966" s="167"/>
-      <c r="E1966" s="167"/>
+      <c r="C1966" s="168"/>
+      <c r="D1966" s="169"/>
+      <c r="E1966" s="169"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -37439,9 +37538,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="166"/>
-      <c r="D1983" s="167"/>
-      <c r="E1983" s="167"/>
+      <c r="C1983" s="168"/>
+      <c r="D1983" s="169"/>
+      <c r="E1983" s="169"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -37592,9 +37691,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="166"/>
-      <c r="D2000" s="167"/>
-      <c r="E2000" s="167"/>
+      <c r="C2000" s="168"/>
+      <c r="D2000" s="169"/>
+      <c r="E2000" s="169"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -37745,9 +37844,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="166"/>
-      <c r="D2017" s="167"/>
-      <c r="E2017" s="167"/>
+      <c r="C2017" s="168"/>
+      <c r="D2017" s="169"/>
+      <c r="E2017" s="169"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -37898,9 +37997,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="166"/>
-      <c r="D2034" s="167"/>
-      <c r="E2034" s="167"/>
+      <c r="C2034" s="168"/>
+      <c r="D2034" s="169"/>
+      <c r="E2034" s="169"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -38051,9 +38150,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="166"/>
-      <c r="D2051" s="167"/>
-      <c r="E2051" s="167"/>
+      <c r="C2051" s="168"/>
+      <c r="D2051" s="169"/>
+      <c r="E2051" s="169"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -38204,9 +38303,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="166"/>
-      <c r="D2068" s="167"/>
-      <c r="E2068" s="167"/>
+      <c r="C2068" s="168"/>
+      <c r="D2068" s="169"/>
+      <c r="E2068" s="169"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -38357,9 +38456,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="166"/>
-      <c r="D2085" s="167"/>
-      <c r="E2085" s="167"/>
+      <c r="C2085" s="168"/>
+      <c r="D2085" s="169"/>
+      <c r="E2085" s="169"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -38510,9 +38609,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="166"/>
-      <c r="D2102" s="167"/>
-      <c r="E2102" s="167"/>
+      <c r="C2102" s="168"/>
+      <c r="D2102" s="169"/>
+      <c r="E2102" s="169"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -38663,9 +38762,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="166"/>
-      <c r="D2119" s="167"/>
-      <c r="E2119" s="167"/>
+      <c r="C2119" s="168"/>
+      <c r="D2119" s="169"/>
+      <c r="E2119" s="169"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -38816,9 +38915,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="166"/>
-      <c r="D2136" s="167"/>
-      <c r="E2136" s="167"/>
+      <c r="C2136" s="168"/>
+      <c r="D2136" s="169"/>
+      <c r="E2136" s="169"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -38969,9 +39068,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="166"/>
-      <c r="D2153" s="167"/>
-      <c r="E2153" s="167"/>
+      <c r="C2153" s="168"/>
+      <c r="D2153" s="169"/>
+      <c r="E2153" s="169"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -39122,9 +39221,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="166"/>
-      <c r="D2170" s="167"/>
-      <c r="E2170" s="167"/>
+      <c r="C2170" s="168"/>
+      <c r="D2170" s="169"/>
+      <c r="E2170" s="169"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -39272,36 +39371,96 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="C1880:E1880"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C1983:E1983"/>
-    <mergeCell ref="C1932:E1932"/>
-    <mergeCell ref="C1949:E1949"/>
-    <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C1966:E1966"/>
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2000:E2000"/>
-    <mergeCell ref="C2017:E2017"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1897:E1897"/>
-    <mergeCell ref="C1914:E1914"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1846:E1846"/>
-    <mergeCell ref="C1863:E1863"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C362:E362"/>
+    <mergeCell ref="C379:E379"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C294:E294"/>
+    <mergeCell ref="C311:E311"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C396:E396"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C328:E328"/>
+    <mergeCell ref="C345:E345"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C567:E567"/>
+    <mergeCell ref="C464:E464"/>
+    <mergeCell ref="C481:E481"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C430:E430"/>
+    <mergeCell ref="C447:E447"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C413:E413"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1317:E1317"/>
     <mergeCell ref="C1642:E1642"/>
     <mergeCell ref="C1659:E1659"/>
     <mergeCell ref="C1624:E1624"/>
@@ -39311,7 +39470,6 @@
     <mergeCell ref="C1454:E1454"/>
     <mergeCell ref="C1471:E1471"/>
     <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1744:E1744"/>
     <mergeCell ref="C1556:E1556"/>
     <mergeCell ref="C1573:E1573"/>
     <mergeCell ref="C1590:E1590"/>
@@ -39319,96 +39477,37 @@
     <mergeCell ref="C1505:E1505"/>
     <mergeCell ref="C1522:E1522"/>
     <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C430:E430"/>
-    <mergeCell ref="C447:E447"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C396:E396"/>
-    <mergeCell ref="C413:E413"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C464:E464"/>
-    <mergeCell ref="C481:E481"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C362:E362"/>
-    <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C294:E294"/>
-    <mergeCell ref="C311:E311"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C328:E328"/>
-    <mergeCell ref="C345:E345"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1897:E1897"/>
+    <mergeCell ref="C1914:E1914"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1846:E1846"/>
+    <mergeCell ref="C1863:E1863"/>
+    <mergeCell ref="C1880:E1880"/>
+    <mergeCell ref="C2017:E2017"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C1932:E1932"/>
+    <mergeCell ref="C1949:E1949"/>
+    <mergeCell ref="C1915:E1915"/>
+    <mergeCell ref="C1966:E1966"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C1983:E1983"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2000:E2000"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
1-6 Done and done
</commit_message>
<xml_diff>
--- a/SPP/SPP.xlsx
+++ b/SPP/SPP.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1794" uniqueCount="271">
   <si>
     <t>Notes</t>
   </si>
@@ -828,6 +828,57 @@
   </si>
   <si>
     <t>Bought extra vibe</t>
+  </si>
+  <si>
+    <t>Get Toda 2, Get to Pipe</t>
+  </si>
+  <si>
+    <t>Exit Pipe</t>
+  </si>
+  <si>
+    <t>Hit 3 Flowers, Exit Pipe</t>
+  </si>
+  <si>
+    <t>Hit 4 Flowers, Exit Pipe</t>
+  </si>
+  <si>
+    <t>Hit 5 Flowers, Exit Pipe</t>
+  </si>
+  <si>
+    <t>Get Toad 3, Get to Wheel</t>
+  </si>
+  <si>
+    <t>First White Frame</t>
+  </si>
+  <si>
+    <t>Enter 1-6</t>
+  </si>
+  <si>
+    <t>Enter Boss level (after start)</t>
+  </si>
+  <si>
+    <t>Hit 1</t>
+  </si>
+  <si>
+    <t>Hit 2</t>
+  </si>
+  <si>
+    <t>Hit 3</t>
+  </si>
+  <si>
+    <t>Hit 4</t>
+  </si>
+  <si>
+    <t>Hit 5</t>
+  </si>
+  <si>
+    <t>Save Toad</t>
+  </si>
+  <si>
+    <t>Exit Story</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1674,28 +1725,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="10"/>
       </left>
       <right/>
@@ -1740,6 +1769,28 @@
       </left>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -2049,13 +2100,10 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="7" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="9" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -2071,29 +2119,32 @@
     <xf numFmtId="0" fontId="29" fillId="20" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2129,41 +2180,41 @@
     <xf numFmtId="0" fontId="41" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="43" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="41" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
   </cellXfs>
@@ -2469,8 +2520,8 @@
   <dimension ref="A1:L153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
+      <pane ySplit="6" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J116" sqref="J116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -2486,20 +2537,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="160" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="162"/>
-      <c r="C1" s="163" t="s">
+      <c r="B1" s="161"/>
+      <c r="C1" s="162" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="164"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="163"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
-        <v>-148</v>
+        <v>-694</v>
       </c>
       <c r="I1" s="139" t="s">
         <v>204</v>
@@ -2521,7 +2572,7 @@
       <c r="G2" s="138"/>
       <c r="H2" s="142">
         <f>IF(H1&lt;3600,H1/60,QUOTIENT(H1, 3600))</f>
-        <v>-2.4666666666666668</v>
+        <v>-11.566666666666666</v>
       </c>
       <c r="I2" s="139" t="str">
         <f>IF(H1&lt;3600,"Seconds","Minutes")</f>
@@ -2573,10 +2624,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="159" t="s">
+      <c r="C5" s="158" t="s">
         <v>216</v>
       </c>
-      <c r="D5" s="159"/>
+      <c r="D5" s="158"/>
       <c r="E5" s="145" t="s">
         <v>217</v>
       </c>
@@ -2596,10 +2647,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="159" t="s">
+      <c r="C6" s="158" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="160"/>
+      <c r="D6" s="159"/>
       <c r="E6" s="145"/>
       <c r="F6" s="141"/>
       <c r="G6" s="138"/>
@@ -2617,7 +2668,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="165" t="s">
+      <c r="A8" s="164" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -2760,7 +2811,7 @@
     </row>
     <row r="18" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A19" s="156" t="s">
+      <c r="A19" s="165" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -2999,7 +3050,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A36" s="158" t="s">
+      <c r="A36" s="156" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -3245,7 +3296,7 @@
     </row>
     <row r="52" spans="1:12" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:12" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A53" s="156" t="s">
+      <c r="A53" s="165" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -3536,7 +3587,7 @@
     </row>
     <row r="69" spans="1:12" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:12" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A70" s="158" t="s">
+      <c r="A70" s="156" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -3640,11 +3691,11 @@
         <v>17971</v>
       </c>
       <c r="D75" s="100">
-        <v>17904</v>
+        <v>17900</v>
       </c>
       <c r="E75" s="121">
         <f t="shared" si="4"/>
-        <v>-67</v>
+        <v>-71</v>
       </c>
       <c r="F75" s="104" t="s">
         <v>248</v>
@@ -3659,11 +3710,11 @@
         <v>19416</v>
       </c>
       <c r="D76" s="100">
-        <v>19305</v>
+        <v>19301</v>
       </c>
       <c r="E76" s="121">
         <f t="shared" si="4"/>
-        <v>-111</v>
+        <v>-115</v>
       </c>
       <c r="F76" s="104" t="s">
         <v>250</v>
@@ -3678,11 +3729,11 @@
         <v>20430</v>
       </c>
       <c r="D77" s="100">
-        <v>20310</v>
+        <v>20290</v>
       </c>
       <c r="E77" s="121">
         <f t="shared" si="4"/>
-        <v>-120</v>
+        <v>-140</v>
       </c>
       <c r="F77" s="104"/>
     </row>
@@ -3761,11 +3812,11 @@
         <v>20850</v>
       </c>
       <c r="D84" s="98">
-        <v>20705</v>
+        <v>20701</v>
       </c>
       <c r="E84" s="123">
         <f t="shared" si="4"/>
-        <v>-145</v>
+        <v>-149</v>
       </c>
       <c r="F84" s="103"/>
     </row>
@@ -3782,21 +3833,21 @@
       </c>
       <c r="D85" s="102">
         <f>D84-D71</f>
-        <v>5873</v>
+        <v>5869</v>
       </c>
       <c r="E85" s="124">
         <f>E84-E71</f>
-        <v>-241</v>
+        <v>-245</v>
       </c>
       <c r="F85" s="106"/>
       <c r="G85" s="111">
         <f>E85</f>
-        <v>-241</v>
+        <v>-245</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A87" s="156" t="s">
+      <c r="A87" s="165" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -3824,11 +3875,11 @@
         <v>20850</v>
       </c>
       <c r="D88" s="98">
-        <v>20725</v>
+        <v>20701</v>
       </c>
       <c r="E88" s="121">
         <f t="shared" ref="E88:E101" si="5">IF(AND(C88&gt;0,D88&gt;0), D88-C88, 0)</f>
-        <v>-125</v>
+        <v>-149</v>
       </c>
       <c r="F88" s="103"/>
     </row>
@@ -3841,132 +3892,198 @@
         <v>21141</v>
       </c>
       <c r="D89" s="100">
-        <v>21013</v>
+        <v>20989</v>
       </c>
       <c r="E89" s="122">
         <f t="shared" si="5"/>
-        <v>-128</v>
+        <v>-152</v>
       </c>
       <c r="F89" s="104"/>
     </row>
     <row r="90" spans="1:7" ht="15" outlineLevel="1">
       <c r="A90" s="157"/>
-      <c r="B90" s="99"/>
-      <c r="C90" s="100"/>
-      <c r="D90" s="100"/>
+      <c r="B90" s="99" t="s">
+        <v>243</v>
+      </c>
+      <c r="C90" s="100">
+        <v>22307</v>
+      </c>
+      <c r="D90" s="100">
+        <v>22155</v>
+      </c>
       <c r="E90" s="121">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-152</v>
       </c>
       <c r="F90" s="104"/>
     </row>
     <row r="91" spans="1:7" ht="15" outlineLevel="1">
       <c r="A91" s="157"/>
-      <c r="B91" s="99"/>
-      <c r="C91" s="100"/>
-      <c r="D91" s="100"/>
+      <c r="B91" s="99" t="s">
+        <v>254</v>
+      </c>
+      <c r="C91" s="100">
+        <v>23454</v>
+      </c>
+      <c r="D91" s="100">
+        <v>23301</v>
+      </c>
       <c r="E91" s="121">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-153</v>
       </c>
       <c r="F91" s="104"/>
     </row>
     <row r="92" spans="1:7" ht="15" outlineLevel="1">
       <c r="A92" s="157"/>
-      <c r="B92" s="99"/>
-      <c r="C92" s="100"/>
-      <c r="D92" s="100"/>
+      <c r="B92" s="99" t="s">
+        <v>255</v>
+      </c>
+      <c r="C92" s="100">
+        <v>23732</v>
+      </c>
+      <c r="D92" s="100">
+        <v>23573</v>
+      </c>
       <c r="E92" s="121">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-159</v>
       </c>
       <c r="F92" s="104"/>
     </row>
     <row r="93" spans="1:7" ht="15" outlineLevel="1">
       <c r="A93" s="157"/>
-      <c r="B93" s="99"/>
-      <c r="C93" s="100"/>
-      <c r="D93" s="100"/>
+      <c r="B93" s="99" t="s">
+        <v>256</v>
+      </c>
+      <c r="C93" s="100">
+        <v>24250</v>
+      </c>
+      <c r="D93" s="100">
+        <v>24086</v>
+      </c>
       <c r="E93" s="121">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-164</v>
       </c>
       <c r="F93" s="104"/>
     </row>
     <row r="94" spans="1:7" ht="15" outlineLevel="1">
       <c r="A94" s="157"/>
-      <c r="B94" s="99"/>
-      <c r="C94" s="100"/>
-      <c r="D94" s="100"/>
+      <c r="B94" s="99" t="s">
+        <v>255</v>
+      </c>
+      <c r="C94" s="100">
+        <v>24527</v>
+      </c>
+      <c r="D94" s="100">
+        <v>24358</v>
+      </c>
       <c r="E94" s="121">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-169</v>
       </c>
       <c r="F94" s="104"/>
     </row>
     <row r="95" spans="1:7" ht="15" outlineLevel="1">
       <c r="A95" s="157"/>
-      <c r="B95" s="99"/>
-      <c r="C95" s="100"/>
-      <c r="D95" s="100"/>
+      <c r="B95" s="99" t="s">
+        <v>257</v>
+      </c>
+      <c r="C95" s="100">
+        <v>25192</v>
+      </c>
+      <c r="D95" s="100">
+        <v>24999</v>
+      </c>
       <c r="E95" s="121">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-193</v>
       </c>
       <c r="F95" s="104"/>
     </row>
     <row r="96" spans="1:7" ht="15" outlineLevel="1">
       <c r="A96" s="157"/>
-      <c r="B96" s="99"/>
-      <c r="C96" s="100"/>
-      <c r="D96" s="100"/>
+      <c r="B96" s="99" t="s">
+        <v>255</v>
+      </c>
+      <c r="C96" s="100">
+        <v>25468</v>
+      </c>
+      <c r="D96" s="100">
+        <v>25270</v>
+      </c>
       <c r="E96" s="121">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-198</v>
       </c>
       <c r="F96" s="104"/>
     </row>
     <row r="97" spans="1:7" ht="15" outlineLevel="1">
       <c r="A97" s="157"/>
-      <c r="B97" s="99"/>
-      <c r="C97" s="100"/>
-      <c r="D97" s="100"/>
+      <c r="B97" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="C97" s="100">
+        <v>27850</v>
+      </c>
+      <c r="D97" s="100">
+        <v>27480</v>
+      </c>
       <c r="E97" s="121">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-370</v>
       </c>
       <c r="F97" s="104"/>
     </row>
     <row r="98" spans="1:7" ht="15" outlineLevel="1">
       <c r="A98" s="157"/>
-      <c r="B98" s="99"/>
-      <c r="C98" s="100"/>
-      <c r="D98" s="100"/>
+      <c r="B98" s="99" t="s">
+        <v>255</v>
+      </c>
+      <c r="C98" s="100">
+        <v>28129</v>
+      </c>
+      <c r="D98" s="100">
+        <v>27753</v>
+      </c>
       <c r="E98" s="121">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-376</v>
       </c>
       <c r="F98" s="104"/>
     </row>
     <row r="99" spans="1:7" ht="15" outlineLevel="1">
       <c r="A99" s="157"/>
-      <c r="B99" s="99"/>
-      <c r="C99" s="100"/>
-      <c r="D99" s="100"/>
+      <c r="B99" s="99" t="s">
+        <v>255</v>
+      </c>
+      <c r="C99" s="100">
+        <v>28918</v>
+      </c>
+      <c r="D99" s="100">
+        <v>28538</v>
+      </c>
       <c r="E99" s="121">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-380</v>
       </c>
       <c r="F99" s="104"/>
     </row>
     <row r="100" spans="1:7" ht="15" outlineLevel="1">
       <c r="A100" s="157"/>
-      <c r="B100" s="99"/>
-      <c r="C100" s="100"/>
-      <c r="D100" s="100"/>
+      <c r="B100" s="99" t="s">
+        <v>259</v>
+      </c>
+      <c r="C100" s="100">
+        <v>30350</v>
+      </c>
+      <c r="D100" s="100">
+        <v>29893</v>
+      </c>
       <c r="E100" s="121">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-457</v>
       </c>
       <c r="F100" s="104"/>
     </row>
@@ -3976,14 +4093,14 @@
         <v>187</v>
       </c>
       <c r="C101" s="98">
-        <v>21141</v>
+        <v>30350</v>
       </c>
       <c r="D101" s="98">
-        <v>21013</v>
+        <v>29893</v>
       </c>
       <c r="E101" s="123">
         <f t="shared" si="5"/>
-        <v>-128</v>
+        <v>-457</v>
       </c>
       <c r="F101" s="103"/>
     </row>
@@ -3996,24 +4113,25 @@
       </c>
       <c r="C102" s="102">
         <f>C101-C88</f>
-        <v>291</v>
+        <v>9500</v>
       </c>
       <c r="D102" s="102">
         <f>D101-D88</f>
-        <v>288</v>
+        <v>9192</v>
       </c>
       <c r="E102" s="124">
         <f>E101-E88</f>
-        <v>-3</v>
+        <v>-308</v>
       </c>
       <c r="F102" s="107"/>
       <c r="G102" s="111">
         <f>E102</f>
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="158" t="s">
+        <v>-308</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="13.5" thickBot="1"/>
+    <row r="104" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A104" s="156" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -4032,130 +4150,194 @@
         <v>183</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="105" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="A105" s="157"/>
       <c r="B105" s="97" t="s">
         <v>184</v>
       </c>
-      <c r="C105" s="98"/>
-      <c r="D105" s="98"/>
+      <c r="C105" s="98">
+        <v>30350</v>
+      </c>
+      <c r="D105" s="98">
+        <v>29893</v>
+      </c>
       <c r="E105" s="121">
         <f t="shared" ref="E105:E118" si="6">IF(AND(C105&gt;0,D105&gt;0), D105-C105, 0)</f>
-        <v>0</v>
+        <v>-457</v>
       </c>
       <c r="F105" s="103"/>
     </row>
-    <row r="106" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
+    <row r="106" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A106" s="157"/>
-      <c r="B106" s="99"/>
-      <c r="C106" s="100"/>
-      <c r="D106" s="100"/>
+      <c r="B106" s="99" t="s">
+        <v>261</v>
+      </c>
+      <c r="C106" s="100">
+        <v>30606</v>
+      </c>
+      <c r="D106" s="100">
+        <v>30146</v>
+      </c>
       <c r="E106" s="122">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-460</v>
       </c>
       <c r="F106" s="104"/>
     </row>
-    <row r="107" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="107" spans="1:7" ht="15" outlineLevel="1">
       <c r="A107" s="157"/>
-      <c r="B107" s="99"/>
-      <c r="C107" s="100"/>
-      <c r="D107" s="100"/>
+      <c r="B107" s="99" t="s">
+        <v>260</v>
+      </c>
+      <c r="C107" s="100">
+        <v>31145</v>
+      </c>
+      <c r="D107" s="100">
+        <v>30558</v>
+      </c>
       <c r="E107" s="121">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-587</v>
       </c>
       <c r="F107" s="104"/>
     </row>
-    <row r="108" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="108" spans="1:7" ht="15" outlineLevel="1">
       <c r="A108" s="157"/>
-      <c r="B108" s="99"/>
-      <c r="C108" s="100"/>
-      <c r="D108" s="100"/>
+      <c r="B108" s="99" t="s">
+        <v>262</v>
+      </c>
+      <c r="C108" s="100">
+        <v>31474</v>
+      </c>
+      <c r="D108" s="100">
+        <v>30873</v>
+      </c>
       <c r="E108" s="121">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-601</v>
       </c>
       <c r="F108" s="104"/>
     </row>
-    <row r="109" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="109" spans="1:7" ht="15" outlineLevel="1">
       <c r="A109" s="157"/>
-      <c r="B109" s="99"/>
-      <c r="C109" s="100"/>
-      <c r="D109" s="100"/>
+      <c r="B109" s="99" t="s">
+        <v>263</v>
+      </c>
+      <c r="C109" s="100">
+        <v>31789</v>
+      </c>
+      <c r="D109" s="100">
+        <v>31185</v>
+      </c>
       <c r="E109" s="121">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-604</v>
       </c>
       <c r="F109" s="104"/>
     </row>
-    <row r="110" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="110" spans="1:7" ht="15" outlineLevel="1">
       <c r="A110" s="157"/>
-      <c r="B110" s="99"/>
-      <c r="C110" s="100"/>
-      <c r="D110" s="100"/>
+      <c r="B110" s="99" t="s">
+        <v>264</v>
+      </c>
+      <c r="C110" s="100">
+        <v>32528</v>
+      </c>
+      <c r="D110" s="100">
+        <v>31865</v>
+      </c>
       <c r="E110" s="121">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-663</v>
       </c>
       <c r="F110" s="104"/>
     </row>
-    <row r="111" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="111" spans="1:7" ht="15" outlineLevel="1">
       <c r="A111" s="157"/>
-      <c r="B111" s="99"/>
-      <c r="C111" s="100"/>
-      <c r="D111" s="100"/>
+      <c r="B111" s="99" t="s">
+        <v>265</v>
+      </c>
+      <c r="C111" s="100">
+        <v>33212</v>
+      </c>
+      <c r="D111" s="100">
+        <v>32552</v>
+      </c>
       <c r="E111" s="121">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-660</v>
       </c>
       <c r="F111" s="104"/>
     </row>
-    <row r="112" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="112" spans="1:7" ht="15" outlineLevel="1">
       <c r="A112" s="157"/>
-      <c r="B112" s="99"/>
-      <c r="C112" s="100"/>
-      <c r="D112" s="100"/>
+      <c r="B112" s="99" t="s">
+        <v>266</v>
+      </c>
+      <c r="C112" s="100">
+        <v>34101</v>
+      </c>
+      <c r="D112" s="100">
+        <v>33435</v>
+      </c>
       <c r="E112" s="121">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-666</v>
       </c>
       <c r="F112" s="104"/>
     </row>
-    <row r="113" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="113" spans="1:10" ht="15" outlineLevel="1">
       <c r="A113" s="157"/>
-      <c r="B113" s="99"/>
-      <c r="C113" s="100"/>
-      <c r="D113" s="100"/>
+      <c r="B113" s="99" t="s">
+        <v>267</v>
+      </c>
+      <c r="C113" s="100">
+        <v>34909</v>
+      </c>
+      <c r="D113" s="100">
+        <v>34214</v>
+      </c>
       <c r="E113" s="121">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-695</v>
       </c>
       <c r="F113" s="104"/>
     </row>
-    <row r="114" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="114" spans="1:10" ht="15" outlineLevel="1">
       <c r="A114" s="157"/>
-      <c r="B114" s="99"/>
-      <c r="C114" s="100"/>
-      <c r="D114" s="100"/>
+      <c r="B114" s="99" t="s">
+        <v>268</v>
+      </c>
+      <c r="C114" s="100">
+        <v>35695</v>
+      </c>
+      <c r="D114" s="100">
+        <v>35003</v>
+      </c>
       <c r="E114" s="121">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-692</v>
       </c>
       <c r="F114" s="104"/>
     </row>
-    <row r="115" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="115" spans="1:10" ht="15" outlineLevel="1">
       <c r="A115" s="157"/>
-      <c r="B115" s="99"/>
-      <c r="C115" s="100"/>
-      <c r="D115" s="100"/>
+      <c r="B115" s="99" t="s">
+        <v>269</v>
+      </c>
+      <c r="C115" s="100">
+        <v>35811</v>
+      </c>
+      <c r="D115" s="100">
+        <v>35117</v>
+      </c>
       <c r="E115" s="121">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-694</v>
       </c>
       <c r="F115" s="104"/>
     </row>
-    <row r="116" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="116" spans="1:10" ht="15" outlineLevel="1">
       <c r="A116" s="157"/>
       <c r="B116" s="99"/>
       <c r="C116" s="100"/>
@@ -4165,8 +4347,11 @@
         <v>0</v>
       </c>
       <c r="F116" s="104"/>
-    </row>
-    <row r="117" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+      <c r="J116" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" ht="15" outlineLevel="1">
       <c r="A117" s="157"/>
       <c r="B117" s="99"/>
       <c r="C117" s="100"/>
@@ -4177,20 +4362,24 @@
       </c>
       <c r="F117" s="104"/>
     </row>
-    <row r="118" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="118" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="A118" s="157"/>
       <c r="B118" s="97" t="s">
         <v>187</v>
       </c>
-      <c r="C118" s="98"/>
-      <c r="D118" s="98"/>
+      <c r="C118" s="98">
+        <v>35811</v>
+      </c>
+      <c r="D118" s="98">
+        <v>35117</v>
+      </c>
       <c r="E118" s="123">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-694</v>
       </c>
       <c r="F118" s="103"/>
     </row>
-    <row r="119" spans="1:7" ht="16.5" collapsed="1" thickBot="1">
+    <row r="119" spans="1:10" ht="17.25" thickTop="1" thickBot="1">
       <c r="A119" s="115">
         <v>6</v>
       </c>
@@ -4199,24 +4388,24 @@
       </c>
       <c r="C119" s="102">
         <f>C118-C105</f>
-        <v>0</v>
+        <v>5461</v>
       </c>
       <c r="D119" s="102">
         <f>D118-D105</f>
-        <v>0</v>
+        <v>5224</v>
       </c>
       <c r="E119" s="102">
         <f>E118-E105</f>
-        <v>0</v>
+        <v>-237</v>
       </c>
       <c r="F119" s="106"/>
       <c r="G119" s="111">
         <f>E119</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="156" t="s">
+        <v>-237</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" ht="15" hidden="1" outlineLevel="1">
+      <c r="A121" s="165" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -4235,7 +4424,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="122" spans="1:10" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A122" s="157"/>
       <c r="B122" s="97" t="s">
         <v>184</v>
@@ -4248,7 +4437,7 @@
       </c>
       <c r="F122" s="103"/>
     </row>
-    <row r="123" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
+    <row r="123" spans="1:10" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
       <c r="A123" s="157"/>
       <c r="B123" s="99"/>
       <c r="C123" s="100"/>
@@ -4259,7 +4448,7 @@
       </c>
       <c r="F123" s="104"/>
     </row>
-    <row r="124" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="124" spans="1:10" ht="15" hidden="1" outlineLevel="1">
       <c r="A124" s="157"/>
       <c r="B124" s="99"/>
       <c r="C124" s="100"/>
@@ -4270,7 +4459,7 @@
       </c>
       <c r="F124" s="104"/>
     </row>
-    <row r="125" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="125" spans="1:10" ht="15" hidden="1" outlineLevel="1">
       <c r="A125" s="157"/>
       <c r="B125" s="99"/>
       <c r="C125" s="100"/>
@@ -4281,7 +4470,7 @@
       </c>
       <c r="F125" s="104"/>
     </row>
-    <row r="126" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="126" spans="1:10" ht="15" hidden="1" outlineLevel="1">
       <c r="A126" s="157"/>
       <c r="B126" s="99"/>
       <c r="C126" s="100"/>
@@ -4292,7 +4481,7 @@
       </c>
       <c r="F126" s="104"/>
     </row>
-    <row r="127" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="127" spans="1:10" ht="15" hidden="1" outlineLevel="1">
       <c r="A127" s="157"/>
       <c r="B127" s="99"/>
       <c r="C127" s="100"/>
@@ -4303,7 +4492,7 @@
       </c>
       <c r="F127" s="104"/>
     </row>
-    <row r="128" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="128" spans="1:10" ht="15" hidden="1" outlineLevel="1">
       <c r="A128" s="157"/>
       <c r="B128" s="99"/>
       <c r="C128" s="100"/>
@@ -4419,7 +4608,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="158" t="s">
+      <c r="A138" s="156" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -4623,6 +4812,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="A138:A152"/>
+    <mergeCell ref="A104:A118"/>
+    <mergeCell ref="A70:A84"/>
+    <mergeCell ref="A121:A135"/>
+    <mergeCell ref="A87:A101"/>
     <mergeCell ref="A36:A50"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
@@ -4630,12 +4825,6 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="A138:A152"/>
-    <mergeCell ref="A104:A118"/>
-    <mergeCell ref="A70:A84"/>
-    <mergeCell ref="A121:A135"/>
-    <mergeCell ref="A87:A101"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5680,7 +5869,7 @@
       </c>
       <c r="C6" s="132">
         <f ca="1">'FrameCounts World 1'!H2</f>
-        <v>-2.4666666666666668</v>
+        <v>-11.566666666666666</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -5692,7 +5881,7 @@
       </c>
       <c r="C7" s="133">
         <f>C6/60</f>
-        <v>-4.1111111111111112E-2</v>
+        <v>-0.19277777777777777</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -5893,10 +6082,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="208" t="s">
+      <c r="A1" s="212" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="209"/>
+      <c r="B1" s="213"/>
       <c r="C1" s="117"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
@@ -5916,127 +6105,142 @@
       <c r="C3" s="118"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="212"/>
-      <c r="B4" s="213"/>
+      <c r="A4" s="216"/>
+      <c r="B4" s="217"/>
       <c r="C4" s="118"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="210" t="s">
+      <c r="A5" s="214" t="s">
         <v>202</v>
       </c>
-      <c r="B5" s="211"/>
+      <c r="B5" s="215"/>
       <c r="C5" s="118"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="216" t="s">
+      <c r="A7" s="206" t="s">
         <v>194</v>
       </c>
-      <c r="B7" s="217"/>
+      <c r="B7" s="207"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="118"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="214" t="s">
+      <c r="A9" s="208" t="s">
         <v>195</v>
       </c>
-      <c r="B9" s="215"/>
+      <c r="B9" s="209"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="204"/>
-      <c r="B10" s="205"/>
+      <c r="A10" s="210"/>
+      <c r="B10" s="211"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="206" t="s">
+      <c r="A11" s="202" t="s">
         <v>196</v>
       </c>
-      <c r="B11" s="207"/>
+      <c r="B11" s="203"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="206" t="s">
+      <c r="A12" s="202" t="s">
         <v>197</v>
       </c>
-      <c r="B12" s="207"/>
+      <c r="B12" s="203"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="206" t="s">
+      <c r="A13" s="202" t="s">
         <v>198</v>
       </c>
-      <c r="B13" s="207"/>
+      <c r="B13" s="203"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="206" t="s">
+      <c r="A14" s="202" t="s">
         <v>199</v>
       </c>
-      <c r="B14" s="207"/>
+      <c r="B14" s="203"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="206" t="s">
+      <c r="A15" s="202" t="s">
         <v>200</v>
       </c>
-      <c r="B15" s="207"/>
+      <c r="B15" s="203"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="206" t="s">
+      <c r="A16" s="202" t="s">
         <v>201</v>
       </c>
-      <c r="B16" s="207"/>
+      <c r="B16" s="203"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="202" t="s">
+      <c r="A17" s="204" t="s">
         <v>203</v>
       </c>
-      <c r="B17" s="203"/>
+      <c r="B17" s="205"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="216" t="s">
+      <c r="A19" s="206" t="s">
         <v>205</v>
       </c>
-      <c r="B19" s="217"/>
+      <c r="B19" s="207"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="118"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="214" t="s">
+      <c r="A21" s="208" t="s">
         <v>206</v>
       </c>
-      <c r="B21" s="215"/>
+      <c r="B21" s="209"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="204"/>
-      <c r="B22" s="205"/>
+      <c r="A22" s="210"/>
+      <c r="B22" s="211"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="206" t="s">
+      <c r="A23" s="202" t="s">
         <v>207</v>
       </c>
-      <c r="B23" s="207"/>
+      <c r="B23" s="203"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="206"/>
-      <c r="B24" s="207"/>
+      <c r="A24" s="202"/>
+      <c r="B24" s="203"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="206" t="s">
+      <c r="A25" s="202" t="s">
         <v>208</v>
       </c>
-      <c r="B25" s="207"/>
+      <c r="B25" s="203"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="206" t="s">
+      <c r="A26" s="202" t="s">
         <v>209</v>
       </c>
-      <c r="B26" s="207"/>
+      <c r="B26" s="203"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="202"/>
-      <c r="B27" s="203"/>
+      <c r="A27" s="204"/>
+      <c r="B27" s="205"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
@@ -6045,21 +6249,6 @@
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -6094,16 +6283,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="160" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="162"/>
-      <c r="C1" s="163" t="s">
+      <c r="B1" s="161"/>
+      <c r="C1" s="162" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="164"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="163"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -6181,10 +6370,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="159" t="s">
+      <c r="C5" s="158" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="159"/>
+      <c r="D5" s="158"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -6200,10 +6389,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="159" t="s">
+      <c r="C6" s="158" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="160"/>
+      <c r="D6" s="159"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -6221,7 +6410,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="165" t="s">
+      <c r="A8" s="164" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -6360,7 +6549,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="156" t="s">
+      <c r="A19" s="165" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -6564,7 +6753,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="158" t="s">
+      <c r="A36" s="156" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -6768,7 +6957,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="156" t="s">
+      <c r="A53" s="165" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -6972,7 +7161,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="158" t="s">
+      <c r="A70" s="156" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -7176,7 +7365,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="156" t="s">
+      <c r="A87" s="165" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -7379,7 +7568,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="158" t="s">
+      <c r="A104" s="156" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -7582,7 +7771,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="156" t="s">
+      <c r="A121" s="165" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -7785,7 +7974,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="158" t="s">
+      <c r="A138" s="156" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -7989,12 +8178,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="A138:A152"/>
-    <mergeCell ref="A104:A118"/>
-    <mergeCell ref="A70:A84"/>
-    <mergeCell ref="A121:A135"/>
-    <mergeCell ref="A87:A101"/>
     <mergeCell ref="A36:A50"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
@@ -8002,6 +8185,12 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="A138:A152"/>
+    <mergeCell ref="A104:A118"/>
+    <mergeCell ref="A70:A84"/>
+    <mergeCell ref="A121:A135"/>
+    <mergeCell ref="A87:A101"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8035,16 +8224,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="160" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="162"/>
-      <c r="C1" s="163" t="s">
+      <c r="B1" s="161"/>
+      <c r="C1" s="162" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="164"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="163"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -8122,10 +8311,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="159" t="s">
+      <c r="C5" s="158" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="159"/>
+      <c r="D5" s="158"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -8141,10 +8330,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="159" t="s">
+      <c r="C6" s="158" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="160"/>
+      <c r="D6" s="159"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -8162,7 +8351,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="165" t="s">
+      <c r="A8" s="164" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -8301,7 +8490,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="156" t="s">
+      <c r="A19" s="165" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -8505,7 +8694,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="158" t="s">
+      <c r="A36" s="156" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -8709,7 +8898,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="156" t="s">
+      <c r="A53" s="165" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -8913,7 +9102,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="158" t="s">
+      <c r="A70" s="156" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -9117,7 +9306,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="156" t="s">
+      <c r="A87" s="165" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -9320,7 +9509,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="158" t="s">
+      <c r="A104" s="156" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -9523,7 +9712,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="156" t="s">
+      <c r="A121" s="165" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -9726,7 +9915,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="158" t="s">
+      <c r="A138" s="156" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -9930,6 +10119,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="A138:A152"/>
+    <mergeCell ref="A104:A118"/>
+    <mergeCell ref="A70:A84"/>
+    <mergeCell ref="A121:A135"/>
+    <mergeCell ref="A87:A101"/>
     <mergeCell ref="A36:A50"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
@@ -9937,12 +10132,6 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="A138:A152"/>
-    <mergeCell ref="A104:A118"/>
-    <mergeCell ref="A70:A84"/>
-    <mergeCell ref="A121:A135"/>
-    <mergeCell ref="A87:A101"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9976,16 +10165,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="160" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="162"/>
-      <c r="C1" s="163" t="s">
+      <c r="B1" s="161"/>
+      <c r="C1" s="162" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="164"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="163"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -10063,10 +10252,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="159" t="s">
+      <c r="C5" s="158" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="159"/>
+      <c r="D5" s="158"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -10082,10 +10271,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="159" t="s">
+      <c r="C6" s="158" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="160"/>
+      <c r="D6" s="159"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -10103,7 +10292,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="165" t="s">
+      <c r="A8" s="164" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -10242,7 +10431,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="156" t="s">
+      <c r="A19" s="165" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -10446,7 +10635,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="158" t="s">
+      <c r="A36" s="156" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -10650,7 +10839,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="156" t="s">
+      <c r="A53" s="165" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -10854,7 +11043,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="158" t="s">
+      <c r="A70" s="156" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -11058,7 +11247,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="156" t="s">
+      <c r="A87" s="165" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -11261,7 +11450,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="158" t="s">
+      <c r="A104" s="156" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -11464,7 +11653,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="156" t="s">
+      <c r="A121" s="165" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -11667,7 +11856,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="158" t="s">
+      <c r="A138" s="156" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -11871,12 +12060,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="A138:A152"/>
-    <mergeCell ref="A104:A118"/>
-    <mergeCell ref="A70:A84"/>
-    <mergeCell ref="A121:A135"/>
-    <mergeCell ref="A87:A101"/>
     <mergeCell ref="A36:A50"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
@@ -11884,6 +12067,12 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="A138:A152"/>
+    <mergeCell ref="A104:A118"/>
+    <mergeCell ref="A70:A84"/>
+    <mergeCell ref="A121:A135"/>
+    <mergeCell ref="A87:A101"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11917,16 +12106,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="160" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="162"/>
-      <c r="C1" s="163" t="s">
+      <c r="B1" s="161"/>
+      <c r="C1" s="162" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="164"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="163"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -12004,10 +12193,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="159" t="s">
+      <c r="C5" s="158" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="159"/>
+      <c r="D5" s="158"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -12023,10 +12212,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="159" t="s">
+      <c r="C6" s="158" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="160"/>
+      <c r="D6" s="159"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -12044,7 +12233,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="165" t="s">
+      <c r="A8" s="164" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -12183,7 +12372,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="156" t="s">
+      <c r="A19" s="165" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -12387,7 +12576,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="158" t="s">
+      <c r="A36" s="156" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -12591,7 +12780,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="156" t="s">
+      <c r="A53" s="165" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -12795,7 +12984,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="158" t="s">
+      <c r="A70" s="156" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -12999,7 +13188,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="156" t="s">
+      <c r="A87" s="165" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -13202,7 +13391,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="158" t="s">
+      <c r="A104" s="156" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -13405,7 +13594,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="156" t="s">
+      <c r="A121" s="165" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -13608,7 +13797,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="158" t="s">
+      <c r="A138" s="156" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -13812,6 +14001,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="A138:A152"/>
+    <mergeCell ref="A104:A118"/>
+    <mergeCell ref="A70:A84"/>
+    <mergeCell ref="A121:A135"/>
+    <mergeCell ref="A87:A101"/>
     <mergeCell ref="A36:A50"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
@@ -13819,12 +14014,6 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="A138:A152"/>
-    <mergeCell ref="A104:A118"/>
-    <mergeCell ref="A70:A84"/>
-    <mergeCell ref="A121:A135"/>
-    <mergeCell ref="A87:A101"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13858,16 +14047,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="160" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="162"/>
-      <c r="C1" s="163" t="s">
+      <c r="B1" s="161"/>
+      <c r="C1" s="162" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="164"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="163"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -13945,10 +14134,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="159" t="s">
+      <c r="C5" s="158" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="159"/>
+      <c r="D5" s="158"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -13964,10 +14153,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="159" t="s">
+      <c r="C6" s="158" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="160"/>
+      <c r="D6" s="159"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -13985,7 +14174,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="165" t="s">
+      <c r="A8" s="164" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -14124,7 +14313,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="156" t="s">
+      <c r="A19" s="165" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -14328,7 +14517,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="158" t="s">
+      <c r="A36" s="156" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -14532,7 +14721,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="156" t="s">
+      <c r="A53" s="165" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -14736,7 +14925,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="158" t="s">
+      <c r="A70" s="156" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -14940,7 +15129,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="156" t="s">
+      <c r="A87" s="165" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -15143,7 +15332,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="158" t="s">
+      <c r="A104" s="156" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -15346,7 +15535,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="156" t="s">
+      <c r="A121" s="165" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -15549,7 +15738,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="158" t="s">
+      <c r="A138" s="156" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -15753,12 +15942,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="A138:A152"/>
-    <mergeCell ref="A104:A118"/>
-    <mergeCell ref="A70:A84"/>
-    <mergeCell ref="A121:A135"/>
-    <mergeCell ref="A87:A101"/>
     <mergeCell ref="A36:A50"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
@@ -15766,6 +15949,12 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="A138:A152"/>
+    <mergeCell ref="A104:A118"/>
+    <mergeCell ref="A70:A84"/>
+    <mergeCell ref="A121:A135"/>
+    <mergeCell ref="A87:A101"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15799,16 +15988,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="160" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="162"/>
-      <c r="C1" s="163" t="s">
+      <c r="B1" s="161"/>
+      <c r="C1" s="162" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="164"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="163"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -15886,10 +16075,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="159" t="s">
+      <c r="C5" s="158" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="159"/>
+      <c r="D5" s="158"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -15905,10 +16094,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="159" t="s">
+      <c r="C6" s="158" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="160"/>
+      <c r="D6" s="159"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -15926,7 +16115,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="165" t="s">
+      <c r="A8" s="164" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -16065,7 +16254,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="156" t="s">
+      <c r="A19" s="165" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -16269,7 +16458,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="158" t="s">
+      <c r="A36" s="156" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -16473,7 +16662,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="156" t="s">
+      <c r="A53" s="165" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -16677,7 +16866,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="158" t="s">
+      <c r="A70" s="156" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -16881,7 +17070,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="156" t="s">
+      <c r="A87" s="165" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -17084,7 +17273,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="158" t="s">
+      <c r="A104" s="156" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -17287,7 +17476,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="156" t="s">
+      <c r="A121" s="165" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -17490,7 +17679,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="158" t="s">
+      <c r="A138" s="156" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -17694,6 +17883,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="A138:A152"/>
+    <mergeCell ref="A104:A118"/>
+    <mergeCell ref="A70:A84"/>
+    <mergeCell ref="A121:A135"/>
+    <mergeCell ref="A87:A101"/>
     <mergeCell ref="A36:A50"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
@@ -17701,12 +17896,6 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="A138:A152"/>
-    <mergeCell ref="A104:A118"/>
-    <mergeCell ref="A70:A84"/>
-    <mergeCell ref="A121:A135"/>
-    <mergeCell ref="A87:A101"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17740,16 +17929,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="160" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="162"/>
-      <c r="C1" s="163" t="s">
+      <c r="B1" s="161"/>
+      <c r="C1" s="162" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="164"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="163"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65535)</f>
@@ -17827,10 +18016,10 @@
       <c r="B5" s="145" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="159" t="s">
+      <c r="C5" s="158" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="159"/>
+      <c r="D5" s="158"/>
       <c r="E5" s="145"/>
       <c r="F5" s="146"/>
       <c r="G5" s="138"/>
@@ -17846,10 +18035,10 @@
       <c r="B6" s="145" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="159" t="s">
+      <c r="C6" s="158" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="160"/>
+      <c r="D6" s="159"/>
       <c r="E6" s="145"/>
       <c r="F6" s="146"/>
       <c r="G6" s="138"/>
@@ -17867,7 +18056,7 @@
       <c r="F7" s="147"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="165" t="s">
+      <c r="A8" s="164" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="94" t="s">
@@ -18006,7 +18195,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="156" t="s">
+      <c r="A19" s="165" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="108" t="s">
@@ -18210,7 +18399,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="158" t="s">
+      <c r="A36" s="156" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -18414,7 +18603,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="156" t="s">
+      <c r="A53" s="165" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="108" t="s">
@@ -18618,7 +18807,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="158" t="s">
+      <c r="A70" s="156" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="112" t="s">
@@ -18822,7 +19011,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="156" t="s">
+      <c r="A87" s="165" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="108" t="s">
@@ -19025,7 +19214,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="158" t="s">
+      <c r="A104" s="156" t="s">
         <v>174</v>
       </c>
       <c r="B104" s="112" t="s">
@@ -19228,7 +19417,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="156" t="s">
+      <c r="A121" s="165" t="s">
         <v>175</v>
       </c>
       <c r="B121" s="108" t="s">
@@ -19431,7 +19620,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="158" t="s">
+      <c r="A138" s="156" t="s">
         <v>176</v>
       </c>
       <c r="B138" s="112" t="s">
@@ -19635,12 +19824,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="A138:A152"/>
-    <mergeCell ref="A104:A118"/>
-    <mergeCell ref="A70:A84"/>
-    <mergeCell ref="A121:A135"/>
-    <mergeCell ref="A87:A101"/>
     <mergeCell ref="A36:A50"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
@@ -19648,6 +19831,12 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="A138:A152"/>
+    <mergeCell ref="A104:A118"/>
+    <mergeCell ref="A70:A84"/>
+    <mergeCell ref="A121:A135"/>
+    <mergeCell ref="A87:A101"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19681,13 +19870,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="184" t="s">
+      <c r="A1" s="168" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="184"/>
-      <c r="C1" s="184"/>
-      <c r="D1" s="184"/>
-      <c r="E1" s="184"/>
+      <c r="B1" s="168"/>
+      <c r="C1" s="168"/>
+      <c r="D1" s="168"/>
+      <c r="E1" s="168"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -19717,18 +19906,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="185"/>
-      <c r="D3" s="186"/>
-      <c r="E3" s="186"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="170"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="168"/>
-      <c r="D4" s="169"/>
-      <c r="E4" s="169"/>
+      <c r="C4" s="166"/>
+      <c r="D4" s="167"/>
+      <c r="E4" s="167"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -19880,9 +20069,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="166"/>
-      <c r="D21" s="167"/>
-      <c r="E21" s="167"/>
+      <c r="C21" s="171"/>
+      <c r="D21" s="172"/>
+      <c r="E21" s="172"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -20033,9 +20222,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="168"/>
-      <c r="D38" s="169"/>
-      <c r="E38" s="169"/>
+      <c r="C38" s="166"/>
+      <c r="D38" s="167"/>
+      <c r="E38" s="167"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -20186,9 +20375,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="168"/>
-      <c r="D55" s="169"/>
-      <c r="E55" s="169"/>
+      <c r="C55" s="166"/>
+      <c r="D55" s="167"/>
+      <c r="E55" s="167"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -20339,9 +20528,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="168"/>
-      <c r="D72" s="169"/>
-      <c r="E72" s="169"/>
+      <c r="C72" s="166"/>
+      <c r="D72" s="167"/>
+      <c r="E72" s="167"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -20492,9 +20681,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="168"/>
-      <c r="D89" s="169"/>
-      <c r="E89" s="169"/>
+      <c r="C89" s="166"/>
+      <c r="D89" s="167"/>
+      <c r="E89" s="167"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -20645,9 +20834,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="168"/>
-      <c r="D106" s="169"/>
-      <c r="E106" s="169"/>
+      <c r="C106" s="166"/>
+      <c r="D106" s="167"/>
+      <c r="E106" s="167"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -20798,9 +20987,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="168"/>
-      <c r="D123" s="169"/>
-      <c r="E123" s="169"/>
+      <c r="C123" s="166"/>
+      <c r="D123" s="167"/>
+      <c r="E123" s="167"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -20951,9 +21140,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="168"/>
-      <c r="D140" s="169"/>
-      <c r="E140" s="169"/>
+      <c r="C140" s="166"/>
+      <c r="D140" s="167"/>
+      <c r="E140" s="167"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -21104,9 +21293,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="168"/>
-      <c r="D157" s="169"/>
-      <c r="E157" s="169"/>
+      <c r="C157" s="166"/>
+      <c r="D157" s="167"/>
+      <c r="E157" s="167"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -21257,9 +21446,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="168"/>
-      <c r="D174" s="169"/>
-      <c r="E174" s="169"/>
+      <c r="C174" s="166"/>
+      <c r="D174" s="167"/>
+      <c r="E174" s="167"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -21410,9 +21599,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="168"/>
-      <c r="D191" s="169"/>
-      <c r="E191" s="169"/>
+      <c r="C191" s="166"/>
+      <c r="D191" s="167"/>
+      <c r="E191" s="167"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -21563,9 +21752,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="168"/>
-      <c r="D208" s="169"/>
-      <c r="E208" s="169"/>
+      <c r="C208" s="166"/>
+      <c r="D208" s="167"/>
+      <c r="E208" s="167"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -21716,9 +21905,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="168"/>
-      <c r="D225" s="169"/>
-      <c r="E225" s="169"/>
+      <c r="C225" s="166"/>
+      <c r="D225" s="167"/>
+      <c r="E225" s="167"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -21869,9 +22058,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="168"/>
-      <c r="D242" s="169"/>
-      <c r="E242" s="169"/>
+      <c r="C242" s="166"/>
+      <c r="D242" s="167"/>
+      <c r="E242" s="167"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -22022,9 +22211,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="168"/>
-      <c r="D259" s="169"/>
-      <c r="E259" s="169"/>
+      <c r="C259" s="166"/>
+      <c r="D259" s="167"/>
+      <c r="E259" s="167"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -22175,18 +22364,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="182"/>
-      <c r="D276" s="183"/>
-      <c r="E276" s="183"/>
+      <c r="C276" s="175"/>
+      <c r="D276" s="176"/>
+      <c r="E276" s="176"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="168"/>
-      <c r="D277" s="169"/>
-      <c r="E277" s="169"/>
+      <c r="C277" s="166"/>
+      <c r="D277" s="167"/>
+      <c r="E277" s="167"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -22337,9 +22526,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="166"/>
-      <c r="D294" s="167"/>
-      <c r="E294" s="167"/>
+      <c r="C294" s="171"/>
+      <c r="D294" s="172"/>
+      <c r="E294" s="172"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -22490,9 +22679,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="168"/>
-      <c r="D311" s="169"/>
-      <c r="E311" s="169"/>
+      <c r="C311" s="166"/>
+      <c r="D311" s="167"/>
+      <c r="E311" s="167"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -22643,9 +22832,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="168"/>
-      <c r="D328" s="169"/>
-      <c r="E328" s="169"/>
+      <c r="C328" s="166"/>
+      <c r="D328" s="167"/>
+      <c r="E328" s="167"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -22796,9 +22985,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="168"/>
-      <c r="D345" s="169"/>
-      <c r="E345" s="169"/>
+      <c r="C345" s="166"/>
+      <c r="D345" s="167"/>
+      <c r="E345" s="167"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -22949,9 +23138,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="168"/>
-      <c r="D362" s="169"/>
-      <c r="E362" s="169"/>
+      <c r="C362" s="166"/>
+      <c r="D362" s="167"/>
+      <c r="E362" s="167"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -23102,9 +23291,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="168"/>
-      <c r="D379" s="169"/>
-      <c r="E379" s="169"/>
+      <c r="C379" s="166"/>
+      <c r="D379" s="167"/>
+      <c r="E379" s="167"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -23255,9 +23444,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="168"/>
-      <c r="D396" s="169"/>
-      <c r="E396" s="169"/>
+      <c r="C396" s="166"/>
+      <c r="D396" s="167"/>
+      <c r="E396" s="167"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -23408,9 +23597,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="168"/>
-      <c r="D413" s="169"/>
-      <c r="E413" s="169"/>
+      <c r="C413" s="166"/>
+      <c r="D413" s="167"/>
+      <c r="E413" s="167"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -23561,9 +23750,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="168"/>
-      <c r="D430" s="169"/>
-      <c r="E430" s="169"/>
+      <c r="C430" s="166"/>
+      <c r="D430" s="167"/>
+      <c r="E430" s="167"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -23714,9 +23903,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="168"/>
-      <c r="D447" s="169"/>
-      <c r="E447" s="169"/>
+      <c r="C447" s="166"/>
+      <c r="D447" s="167"/>
+      <c r="E447" s="167"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -23867,9 +24056,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="168"/>
-      <c r="D464" s="169"/>
-      <c r="E464" s="169"/>
+      <c r="C464" s="166"/>
+      <c r="D464" s="167"/>
+      <c r="E464" s="167"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -24020,9 +24209,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="168"/>
-      <c r="D481" s="169"/>
-      <c r="E481" s="169"/>
+      <c r="C481" s="166"/>
+      <c r="D481" s="167"/>
+      <c r="E481" s="167"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -24173,9 +24362,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="168"/>
-      <c r="D498" s="169"/>
-      <c r="E498" s="169"/>
+      <c r="C498" s="166"/>
+      <c r="D498" s="167"/>
+      <c r="E498" s="167"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -24326,9 +24515,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="168"/>
-      <c r="D515" s="169"/>
-      <c r="E515" s="169"/>
+      <c r="C515" s="166"/>
+      <c r="D515" s="167"/>
+      <c r="E515" s="167"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -24479,9 +24668,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="168"/>
-      <c r="D532" s="169"/>
-      <c r="E532" s="169"/>
+      <c r="C532" s="166"/>
+      <c r="D532" s="167"/>
+      <c r="E532" s="167"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -24632,18 +24821,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="180"/>
-      <c r="D549" s="181"/>
-      <c r="E549" s="181"/>
+      <c r="C549" s="173"/>
+      <c r="D549" s="174"/>
+      <c r="E549" s="174"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="168"/>
-      <c r="D550" s="169"/>
-      <c r="E550" s="169"/>
+      <c r="C550" s="166"/>
+      <c r="D550" s="167"/>
+      <c r="E550" s="167"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -24794,9 +24983,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="166"/>
-      <c r="D567" s="167"/>
-      <c r="E567" s="167"/>
+      <c r="C567" s="171"/>
+      <c r="D567" s="172"/>
+      <c r="E567" s="172"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -24947,9 +25136,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="168"/>
-      <c r="D584" s="169"/>
-      <c r="E584" s="169"/>
+      <c r="C584" s="166"/>
+      <c r="D584" s="167"/>
+      <c r="E584" s="167"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -25100,9 +25289,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="168"/>
-      <c r="D601" s="169"/>
-      <c r="E601" s="169"/>
+      <c r="C601" s="166"/>
+      <c r="D601" s="167"/>
+      <c r="E601" s="167"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -25253,9 +25442,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="168"/>
-      <c r="D618" s="169"/>
-      <c r="E618" s="169"/>
+      <c r="C618" s="166"/>
+      <c r="D618" s="167"/>
+      <c r="E618" s="167"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -25406,9 +25595,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="168"/>
-      <c r="D635" s="169"/>
-      <c r="E635" s="169"/>
+      <c r="C635" s="166"/>
+      <c r="D635" s="167"/>
+      <c r="E635" s="167"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -25559,9 +25748,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="168"/>
-      <c r="D652" s="169"/>
-      <c r="E652" s="169"/>
+      <c r="C652" s="166"/>
+      <c r="D652" s="167"/>
+      <c r="E652" s="167"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -25712,9 +25901,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="168"/>
-      <c r="D669" s="169"/>
-      <c r="E669" s="169"/>
+      <c r="C669" s="166"/>
+      <c r="D669" s="167"/>
+      <c r="E669" s="167"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -25865,9 +26054,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="168"/>
-      <c r="D686" s="169"/>
-      <c r="E686" s="169"/>
+      <c r="C686" s="166"/>
+      <c r="D686" s="167"/>
+      <c r="E686" s="167"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -26018,9 +26207,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="168"/>
-      <c r="D703" s="169"/>
-      <c r="E703" s="169"/>
+      <c r="C703" s="166"/>
+      <c r="D703" s="167"/>
+      <c r="E703" s="167"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -26171,9 +26360,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="168"/>
-      <c r="D720" s="169"/>
-      <c r="E720" s="169"/>
+      <c r="C720" s="166"/>
+      <c r="D720" s="167"/>
+      <c r="E720" s="167"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -26324,9 +26513,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="168"/>
-      <c r="D737" s="169"/>
-      <c r="E737" s="169"/>
+      <c r="C737" s="166"/>
+      <c r="D737" s="167"/>
+      <c r="E737" s="167"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -26477,9 +26666,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="168"/>
-      <c r="D754" s="169"/>
-      <c r="E754" s="169"/>
+      <c r="C754" s="166"/>
+      <c r="D754" s="167"/>
+      <c r="E754" s="167"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -26630,9 +26819,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="168"/>
-      <c r="D771" s="169"/>
-      <c r="E771" s="169"/>
+      <c r="C771" s="166"/>
+      <c r="D771" s="167"/>
+      <c r="E771" s="167"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -26783,9 +26972,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="168"/>
-      <c r="D788" s="169"/>
-      <c r="E788" s="169"/>
+      <c r="C788" s="166"/>
+      <c r="D788" s="167"/>
+      <c r="E788" s="167"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -26936,9 +27125,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="168"/>
-      <c r="D805" s="169"/>
-      <c r="E805" s="169"/>
+      <c r="C805" s="166"/>
+      <c r="D805" s="167"/>
+      <c r="E805" s="167"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -27089,18 +27278,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="178"/>
-      <c r="D822" s="179"/>
-      <c r="E822" s="179"/>
+      <c r="C822" s="177"/>
+      <c r="D822" s="178"/>
+      <c r="E822" s="178"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="168"/>
-      <c r="D823" s="169"/>
-      <c r="E823" s="169"/>
+      <c r="C823" s="166"/>
+      <c r="D823" s="167"/>
+      <c r="E823" s="167"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -27251,9 +27440,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="166"/>
-      <c r="D840" s="167"/>
-      <c r="E840" s="167"/>
+      <c r="C840" s="171"/>
+      <c r="D840" s="172"/>
+      <c r="E840" s="172"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -27404,9 +27593,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="168"/>
-      <c r="D857" s="169"/>
-      <c r="E857" s="169"/>
+      <c r="C857" s="166"/>
+      <c r="D857" s="167"/>
+      <c r="E857" s="167"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -27557,9 +27746,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="168"/>
-      <c r="D874" s="169"/>
-      <c r="E874" s="169"/>
+      <c r="C874" s="166"/>
+      <c r="D874" s="167"/>
+      <c r="E874" s="167"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -27710,9 +27899,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="168"/>
-      <c r="D891" s="169"/>
-      <c r="E891" s="169"/>
+      <c r="C891" s="166"/>
+      <c r="D891" s="167"/>
+      <c r="E891" s="167"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -27863,9 +28052,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="168"/>
-      <c r="D908" s="169"/>
-      <c r="E908" s="169"/>
+      <c r="C908" s="166"/>
+      <c r="D908" s="167"/>
+      <c r="E908" s="167"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -28016,9 +28205,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="168"/>
-      <c r="D925" s="169"/>
-      <c r="E925" s="169"/>
+      <c r="C925" s="166"/>
+      <c r="D925" s="167"/>
+      <c r="E925" s="167"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -28169,9 +28358,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="168"/>
-      <c r="D942" s="169"/>
-      <c r="E942" s="169"/>
+      <c r="C942" s="166"/>
+      <c r="D942" s="167"/>
+      <c r="E942" s="167"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -28322,9 +28511,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="168"/>
-      <c r="D959" s="169"/>
-      <c r="E959" s="169"/>
+      <c r="C959" s="166"/>
+      <c r="D959" s="167"/>
+      <c r="E959" s="167"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -28475,9 +28664,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="168"/>
-      <c r="D976" s="169"/>
-      <c r="E976" s="169"/>
+      <c r="C976" s="166"/>
+      <c r="D976" s="167"/>
+      <c r="E976" s="167"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -28628,9 +28817,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="168"/>
-      <c r="D993" s="169"/>
-      <c r="E993" s="169"/>
+      <c r="C993" s="166"/>
+      <c r="D993" s="167"/>
+      <c r="E993" s="167"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -28781,9 +28970,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="168"/>
-      <c r="D1010" s="169"/>
-      <c r="E1010" s="169"/>
+      <c r="C1010" s="166"/>
+      <c r="D1010" s="167"/>
+      <c r="E1010" s="167"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -28934,9 +29123,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="168"/>
-      <c r="D1027" s="169"/>
-      <c r="E1027" s="169"/>
+      <c r="C1027" s="166"/>
+      <c r="D1027" s="167"/>
+      <c r="E1027" s="167"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -29087,9 +29276,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="168"/>
-      <c r="D1044" s="169"/>
-      <c r="E1044" s="169"/>
+      <c r="C1044" s="166"/>
+      <c r="D1044" s="167"/>
+      <c r="E1044" s="167"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -29240,9 +29429,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="168"/>
-      <c r="D1061" s="169"/>
-      <c r="E1061" s="169"/>
+      <c r="C1061" s="166"/>
+      <c r="D1061" s="167"/>
+      <c r="E1061" s="167"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -29393,9 +29582,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="168"/>
-      <c r="D1078" s="169"/>
-      <c r="E1078" s="169"/>
+      <c r="C1078" s="166"/>
+      <c r="D1078" s="167"/>
+      <c r="E1078" s="167"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -29546,18 +29735,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="176"/>
-      <c r="D1095" s="177"/>
-      <c r="E1095" s="177"/>
+      <c r="C1095" s="179"/>
+      <c r="D1095" s="180"/>
+      <c r="E1095" s="180"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="168"/>
-      <c r="D1096" s="169"/>
-      <c r="E1096" s="169"/>
+      <c r="C1096" s="166"/>
+      <c r="D1096" s="167"/>
+      <c r="E1096" s="167"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -29708,9 +29897,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="166"/>
-      <c r="D1113" s="167"/>
-      <c r="E1113" s="167"/>
+      <c r="C1113" s="171"/>
+      <c r="D1113" s="172"/>
+      <c r="E1113" s="172"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -29861,9 +30050,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="168"/>
-      <c r="D1130" s="169"/>
-      <c r="E1130" s="169"/>
+      <c r="C1130" s="166"/>
+      <c r="D1130" s="167"/>
+      <c r="E1130" s="167"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -30014,9 +30203,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="168"/>
-      <c r="D1147" s="169"/>
-      <c r="E1147" s="169"/>
+      <c r="C1147" s="166"/>
+      <c r="D1147" s="167"/>
+      <c r="E1147" s="167"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -30167,9 +30356,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="168"/>
-      <c r="D1164" s="169"/>
-      <c r="E1164" s="169"/>
+      <c r="C1164" s="166"/>
+      <c r="D1164" s="167"/>
+      <c r="E1164" s="167"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -30320,9 +30509,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="168"/>
-      <c r="D1181" s="169"/>
-      <c r="E1181" s="169"/>
+      <c r="C1181" s="166"/>
+      <c r="D1181" s="167"/>
+      <c r="E1181" s="167"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -30473,9 +30662,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="168"/>
-      <c r="D1198" s="169"/>
-      <c r="E1198" s="169"/>
+      <c r="C1198" s="166"/>
+      <c r="D1198" s="167"/>
+      <c r="E1198" s="167"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -30626,9 +30815,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="168"/>
-      <c r="D1215" s="169"/>
-      <c r="E1215" s="169"/>
+      <c r="C1215" s="166"/>
+      <c r="D1215" s="167"/>
+      <c r="E1215" s="167"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -30779,9 +30968,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="168"/>
-      <c r="D1232" s="169"/>
-      <c r="E1232" s="169"/>
+      <c r="C1232" s="166"/>
+      <c r="D1232" s="167"/>
+      <c r="E1232" s="167"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -30932,9 +31121,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="168"/>
-      <c r="D1249" s="169"/>
-      <c r="E1249" s="169"/>
+      <c r="C1249" s="166"/>
+      <c r="D1249" s="167"/>
+      <c r="E1249" s="167"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -31085,9 +31274,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="168"/>
-      <c r="D1266" s="169"/>
-      <c r="E1266" s="169"/>
+      <c r="C1266" s="166"/>
+      <c r="D1266" s="167"/>
+      <c r="E1266" s="167"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -31238,9 +31427,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="168"/>
-      <c r="D1283" s="169"/>
-      <c r="E1283" s="169"/>
+      <c r="C1283" s="166"/>
+      <c r="D1283" s="167"/>
+      <c r="E1283" s="167"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -31391,9 +31580,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="168"/>
-      <c r="D1300" s="169"/>
-      <c r="E1300" s="169"/>
+      <c r="C1300" s="166"/>
+      <c r="D1300" s="167"/>
+      <c r="E1300" s="167"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -31544,9 +31733,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="168"/>
-      <c r="D1317" s="169"/>
-      <c r="E1317" s="169"/>
+      <c r="C1317" s="166"/>
+      <c r="D1317" s="167"/>
+      <c r="E1317" s="167"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -31697,9 +31886,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="168"/>
-      <c r="D1334" s="169"/>
-      <c r="E1334" s="169"/>
+      <c r="C1334" s="166"/>
+      <c r="D1334" s="167"/>
+      <c r="E1334" s="167"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -31850,9 +32039,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="168"/>
-      <c r="D1351" s="169"/>
-      <c r="E1351" s="169"/>
+      <c r="C1351" s="166"/>
+      <c r="D1351" s="167"/>
+      <c r="E1351" s="167"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -32003,18 +32192,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="174"/>
-      <c r="D1368" s="175"/>
-      <c r="E1368" s="175"/>
+      <c r="C1368" s="181"/>
+      <c r="D1368" s="182"/>
+      <c r="E1368" s="182"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="168"/>
-      <c r="D1369" s="169"/>
-      <c r="E1369" s="169"/>
+      <c r="C1369" s="166"/>
+      <c r="D1369" s="167"/>
+      <c r="E1369" s="167"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -32165,9 +32354,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="166"/>
-      <c r="D1386" s="167"/>
-      <c r="E1386" s="167"/>
+      <c r="C1386" s="171"/>
+      <c r="D1386" s="172"/>
+      <c r="E1386" s="172"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -32318,9 +32507,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="168"/>
-      <c r="D1403" s="169"/>
-      <c r="E1403" s="169"/>
+      <c r="C1403" s="166"/>
+      <c r="D1403" s="167"/>
+      <c r="E1403" s="167"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -32471,9 +32660,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="168"/>
-      <c r="D1420" s="169"/>
-      <c r="E1420" s="169"/>
+      <c r="C1420" s="166"/>
+      <c r="D1420" s="167"/>
+      <c r="E1420" s="167"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -32624,9 +32813,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="168"/>
-      <c r="D1437" s="169"/>
-      <c r="E1437" s="169"/>
+      <c r="C1437" s="166"/>
+      <c r="D1437" s="167"/>
+      <c r="E1437" s="167"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -32777,9 +32966,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="168"/>
-      <c r="D1454" s="169"/>
-      <c r="E1454" s="169"/>
+      <c r="C1454" s="166"/>
+      <c r="D1454" s="167"/>
+      <c r="E1454" s="167"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -32930,9 +33119,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="168"/>
-      <c r="D1471" s="169"/>
-      <c r="E1471" s="169"/>
+      <c r="C1471" s="166"/>
+      <c r="D1471" s="167"/>
+      <c r="E1471" s="167"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -33083,9 +33272,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="168"/>
-      <c r="D1488" s="169"/>
-      <c r="E1488" s="169"/>
+      <c r="C1488" s="166"/>
+      <c r="D1488" s="167"/>
+      <c r="E1488" s="167"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -33236,9 +33425,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="168"/>
-      <c r="D1505" s="169"/>
-      <c r="E1505" s="169"/>
+      <c r="C1505" s="166"/>
+      <c r="D1505" s="167"/>
+      <c r="E1505" s="167"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -33389,9 +33578,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="168"/>
-      <c r="D1522" s="169"/>
-      <c r="E1522" s="169"/>
+      <c r="C1522" s="166"/>
+      <c r="D1522" s="167"/>
+      <c r="E1522" s="167"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -33542,9 +33731,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="168"/>
-      <c r="D1539" s="169"/>
-      <c r="E1539" s="169"/>
+      <c r="C1539" s="166"/>
+      <c r="D1539" s="167"/>
+      <c r="E1539" s="167"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -33695,9 +33884,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="168"/>
-      <c r="D1556" s="169"/>
-      <c r="E1556" s="169"/>
+      <c r="C1556" s="166"/>
+      <c r="D1556" s="167"/>
+      <c r="E1556" s="167"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -33848,9 +34037,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="168"/>
-      <c r="D1573" s="169"/>
-      <c r="E1573" s="169"/>
+      <c r="C1573" s="166"/>
+      <c r="D1573" s="167"/>
+      <c r="E1573" s="167"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -34001,9 +34190,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="168"/>
-      <c r="D1590" s="169"/>
-      <c r="E1590" s="169"/>
+      <c r="C1590" s="166"/>
+      <c r="D1590" s="167"/>
+      <c r="E1590" s="167"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -34154,9 +34343,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="168"/>
-      <c r="D1607" s="169"/>
-      <c r="E1607" s="169"/>
+      <c r="C1607" s="166"/>
+      <c r="D1607" s="167"/>
+      <c r="E1607" s="167"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -34307,9 +34496,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="168"/>
-      <c r="D1624" s="169"/>
-      <c r="E1624" s="169"/>
+      <c r="C1624" s="166"/>
+      <c r="D1624" s="167"/>
+      <c r="E1624" s="167"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -34460,18 +34649,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="172"/>
-      <c r="D1641" s="173"/>
-      <c r="E1641" s="173"/>
+      <c r="C1641" s="183"/>
+      <c r="D1641" s="184"/>
+      <c r="E1641" s="184"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="168"/>
-      <c r="D1642" s="169"/>
-      <c r="E1642" s="169"/>
+      <c r="C1642" s="166"/>
+      <c r="D1642" s="167"/>
+      <c r="E1642" s="167"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -34622,9 +34811,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="166"/>
-      <c r="D1659" s="167"/>
-      <c r="E1659" s="167"/>
+      <c r="C1659" s="171"/>
+      <c r="D1659" s="172"/>
+      <c r="E1659" s="172"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -34775,9 +34964,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="168"/>
-      <c r="D1676" s="169"/>
-      <c r="E1676" s="169"/>
+      <c r="C1676" s="166"/>
+      <c r="D1676" s="167"/>
+      <c r="E1676" s="167"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -34928,9 +35117,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="168"/>
-      <c r="D1693" s="169"/>
-      <c r="E1693" s="169"/>
+      <c r="C1693" s="166"/>
+      <c r="D1693" s="167"/>
+      <c r="E1693" s="167"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -35081,9 +35270,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="168"/>
-      <c r="D1710" s="169"/>
-      <c r="E1710" s="169"/>
+      <c r="C1710" s="166"/>
+      <c r="D1710" s="167"/>
+      <c r="E1710" s="167"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -35234,9 +35423,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="168"/>
-      <c r="D1727" s="169"/>
-      <c r="E1727" s="169"/>
+      <c r="C1727" s="166"/>
+      <c r="D1727" s="167"/>
+      <c r="E1727" s="167"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -35387,9 +35576,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="168"/>
-      <c r="D1744" s="169"/>
-      <c r="E1744" s="169"/>
+      <c r="C1744" s="166"/>
+      <c r="D1744" s="167"/>
+      <c r="E1744" s="167"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -35540,9 +35729,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="168"/>
-      <c r="D1761" s="169"/>
-      <c r="E1761" s="169"/>
+      <c r="C1761" s="166"/>
+      <c r="D1761" s="167"/>
+      <c r="E1761" s="167"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -35693,9 +35882,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="168"/>
-      <c r="D1778" s="169"/>
-      <c r="E1778" s="169"/>
+      <c r="C1778" s="166"/>
+      <c r="D1778" s="167"/>
+      <c r="E1778" s="167"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -35846,9 +36035,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="168"/>
-      <c r="D1795" s="169"/>
-      <c r="E1795" s="169"/>
+      <c r="C1795" s="166"/>
+      <c r="D1795" s="167"/>
+      <c r="E1795" s="167"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -35999,9 +36188,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="168"/>
-      <c r="D1812" s="169"/>
-      <c r="E1812" s="169"/>
+      <c r="C1812" s="166"/>
+      <c r="D1812" s="167"/>
+      <c r="E1812" s="167"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -36152,9 +36341,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="168"/>
-      <c r="D1829" s="169"/>
-      <c r="E1829" s="169"/>
+      <c r="C1829" s="166"/>
+      <c r="D1829" s="167"/>
+      <c r="E1829" s="167"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -36305,9 +36494,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="168"/>
-      <c r="D1846" s="169"/>
-      <c r="E1846" s="169"/>
+      <c r="C1846" s="166"/>
+      <c r="D1846" s="167"/>
+      <c r="E1846" s="167"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -36458,9 +36647,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="168"/>
-      <c r="D1863" s="169"/>
-      <c r="E1863" s="169"/>
+      <c r="C1863" s="166"/>
+      <c r="D1863" s="167"/>
+      <c r="E1863" s="167"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -36611,9 +36800,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="168"/>
-      <c r="D1880" s="169"/>
-      <c r="E1880" s="169"/>
+      <c r="C1880" s="166"/>
+      <c r="D1880" s="167"/>
+      <c r="E1880" s="167"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -36764,9 +36953,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="168"/>
-      <c r="D1897" s="169"/>
-      <c r="E1897" s="169"/>
+      <c r="C1897" s="166"/>
+      <c r="D1897" s="167"/>
+      <c r="E1897" s="167"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -36917,18 +37106,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="170"/>
-      <c r="D1914" s="171"/>
-      <c r="E1914" s="171"/>
+      <c r="C1914" s="185"/>
+      <c r="D1914" s="186"/>
+      <c r="E1914" s="186"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="168"/>
-      <c r="D1915" s="169"/>
-      <c r="E1915" s="169"/>
+      <c r="C1915" s="166"/>
+      <c r="D1915" s="167"/>
+      <c r="E1915" s="167"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -37079,9 +37268,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="166"/>
-      <c r="D1932" s="167"/>
-      <c r="E1932" s="167"/>
+      <c r="C1932" s="171"/>
+      <c r="D1932" s="172"/>
+      <c r="E1932" s="172"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -37232,9 +37421,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="168"/>
-      <c r="D1949" s="169"/>
-      <c r="E1949" s="169"/>
+      <c r="C1949" s="166"/>
+      <c r="D1949" s="167"/>
+      <c r="E1949" s="167"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -37385,9 +37574,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="168"/>
-      <c r="D1966" s="169"/>
-      <c r="E1966" s="169"/>
+      <c r="C1966" s="166"/>
+      <c r="D1966" s="167"/>
+      <c r="E1966" s="167"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -37538,9 +37727,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="168"/>
-      <c r="D1983" s="169"/>
-      <c r="E1983" s="169"/>
+      <c r="C1983" s="166"/>
+      <c r="D1983" s="167"/>
+      <c r="E1983" s="167"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -37691,9 +37880,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="168"/>
-      <c r="D2000" s="169"/>
-      <c r="E2000" s="169"/>
+      <c r="C2000" s="166"/>
+      <c r="D2000" s="167"/>
+      <c r="E2000" s="167"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -37844,9 +38033,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="168"/>
-      <c r="D2017" s="169"/>
-      <c r="E2017" s="169"/>
+      <c r="C2017" s="166"/>
+      <c r="D2017" s="167"/>
+      <c r="E2017" s="167"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -37997,9 +38186,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="168"/>
-      <c r="D2034" s="169"/>
-      <c r="E2034" s="169"/>
+      <c r="C2034" s="166"/>
+      <c r="D2034" s="167"/>
+      <c r="E2034" s="167"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -38150,9 +38339,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="168"/>
-      <c r="D2051" s="169"/>
-      <c r="E2051" s="169"/>
+      <c r="C2051" s="166"/>
+      <c r="D2051" s="167"/>
+      <c r="E2051" s="167"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -38303,9 +38492,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="168"/>
-      <c r="D2068" s="169"/>
-      <c r="E2068" s="169"/>
+      <c r="C2068" s="166"/>
+      <c r="D2068" s="167"/>
+      <c r="E2068" s="167"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -38456,9 +38645,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="168"/>
-      <c r="D2085" s="169"/>
-      <c r="E2085" s="169"/>
+      <c r="C2085" s="166"/>
+      <c r="D2085" s="167"/>
+      <c r="E2085" s="167"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -38609,9 +38798,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="168"/>
-      <c r="D2102" s="169"/>
-      <c r="E2102" s="169"/>
+      <c r="C2102" s="166"/>
+      <c r="D2102" s="167"/>
+      <c r="E2102" s="167"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -38762,9 +38951,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="168"/>
-      <c r="D2119" s="169"/>
-      <c r="E2119" s="169"/>
+      <c r="C2119" s="166"/>
+      <c r="D2119" s="167"/>
+      <c r="E2119" s="167"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -38915,9 +39104,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="168"/>
-      <c r="D2136" s="169"/>
-      <c r="E2136" s="169"/>
+      <c r="C2136" s="166"/>
+      <c r="D2136" s="167"/>
+      <c r="E2136" s="167"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -39068,9 +39257,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="168"/>
-      <c r="D2153" s="169"/>
-      <c r="E2153" s="169"/>
+      <c r="C2153" s="166"/>
+      <c r="D2153" s="167"/>
+      <c r="E2153" s="167"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -39221,9 +39410,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="168"/>
-      <c r="D2170" s="169"/>
-      <c r="E2170" s="169"/>
+      <c r="C2170" s="166"/>
+      <c r="D2170" s="167"/>
+      <c r="E2170" s="167"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -39371,6 +39560,135 @@
     </row>
   </sheetData>
   <mergeCells count="137">
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C1949:E1949"/>
+    <mergeCell ref="C1983:E1983"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2000:E2000"/>
+    <mergeCell ref="C2017:E2017"/>
+    <mergeCell ref="C1966:E1966"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
+    <mergeCell ref="C1914:E1914"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1897:E1897"/>
+    <mergeCell ref="C1932:E1932"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1846:E1846"/>
+    <mergeCell ref="C1863:E1863"/>
+    <mergeCell ref="C1880:E1880"/>
+    <mergeCell ref="C1915:E1915"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C328:E328"/>
+    <mergeCell ref="C345:E345"/>
+    <mergeCell ref="C379:E379"/>
+    <mergeCell ref="C413:E413"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C362:E362"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C430:E430"/>
+    <mergeCell ref="C447:E447"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C396:E396"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C567:E567"/>
+    <mergeCell ref="C464:E464"/>
+    <mergeCell ref="C481:E481"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C311:E311"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C294:E294"/>
+    <mergeCell ref="C123:E123"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
@@ -39379,135 +39697,6 @@
     <mergeCell ref="C38:E38"/>
     <mergeCell ref="C55:E55"/>
     <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C362:E362"/>
-    <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C294:E294"/>
-    <mergeCell ref="C311:E311"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="C396:E396"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C328:E328"/>
-    <mergeCell ref="C345:E345"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C464:E464"/>
-    <mergeCell ref="C481:E481"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C430:E430"/>
-    <mergeCell ref="C447:E447"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C413:E413"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1897:E1897"/>
-    <mergeCell ref="C1914:E1914"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1846:E1846"/>
-    <mergeCell ref="C1863:E1863"/>
-    <mergeCell ref="C1880:E1880"/>
-    <mergeCell ref="C2017:E2017"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
-    <mergeCell ref="C1932:E1932"/>
-    <mergeCell ref="C1949:E1949"/>
-    <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C1966:E1966"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C1983:E1983"/>
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2000:E2000"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>